<commit_message>
add intial signature image in the pds generation
</commit_message>
<xml_diff>
--- a/backend/temp/updated_filled_pds.xlsx
+++ b/backend/temp/updated_filled_pds.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="450">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -79,7 +79,7 @@
     <t>SURNAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hatdog</t>
+    <t xml:space="preserve"> Hassan</t>
   </si>
   <si>
     <t/>
@@ -88,10 +88,10 @@
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> asdasdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 123123</t>
+    <t xml:space="preserve"> Adnan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Married</t>
@@ -103,7 +103,7 @@
     <t>MIDDLE NAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> t</t>
+    <t xml:space="preserve"> T.</t>
   </si>
   <si>
     <t>Widow/er</t>
@@ -119,13 +119,13 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
-    <t>2024-08-01</t>
+    <t>2024-08-15</t>
   </si>
   <si>
     <t>16. CITIZENSHIP</t>
   </si>
   <si>
-    <t xml:space="preserve">☑ Filipino               ☐ Dual Citizenship
+    <t xml:space="preserve">☐ Filipino               ☑ Dual Citizenship
 </t>
   </si>
   <si>
@@ -135,7 +135,7 @@
     <t>Albania</t>
   </si>
   <si>
-    <t>☐ by birth             ☐ by naturalization</t>
+    <t>☑ by birth             ☐ by naturalization</t>
   </si>
   <si>
     <t>4.</t>
@@ -144,7 +144,7 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
-    <t>Maguindanao</t>
+    <t>Datu Piang, Maguindanao</t>
   </si>
   <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
@@ -165,10 +165,13 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>☐ Male                 ☐ Female</t>
+    <t>☑ Male                 ☐ Female</t>
   </si>
   <si>
     <t>please indicate the details.</t>
+  </si>
+  <si>
+    <t>Japan</t>
   </si>
   <si>
     <t>Others</t>
@@ -290,7 +293,7 @@
     <t>GSIS ID NO.</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>12378123782</t>
   </si>
   <si>
     <t>Bangladesh</t>
@@ -305,6 +308,9 @@
     <t>PAG-IBIG ID NO.</t>
   </si>
   <si>
+    <t>55875695674</t>
+  </si>
+  <si>
     <t>Belarus</t>
   </si>
   <si>
@@ -317,7 +323,7 @@
     <t>PHILHEALTH NO.</t>
   </si>
   <si>
-    <t>23423423423</t>
+    <t>2367465856</t>
   </si>
   <si>
     <t>Belize</t>
@@ -329,7 +335,7 @@
     <t>SSS NO.</t>
   </si>
   <si>
-    <t>16584657456</t>
+    <t>47357835345</t>
   </si>
   <si>
     <t>19. TELEPHONE NO.</t>
@@ -341,13 +347,13 @@
     <t>14. TIN NO.</t>
   </si>
   <si>
-    <t>32423423423</t>
+    <t>346738756634</t>
   </si>
   <si>
     <t>20. MOBILE NO.</t>
   </si>
   <si>
-    <t>99999</t>
+    <t>09460994104</t>
   </si>
   <si>
     <t>Bhutan</t>
@@ -377,9 +383,6 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> asds</t>
-  </si>
-  <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
   </si>
   <si>
@@ -392,13 +395,13 @@
     <t xml:space="preserve">  FIRST NAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                     </t>
   </si>
   <si>
-    <t>asd</t>
+    <t>Adnan HASsan</t>
+  </si>
+  <si>
+    <t>2024-09-11</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -407,6 +410,12 @@
     <t xml:space="preserve">  MIDDLE NAME</t>
   </si>
   <si>
+    <t>terst</t>
+  </si>
+  <si>
+    <t>2024-09-21</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brunei </t>
   </si>
   <si>
@@ -440,9 +449,15 @@
     <t>FATHER'S SURNAME</t>
   </si>
   <si>
+    <t xml:space="preserve"> Ebrahim</t>
+  </si>
+  <si>
     <t>Cambodia</t>
   </si>
   <si>
+    <t xml:space="preserve"> Abdulkadir</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                                  </t>
   </si>
   <si>
@@ -462,6 +477,9 @@
   </si>
   <si>
     <t>Central African Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anida</t>
   </si>
   <si>
     <t>Chad</t>
@@ -525,12 +543,33 @@
     <t>ELEMENTARY</t>
   </si>
   <si>
+    <t>Example school</t>
+  </si>
+  <si>
+    <t>2024-09-05</t>
+  </si>
+  <si>
+    <t>2024-09-20</t>
+  </si>
+  <si>
     <t>Congo, Republic of the</t>
   </si>
   <si>
     <t>SECONDARY</t>
   </si>
   <si>
+    <t>MRTHS</t>
+  </si>
+  <si>
+    <t>2024-09-14</t>
+  </si>
+  <si>
+    <t>2024-09-19</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
     <t>Costa Rica</t>
   </si>
   <si>
@@ -543,6 +582,24 @@
     <t>COLLEGE</t>
   </si>
   <si>
+    <t>PUP - Taguig</t>
+  </si>
+  <si>
+    <t>BSIT</t>
+  </si>
+  <si>
+    <t>2024-09-06</t>
+  </si>
+  <si>
+    <t>2024-09-28</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
     <t>Croatia</t>
   </si>
   <si>
@@ -561,6 +618,9 @@
     <t>DATE</t>
   </si>
   <si>
+    <t>2024-09-26</t>
+  </si>
+  <si>
     <t>Cyprus</t>
   </si>
   <si>
@@ -685,9 +745,6 @@
   </si>
   <si>
     <t>Jamaica</t>
-  </si>
-  <si>
-    <t>Japan</t>
   </si>
   <si>
     <t>Jordan</t>
@@ -3487,7 +3544,7 @@
     <xf numFmtId="49" fontId="29" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -4727,6 +4784,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5455,15 +5561,15 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="31"/>
       <c r="P16" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q16" s="57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5471,30 +5577,30 @@
         <v>6</v>
       </c>
       <c r="B17" s="90" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="91"/>
       <c r="D17" s="92" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17" s="92"/>
       <c r="F17" s="92"/>
       <c r="G17" s="93" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H17" s="94"/>
       <c r="I17" s="95" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J17" s="96"/>
       <c r="K17" s="96"/>
       <c r="L17" s="96" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M17" s="96"/>
       <c r="N17" s="97"/>
       <c r="Q17" s="57" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" ht="9" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5507,17 +5613,17 @@
       <c r="G18" s="102"/>
       <c r="H18" s="103"/>
       <c r="I18" s="104" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J18" s="105"/>
       <c r="K18" s="105"/>
       <c r="L18" s="105" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M18" s="105"/>
       <c r="N18" s="106"/>
       <c r="Q18" s="57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" ht="5.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5535,12 +5641,12 @@
       <c r="J19" s="109"/>
       <c r="K19" s="109"/>
       <c r="L19" s="110" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M19" s="109"/>
       <c r="N19" s="111"/>
       <c r="Q19" s="57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" ht="9.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5548,7 +5654,7 @@
       <c r="B20" s="107"/>
       <c r="C20" s="112"/>
       <c r="D20" s="113" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="101"/>
       <c r="F20" s="101"/>
@@ -5561,7 +5667,7 @@
       <c r="M20" s="115"/>
       <c r="N20" s="116"/>
       <c r="Q20" s="57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" ht="9" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5574,46 +5680,46 @@
       <c r="G21" s="69"/>
       <c r="H21" s="41"/>
       <c r="I21" s="122" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J21" s="123"/>
       <c r="K21" s="123"/>
       <c r="L21" s="124" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M21" s="125"/>
       <c r="N21" s="126"/>
       <c r="Q21" s="57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B22" s="127" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="128"/>
       <c r="D22" s="129">
-        <v>32</v>
+        <v>3.35</v>
       </c>
       <c r="E22" s="129"/>
       <c r="F22" s="129"/>
       <c r="G22" s="69"/>
       <c r="H22" s="41"/>
       <c r="I22" s="95" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J22" s="96"/>
       <c r="K22" s="96"/>
       <c r="L22" s="96" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M22" s="96"/>
       <c r="N22" s="97"/>
       <c r="Q22" s="57" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" ht="8.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5626,38 +5732,38 @@
       <c r="G23" s="69"/>
       <c r="H23" s="41"/>
       <c r="I23" s="134" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J23" s="135"/>
       <c r="K23" s="135"/>
       <c r="L23" s="136" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M23" s="136"/>
       <c r="N23" s="137"/>
       <c r="Q23" s="57" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" ht="22.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" s="138" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="139"/>
       <c r="D24" s="140">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="E24" s="140"/>
       <c r="F24" s="140"/>
       <c r="G24" s="141" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H24" s="142"/>
       <c r="I24" s="143" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J24" s="144"/>
       <c r="K24" s="144"/>
@@ -5665,38 +5771,38 @@
       <c r="M24" s="144"/>
       <c r="N24" s="145"/>
       <c r="Q24" s="57" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="146" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B25" s="127" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C25" s="128"/>
       <c r="D25" s="147" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E25" s="147"/>
       <c r="F25" s="147"/>
       <c r="G25" s="148" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H25" s="127"/>
       <c r="I25" s="95" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J25" s="96"/>
       <c r="K25" s="96"/>
       <c r="L25" s="96" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M25" s="96"/>
       <c r="N25" s="149"/>
       <c r="Q25" s="57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" ht="9" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5709,29 +5815,29 @@
       <c r="G26" s="69"/>
       <c r="H26" s="41"/>
       <c r="I26" s="104" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J26" s="105"/>
       <c r="K26" s="105"/>
       <c r="L26" s="105" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M26" s="105"/>
       <c r="N26" s="106"/>
       <c r="Q26" s="57" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="146" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="127" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" s="128"/>
       <c r="D27" s="147" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" s="147"/>
       <c r="F27" s="147"/>
@@ -5743,12 +5849,12 @@
       <c r="J27" s="96"/>
       <c r="K27" s="96"/>
       <c r="L27" s="96" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M27" s="96"/>
       <c r="N27" s="149"/>
       <c r="Q27" s="57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" ht="9" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5761,29 +5867,29 @@
       <c r="G28" s="102"/>
       <c r="H28" s="103"/>
       <c r="I28" s="151" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J28" s="152"/>
       <c r="K28" s="152"/>
       <c r="L28" s="153" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M28" s="152"/>
       <c r="N28" s="154"/>
       <c r="Q28" s="57" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="146" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B29" s="127" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="128"/>
       <c r="D29" s="147" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E29" s="147"/>
       <c r="F29" s="147"/>
@@ -5791,16 +5897,16 @@
       <c r="H29" s="155"/>
       <c r="I29" s="156"/>
       <c r="J29" s="157" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K29" s="157"/>
       <c r="L29" s="157"/>
       <c r="M29" s="157" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N29" s="158"/>
       <c r="Q29" s="57" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" ht="9.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5813,38 +5919,38 @@
       <c r="G30" s="102"/>
       <c r="H30" s="155"/>
       <c r="I30" s="159" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J30" s="159"/>
       <c r="K30" s="159"/>
       <c r="L30" s="159" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M30" s="159"/>
       <c r="N30" s="160"/>
       <c r="Q30" s="57" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" ht="24.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B31" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C31" s="83"/>
       <c r="D31" s="147" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E31" s="147"/>
       <c r="F31" s="147"/>
       <c r="G31" s="141" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H31" s="142"/>
       <c r="I31" s="134" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J31" s="135"/>
       <c r="K31" s="135"/>
@@ -5852,24 +5958,24 @@
       <c r="M31" s="124"/>
       <c r="N31" s="161"/>
       <c r="Q31" s="57" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" ht="24.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B32" s="73" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C32" s="83"/>
       <c r="D32" s="140" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E32" s="140"/>
       <c r="F32" s="140"/>
       <c r="G32" s="162" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H32" s="138"/>
       <c r="I32" s="143" t="s">
@@ -5881,26 +5987,26 @@
       <c r="M32" s="144"/>
       <c r="N32" s="145"/>
       <c r="Q32" s="57" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" ht="24.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="162" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B33" s="139"/>
       <c r="C33" s="163"/>
       <c r="D33" s="140" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E33" s="140"/>
       <c r="F33" s="140"/>
       <c r="G33" s="164" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H33" s="165"/>
       <c r="I33" s="143" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J33" s="144"/>
       <c r="K33" s="144"/>
@@ -5908,12 +6014,12 @@
       <c r="M33" s="144"/>
       <c r="N33" s="145"/>
       <c r="Q33" s="57" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" ht="24.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="166" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B34" s="99"/>
       <c r="C34" s="167"/>
@@ -5923,11 +6029,11 @@
       <c r="E34" s="147"/>
       <c r="F34" s="147"/>
       <c r="G34" s="148" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H34" s="127"/>
       <c r="I34" s="108" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J34" s="168"/>
       <c r="K34" s="168"/>
@@ -5935,12 +6041,12 @@
       <c r="M34" s="168"/>
       <c r="N34" s="169"/>
       <c r="Q34" s="57" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" ht="16.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="170" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B35" s="171"/>
       <c r="C35" s="171"/>
@@ -5956,46 +6062,46 @@
       <c r="M35" s="171"/>
       <c r="N35" s="172"/>
       <c r="Q35" s="57" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B36" s="173" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C36" s="174"/>
       <c r="D36" s="175" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="E36" s="175"/>
       <c r="F36" s="175"/>
       <c r="G36" s="175"/>
       <c r="H36" s="175"/>
       <c r="I36" s="176" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J36" s="176"/>
       <c r="K36" s="176"/>
       <c r="L36" s="177"/>
       <c r="M36" s="178" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N36" s="179"/>
       <c r="Q36" s="57" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="69"/>
       <c r="B37" s="103" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C37" s="155"/>
       <c r="D37" s="180" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E37" s="181"/>
       <c r="F37" s="182"/>
@@ -6010,44 +6116,48 @@
       <c r="K37" s="184"/>
       <c r="L37" s="185"/>
       <c r="M37" s="186" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="N37" s="187"/>
       <c r="Q37" s="57" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="188"/>
       <c r="B38" s="189" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C38" s="190"/>
       <c r="D38" s="180" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E38" s="181"/>
       <c r="F38" s="181"/>
       <c r="G38" s="181"/>
       <c r="H38" s="182"/>
-      <c r="I38" s="184"/>
+      <c r="I38" s="184" t="s">
+        <v>122</v>
+      </c>
       <c r="J38" s="184"/>
       <c r="K38" s="184"/>
       <c r="L38" s="185"/>
-      <c r="M38" s="186"/>
+      <c r="M38" s="186" t="s">
+        <v>123</v>
+      </c>
       <c r="N38" s="187"/>
       <c r="Q38" s="57" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="191"/>
       <c r="B39" s="73" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C39" s="83"/>
       <c r="D39" s="192" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E39" s="192"/>
       <c r="F39" s="192"/>
@@ -6060,17 +6170,17 @@
       <c r="M39" s="186"/>
       <c r="N39" s="187"/>
       <c r="Q39" s="57" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="191"/>
       <c r="B40" s="73" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C40" s="83"/>
       <c r="D40" s="192" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E40" s="192"/>
       <c r="F40" s="192"/>
@@ -6083,17 +6193,17 @@
       <c r="M40" s="186"/>
       <c r="N40" s="187"/>
       <c r="Q40" s="57" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="191"/>
       <c r="B41" s="73" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C41" s="83"/>
       <c r="D41" s="192" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E41" s="192"/>
       <c r="F41" s="192"/>
@@ -6106,17 +6216,17 @@
       <c r="M41" s="186"/>
       <c r="N41" s="187"/>
       <c r="Q41" s="57" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="93"/>
       <c r="B42" s="94" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C42" s="193"/>
       <c r="D42" s="192" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E42" s="192"/>
       <c r="F42" s="192"/>
@@ -6129,19 +6239,19 @@
       <c r="M42" s="186"/>
       <c r="N42" s="187"/>
       <c r="Q42" s="57" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="194" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B43" s="195" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C43" s="94"/>
       <c r="D43" s="192" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="E43" s="192"/>
       <c r="F43" s="192"/>
@@ -6154,7 +6264,7 @@
       <c r="M43" s="186"/>
       <c r="N43" s="187"/>
       <c r="Q43" s="57" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6164,12 +6274,12 @@
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="180" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="E44" s="181"/>
       <c r="F44" s="182"/>
       <c r="G44" s="183" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H44" s="183"/>
       <c r="I44" s="184"/>
@@ -6179,7 +6289,7 @@
       <c r="M44" s="186"/>
       <c r="N44" s="187"/>
       <c r="Q44" s="57" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6189,7 +6299,7 @@
       </c>
       <c r="C45" s="131"/>
       <c r="D45" s="180" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E45" s="181"/>
       <c r="F45" s="181"/>
@@ -6202,15 +6312,15 @@
       <c r="M45" s="186"/>
       <c r="N45" s="187"/>
       <c r="Q45" s="57" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="69" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B46" s="127" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C46" s="127"/>
       <c r="D46" s="127"/>
@@ -6225,7 +6335,7 @@
       <c r="M46" s="186"/>
       <c r="N46" s="187"/>
       <c r="Q46" s="57" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6235,7 +6345,7 @@
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="196" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c r="E47" s="196"/>
       <c r="F47" s="196"/>
@@ -6248,7 +6358,7 @@
       <c r="M47" s="186"/>
       <c r="N47" s="187"/>
       <c r="Q47" s="57" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6258,7 +6368,7 @@
       </c>
       <c r="C48" s="41"/>
       <c r="D48" s="196" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="E48" s="196"/>
       <c r="F48" s="196"/>
@@ -6271,7 +6381,7 @@
       <c r="M48" s="186"/>
       <c r="N48" s="187"/>
       <c r="Q48" s="57" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6281,14 +6391,14 @@
       </c>
       <c r="C49" s="51"/>
       <c r="D49" s="198" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="E49" s="198"/>
       <c r="F49" s="198"/>
       <c r="G49" s="198"/>
       <c r="H49" s="198"/>
       <c r="I49" s="199" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="J49" s="199"/>
       <c r="K49" s="199"/>
@@ -6296,12 +6406,12 @@
       <c r="M49" s="199"/>
       <c r="N49" s="200"/>
       <c r="Q49" s="57" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="201" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B50" s="201"/>
       <c r="C50" s="202"/>
@@ -6311,7 +6421,7 @@
       <c r="G50" s="203"/>
       <c r="H50" s="203"/>
       <c r="I50" s="204" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="J50" s="204"/>
       <c r="K50" s="204"/>
@@ -6319,42 +6429,42 @@
       <c r="M50" s="204"/>
       <c r="N50" s="205"/>
       <c r="Q50" s="57" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="206" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B51" s="207" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C51" s="207"/>
       <c r="D51" s="208" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E51" s="209"/>
       <c r="F51" s="210"/>
       <c r="G51" s="208" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H51" s="209"/>
       <c r="I51" s="211"/>
       <c r="J51" s="212" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="K51" s="213"/>
       <c r="L51" s="214" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="M51" s="215" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="N51" s="216" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="Q51" s="57" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" ht="19.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6373,7 +6483,7 @@
       <c r="M52" s="215"/>
       <c r="N52" s="216"/>
       <c r="Q52" s="57" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6387,10 +6497,10 @@
       <c r="H53" s="226"/>
       <c r="I53" s="227"/>
       <c r="J53" s="228" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K53" s="229" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="L53" s="230"/>
       <c r="M53" s="231"/>
@@ -6398,69 +6508,83 @@
       <c r="O53" s="233"/>
       <c r="P53" s="233"/>
       <c r="Q53" s="57" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="234"/>
       <c r="B54" s="235" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C54" s="235"/>
-      <c r="D54" s="236"/>
+      <c r="D54" s="236" t="s">
+        <v>166</v>
+      </c>
       <c r="E54" s="237"/>
       <c r="F54" s="238"/>
-      <c r="G54" s="239"/>
+      <c r="G54" s="239" t="s">
+        <v>14</v>
+      </c>
       <c r="H54" s="240"/>
       <c r="I54" s="241"/>
-      <c r="J54" s="242"/>
-      <c r="K54" s="243"/>
-      <c r="L54" s="244"/>
-      <c r="M54" s="245"/>
-      <c r="N54" s="246"/>
+      <c r="J54" s="242" t="s">
+        <v>167</v>
+      </c>
+      <c r="K54" s="243" t="s">
+        <v>168</v>
+      </c>
+      <c r="L54" s="244" t="s">
+        <v>14</v>
+      </c>
+      <c r="M54" s="245" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" s="246" t="s">
+        <v>14</v>
+      </c>
       <c r="Q54" s="57" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="234"/>
       <c r="B55" s="235" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C55" s="235"/>
       <c r="D55" s="236" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="E55" s="237"/>
       <c r="F55" s="238"/>
       <c r="G55" s="239" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="H55" s="240"/>
       <c r="I55" s="241"/>
       <c r="J55" s="242" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="K55" s="247" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="L55" s="248" t="s">
         <v>14</v>
       </c>
       <c r="M55" s="249" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="N55" s="246" t="s">
         <v>14</v>
       </c>
       <c r="Q55" s="57" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="234"/>
       <c r="B56" s="235" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C56" s="235"/>
       <c r="D56" s="236"/>
@@ -6475,34 +6599,48 @@
       <c r="M56" s="245"/>
       <c r="N56" s="246"/>
       <c r="Q56" s="57" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="234"/>
       <c r="B57" s="235" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C57" s="235"/>
-      <c r="D57" s="236"/>
+      <c r="D57" s="236" t="s">
+        <v>179</v>
+      </c>
       <c r="E57" s="237"/>
       <c r="F57" s="238"/>
-      <c r="G57" s="250"/>
+      <c r="G57" s="250" t="s">
+        <v>180</v>
+      </c>
       <c r="H57" s="251"/>
       <c r="I57" s="252"/>
-      <c r="J57" s="242"/>
-      <c r="K57" s="247"/>
-      <c r="L57" s="244"/>
-      <c r="M57" s="249"/>
-      <c r="N57" s="246"/>
+      <c r="J57" s="242" t="s">
+        <v>181</v>
+      </c>
+      <c r="K57" s="247" t="s">
+        <v>182</v>
+      </c>
+      <c r="L57" s="244" t="s">
+        <v>183</v>
+      </c>
+      <c r="M57" s="249" t="s">
+        <v>184</v>
+      </c>
+      <c r="N57" s="246" t="s">
+        <v>14</v>
+      </c>
       <c r="Q57" s="57" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="253"/>
       <c r="B58" s="254" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="C58" s="254"/>
       <c r="D58" s="255"/>
@@ -6517,12 +6655,12 @@
       <c r="M58" s="264"/>
       <c r="N58" s="246"/>
       <c r="Q58" s="57" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" ht="12" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="265" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B59" s="266"/>
       <c r="C59" s="266"/>
@@ -6538,12 +6676,12 @@
       <c r="M59" s="266"/>
       <c r="N59" s="267"/>
       <c r="Q59" s="57" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" ht="27.75" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" ht="60" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="268" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B60" s="269"/>
       <c r="C60" s="270"/>
@@ -6554,21 +6692,23 @@
       <c r="H60" s="272"/>
       <c r="I60" s="273"/>
       <c r="J60" s="274" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="K60" s="275"/>
-      <c r="L60" s="276"/>
+      <c r="L60" s="276" t="s">
+        <v>191</v>
+      </c>
       <c r="M60" s="277"/>
       <c r="N60" s="278"/>
       <c r="Q60" s="57" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
     </row>
     <row r="61" ht="12" customHeight="1" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="279" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="B61" s="279"/>
       <c r="C61" s="279"/>
@@ -6584,7 +6724,7 @@
       <c r="M61" s="279"/>
       <c r="N61" s="279"/>
       <c r="Q61" s="280" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="R61" s="49"/>
       <c r="S61" s="49"/>
@@ -6605,7 +6745,7 @@
       <c r="M62" s="281"/>
       <c r="N62" s="281"/>
       <c r="Q62" s="57" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6624,7 +6764,7 @@
       <c r="M63" s="281"/>
       <c r="N63" s="281"/>
       <c r="Q63" s="57" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6643,7 +6783,7 @@
       <c r="M64" s="281"/>
       <c r="N64" s="281"/>
       <c r="Q64" s="57" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6662,7 +6802,7 @@
       <c r="M65" s="281"/>
       <c r="N65" s="281"/>
       <c r="Q65" s="57" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6681,7 +6821,7 @@
       <c r="M66" s="281"/>
       <c r="N66" s="281"/>
       <c r="Q66" s="57" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6700,7 +6840,7 @@
       <c r="M67" s="281"/>
       <c r="N67" s="281"/>
       <c r="Q67" s="57" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6719,7 +6859,7 @@
       <c r="M68" s="281"/>
       <c r="N68" s="281"/>
       <c r="Q68" s="57" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6738,7 +6878,7 @@
       <c r="M69" s="281"/>
       <c r="N69" s="281"/>
       <c r="Q69" s="57" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6757,7 +6897,7 @@
       <c r="M70" s="281"/>
       <c r="N70" s="281"/>
       <c r="Q70" s="57" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6776,7 +6916,7 @@
       <c r="M71" s="281"/>
       <c r="N71" s="281"/>
       <c r="Q71" s="57" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6795,7 +6935,7 @@
       <c r="M72" s="281"/>
       <c r="N72" s="281"/>
       <c r="Q72" s="57" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6814,7 +6954,7 @@
       <c r="M73" s="281"/>
       <c r="N73" s="281"/>
       <c r="Q73" s="57" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6833,7 +6973,7 @@
       <c r="M74" s="281"/>
       <c r="N74" s="281"/>
       <c r="Q74" s="57" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6852,7 +6992,7 @@
       <c r="M75" s="281"/>
       <c r="N75" s="281"/>
       <c r="Q75" s="57" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6871,7 +7011,7 @@
       <c r="M76" s="281"/>
       <c r="N76" s="281"/>
       <c r="Q76" s="57" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6890,7 +7030,7 @@
       <c r="M77" s="281"/>
       <c r="N77" s="281"/>
       <c r="Q77" s="57" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6909,7 +7049,7 @@
       <c r="M78" s="281"/>
       <c r="N78" s="281"/>
       <c r="Q78" s="57" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6928,7 +7068,7 @@
       <c r="M79" s="281"/>
       <c r="N79" s="281"/>
       <c r="Q79" s="57" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6947,7 +7087,7 @@
       <c r="M80" s="281"/>
       <c r="N80" s="281"/>
       <c r="Q80" s="57" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6966,7 +7106,7 @@
       <c r="M81" s="281"/>
       <c r="N81" s="281"/>
       <c r="Q81" s="57" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6985,7 +7125,7 @@
       <c r="M82" s="281"/>
       <c r="N82" s="281"/>
       <c r="Q82" s="57" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7004,7 +7144,7 @@
       <c r="M83" s="281"/>
       <c r="N83" s="281"/>
       <c r="Q83" s="57" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7023,7 +7163,7 @@
       <c r="M84" s="281"/>
       <c r="N84" s="281"/>
       <c r="Q84" s="57" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7042,7 +7182,7 @@
       <c r="M85" s="281"/>
       <c r="N85" s="281"/>
       <c r="Q85" s="57" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7061,7 +7201,7 @@
       <c r="M86" s="281"/>
       <c r="N86" s="281"/>
       <c r="Q86" s="57" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7080,7 +7220,7 @@
       <c r="M87" s="281"/>
       <c r="N87" s="281"/>
       <c r="Q87" s="57" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7099,7 +7239,7 @@
       <c r="M88" s="281"/>
       <c r="N88" s="281"/>
       <c r="Q88" s="57" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7118,7 +7258,7 @@
       <c r="M89" s="281"/>
       <c r="N89" s="281"/>
       <c r="Q89" s="57" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
     </row>
     <row r="90" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7137,7 +7277,7 @@
       <c r="M90" s="281"/>
       <c r="N90" s="281"/>
       <c r="Q90" s="57" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7156,7 +7296,7 @@
       <c r="M91" s="281"/>
       <c r="N91" s="281"/>
       <c r="Q91" s="57" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7175,7 +7315,7 @@
       <c r="M92" s="281"/>
       <c r="N92" s="281"/>
       <c r="Q92" s="57" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7194,7 +7334,7 @@
       <c r="M93" s="281"/>
       <c r="N93" s="281"/>
       <c r="Q93" s="57" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7213,7 +7353,7 @@
       <c r="M94" s="281"/>
       <c r="N94" s="281"/>
       <c r="Q94" s="57" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7232,7 +7372,7 @@
       <c r="M95" s="281"/>
       <c r="N95" s="281"/>
       <c r="Q95" s="57" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7251,7 +7391,7 @@
       <c r="M96" s="281"/>
       <c r="N96" s="281"/>
       <c r="Q96" s="57" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7270,7 +7410,7 @@
       <c r="M97" s="281"/>
       <c r="N97" s="281"/>
       <c r="Q97" s="57" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7289,7 +7429,7 @@
       <c r="M98" s="281"/>
       <c r="N98" s="281"/>
       <c r="Q98" s="57" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7308,7 +7448,7 @@
       <c r="M99" s="281"/>
       <c r="N99" s="281"/>
       <c r="Q99" s="57" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7327,7 +7467,7 @@
       <c r="M100" s="281"/>
       <c r="N100" s="281"/>
       <c r="Q100" s="57" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7346,7 +7486,7 @@
       <c r="M101" s="281"/>
       <c r="N101" s="281"/>
       <c r="Q101" s="57" t="s">
-        <v>214</v>
+        <v>43</v>
       </c>
     </row>
     <row r="102" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7365,7 +7505,7 @@
       <c r="M102" s="281"/>
       <c r="N102" s="281"/>
       <c r="Q102" s="57" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
     </row>
     <row r="103" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7384,7 +7524,7 @@
       <c r="M103" s="281"/>
       <c r="N103" s="281"/>
       <c r="Q103" s="57" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7403,7 +7543,7 @@
       <c r="M104" s="281"/>
       <c r="N104" s="281"/>
       <c r="Q104" s="57" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7422,7 +7562,7 @@
       <c r="M105" s="281"/>
       <c r="N105" s="281"/>
       <c r="Q105" s="57" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
     </row>
     <row r="106" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7441,7 +7581,7 @@
       <c r="M106" s="281"/>
       <c r="N106" s="281"/>
       <c r="Q106" s="57" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7460,7 +7600,7 @@
       <c r="M107" s="281"/>
       <c r="N107" s="281"/>
       <c r="Q107" s="57" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7479,7 +7619,7 @@
       <c r="M108" s="281"/>
       <c r="N108" s="281"/>
       <c r="Q108" s="57" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7498,7 +7638,7 @@
       <c r="M109" s="281"/>
       <c r="N109" s="281"/>
       <c r="Q109" s="57" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7517,7 +7657,7 @@
       <c r="M110" s="281"/>
       <c r="N110" s="281"/>
       <c r="Q110" s="57" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7536,7 +7676,7 @@
       <c r="M111" s="281"/>
       <c r="N111" s="281"/>
       <c r="Q111" s="57" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7555,7 +7695,7 @@
       <c r="M112" s="281"/>
       <c r="N112" s="281"/>
       <c r="Q112" s="57" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7574,7 +7714,7 @@
       <c r="M113" s="281"/>
       <c r="N113" s="281"/>
       <c r="Q113" s="57" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7593,7 +7733,7 @@
       <c r="M114" s="281"/>
       <c r="N114" s="281"/>
       <c r="Q114" s="57" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7612,7 +7752,7 @@
       <c r="M115" s="281"/>
       <c r="N115" s="281"/>
       <c r="Q115" s="57" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7631,7 +7771,7 @@
       <c r="M116" s="281"/>
       <c r="N116" s="281"/>
       <c r="Q116" s="57" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7650,7 +7790,7 @@
       <c r="M117" s="281"/>
       <c r="N117" s="281"/>
       <c r="Q117" s="57" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7669,7 +7809,7 @@
       <c r="M118" s="281"/>
       <c r="N118" s="281"/>
       <c r="Q118" s="57" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7688,7 +7828,7 @@
       <c r="M119" s="281"/>
       <c r="N119" s="281"/>
       <c r="Q119" s="57" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7707,7 +7847,7 @@
       <c r="M120" s="281"/>
       <c r="N120" s="281"/>
       <c r="Q120" s="57" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7726,7 +7866,7 @@
       <c r="M121" s="281"/>
       <c r="N121" s="281"/>
       <c r="Q121" s="57" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7745,7 +7885,7 @@
       <c r="M122" s="281"/>
       <c r="N122" s="281"/>
       <c r="Q122" s="57" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
     </row>
     <row r="123" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7764,7 +7904,7 @@
       <c r="M123" s="281"/>
       <c r="N123" s="281"/>
       <c r="Q123" s="57" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7783,7 +7923,7 @@
       <c r="M124" s="281"/>
       <c r="N124" s="281"/>
       <c r="Q124" s="57" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7802,7 +7942,7 @@
       <c r="M125" s="281"/>
       <c r="N125" s="281"/>
       <c r="Q125" s="57" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7821,7 +7961,7 @@
       <c r="M126" s="281"/>
       <c r="N126" s="281"/>
       <c r="Q126" s="57" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7840,7 +7980,7 @@
       <c r="M127" s="281"/>
       <c r="N127" s="281"/>
       <c r="Q127" s="57" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7859,7 +7999,7 @@
       <c r="M128" s="281"/>
       <c r="N128" s="281"/>
       <c r="Q128" s="57" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
     </row>
     <row r="129" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7878,7 +8018,7 @@
       <c r="M129" s="281"/>
       <c r="N129" s="281"/>
       <c r="Q129" s="57" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="130" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7897,7 +8037,7 @@
       <c r="M130" s="281"/>
       <c r="N130" s="281"/>
       <c r="Q130" s="57" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7916,7 +8056,7 @@
       <c r="M131" s="281"/>
       <c r="N131" s="281"/>
       <c r="Q131" s="57" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7935,7 +8075,7 @@
       <c r="M132" s="281"/>
       <c r="N132" s="281"/>
       <c r="Q132" s="57" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7954,7 +8094,7 @@
       <c r="M133" s="281"/>
       <c r="N133" s="281"/>
       <c r="Q133" s="57" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7973,7 +8113,7 @@
       <c r="M134" s="281"/>
       <c r="N134" s="281"/>
       <c r="Q134" s="57" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7992,7 +8132,7 @@
       <c r="M135" s="281"/>
       <c r="N135" s="281"/>
       <c r="Q135" s="57" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8011,7 +8151,7 @@
       <c r="M136" s="281"/>
       <c r="N136" s="281"/>
       <c r="Q136" s="57" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8030,7 +8170,7 @@
       <c r="M137" s="281"/>
       <c r="N137" s="281"/>
       <c r="Q137" s="57" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8049,7 +8189,7 @@
       <c r="M138" s="281"/>
       <c r="N138" s="281"/>
       <c r="Q138" s="57" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8068,7 +8208,7 @@
       <c r="M139" s="281"/>
       <c r="N139" s="281"/>
       <c r="Q139" s="57" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8087,7 +8227,7 @@
       <c r="M140" s="281"/>
       <c r="N140" s="281"/>
       <c r="Q140" s="57" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8106,7 +8246,7 @@
       <c r="M141" s="281"/>
       <c r="N141" s="281"/>
       <c r="Q141" s="57" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8125,7 +8265,7 @@
       <c r="M142" s="281"/>
       <c r="N142" s="281"/>
       <c r="Q142" s="57" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8144,7 +8284,7 @@
       <c r="M143" s="281"/>
       <c r="N143" s="281"/>
       <c r="Q143" s="57" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8163,7 +8303,7 @@
       <c r="M144" s="281"/>
       <c r="N144" s="281"/>
       <c r="Q144" s="57" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8182,7 +8322,7 @@
       <c r="M145" s="281"/>
       <c r="N145" s="281"/>
       <c r="Q145" s="57" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8201,7 +8341,7 @@
       <c r="M146" s="281"/>
       <c r="N146" s="281"/>
       <c r="Q146" s="57" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8220,7 +8360,7 @@
       <c r="M147" s="281"/>
       <c r="N147" s="281"/>
       <c r="Q147" s="57" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8239,7 +8379,7 @@
       <c r="M148" s="281"/>
       <c r="N148" s="281"/>
       <c r="Q148" s="57" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8258,7 +8398,7 @@
       <c r="M149" s="281"/>
       <c r="N149" s="281"/>
       <c r="Q149" s="57" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
     </row>
     <row r="150" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8277,7 +8417,7 @@
       <c r="M150" s="281"/>
       <c r="N150" s="281"/>
       <c r="Q150" s="57" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
     </row>
     <row r="151" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8296,7 +8436,7 @@
       <c r="M151" s="281"/>
       <c r="N151" s="281"/>
       <c r="Q151" s="57" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8315,7 +8455,7 @@
       <c r="M152" s="281"/>
       <c r="N152" s="281"/>
       <c r="Q152" s="57" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
     </row>
     <row r="153" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8334,7 +8474,7 @@
       <c r="M153" s="281"/>
       <c r="N153" s="281"/>
       <c r="Q153" s="57" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
     </row>
     <row r="154" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8353,7 +8493,7 @@
       <c r="M154" s="281"/>
       <c r="N154" s="281"/>
       <c r="Q154" s="57" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="155" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8372,7 +8512,7 @@
       <c r="M155" s="281"/>
       <c r="N155" s="281"/>
       <c r="Q155" s="57" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8391,7 +8531,7 @@
       <c r="M156" s="281"/>
       <c r="N156" s="281"/>
       <c r="Q156" s="57" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8410,7 +8550,7 @@
       <c r="M157" s="281"/>
       <c r="N157" s="281"/>
       <c r="Q157" s="57" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8429,7 +8569,7 @@
       <c r="M158" s="281"/>
       <c r="N158" s="281"/>
       <c r="Q158" s="57" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
     </row>
     <row r="159" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8448,7 +8588,7 @@
       <c r="M159" s="281"/>
       <c r="N159" s="281"/>
       <c r="Q159" s="57" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
     </row>
     <row r="160" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8467,7 +8607,7 @@
       <c r="M160" s="281"/>
       <c r="N160" s="281"/>
       <c r="Q160" s="57" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
     </row>
     <row r="161" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8486,7 +8626,7 @@
       <c r="M161" s="281"/>
       <c r="N161" s="281"/>
       <c r="Q161" s="57" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
     </row>
     <row r="162" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8505,7 +8645,7 @@
       <c r="M162" s="281"/>
       <c r="N162" s="281"/>
       <c r="Q162" s="57" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
     </row>
     <row r="163" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8524,7 +8664,7 @@
       <c r="M163" s="281"/>
       <c r="N163" s="281"/>
       <c r="Q163" s="57" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
     </row>
     <row r="164" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8543,7 +8683,7 @@
       <c r="M164" s="281"/>
       <c r="N164" s="281"/>
       <c r="Q164" s="57" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
     </row>
     <row r="165" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8562,7 +8702,7 @@
       <c r="M165" s="281"/>
       <c r="N165" s="281"/>
       <c r="Q165" s="57" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
     </row>
     <row r="166" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8581,7 +8721,7 @@
       <c r="M166" s="281"/>
       <c r="N166" s="281"/>
       <c r="Q166" s="57" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
     </row>
     <row r="167" ht="42.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8600,7 +8740,7 @@
       <c r="M167" s="281"/>
       <c r="N167" s="281"/>
       <c r="Q167" s="57" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="168" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8619,7 +8759,7 @@
       <c r="M168" s="281"/>
       <c r="N168" s="281"/>
       <c r="Q168" s="57" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
     </row>
     <row r="169" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8638,7 +8778,7 @@
       <c r="M169" s="281"/>
       <c r="N169" s="281"/>
       <c r="Q169" s="57" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
     </row>
     <row r="170" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8657,7 +8797,7 @@
       <c r="M170" s="281"/>
       <c r="N170" s="281"/>
       <c r="Q170" s="57" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
     </row>
     <row r="171" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8676,7 +8816,7 @@
       <c r="M171" s="281"/>
       <c r="N171" s="281"/>
       <c r="Q171" s="57" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
     </row>
     <row r="172" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8695,7 +8835,7 @@
       <c r="M172" s="281"/>
       <c r="N172" s="281"/>
       <c r="Q172" s="57" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
     </row>
     <row r="173" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8714,7 +8854,7 @@
       <c r="M173" s="281"/>
       <c r="N173" s="281"/>
       <c r="Q173" s="57" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
     </row>
     <row r="174" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8733,7 +8873,7 @@
       <c r="M174" s="281"/>
       <c r="N174" s="281"/>
       <c r="Q174" s="57" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
     </row>
     <row r="175" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8752,7 +8892,7 @@
       <c r="M175" s="281"/>
       <c r="N175" s="281"/>
       <c r="Q175" s="57" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
     </row>
     <row r="176" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8771,7 +8911,7 @@
       <c r="M176" s="281"/>
       <c r="N176" s="281"/>
       <c r="Q176" s="57" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8790,7 +8930,7 @@
       <c r="M177" s="281"/>
       <c r="N177" s="281"/>
       <c r="Q177" s="57" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
     </row>
     <row r="178" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8809,7 +8949,7 @@
       <c r="M178" s="281"/>
       <c r="N178" s="281"/>
       <c r="Q178" s="57" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
     </row>
     <row r="179" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8828,7 +8968,7 @@
       <c r="M179" s="281"/>
       <c r="N179" s="281"/>
       <c r="Q179" s="57" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
     </row>
     <row r="180" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8847,7 +8987,7 @@
       <c r="M180" s="281"/>
       <c r="N180" s="281"/>
       <c r="Q180" s="57" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
     </row>
     <row r="181" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8866,7 +9006,7 @@
       <c r="M181" s="281"/>
       <c r="N181" s="281"/>
       <c r="Q181" s="57" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
     </row>
     <row r="182" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8885,7 +9025,7 @@
       <c r="M182" s="281"/>
       <c r="N182" s="281"/>
       <c r="Q182" s="57" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
     </row>
     <row r="183" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8904,7 +9044,7 @@
       <c r="M183" s="281"/>
       <c r="N183" s="281"/>
       <c r="Q183" s="57" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
     </row>
     <row r="184" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8923,7 +9063,7 @@
       <c r="M184" s="281"/>
       <c r="N184" s="281"/>
       <c r="Q184" s="57" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
     </row>
     <row r="185" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8942,7 +9082,7 @@
       <c r="M185" s="281"/>
       <c r="N185" s="281"/>
       <c r="Q185" s="57" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
     </row>
     <row r="186" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8961,7 +9101,7 @@
       <c r="M186" s="281"/>
       <c r="N186" s="281"/>
       <c r="Q186" s="57" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
     </row>
     <row r="187" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8980,7 +9120,7 @@
       <c r="M187" s="281"/>
       <c r="N187" s="281"/>
       <c r="Q187" s="57" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
     </row>
     <row r="188" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8999,7 +9139,7 @@
       <c r="M188" s="281"/>
       <c r="N188" s="281"/>
       <c r="Q188" s="57" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
     </row>
     <row r="189" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9018,7 +9158,7 @@
       <c r="M189" s="281"/>
       <c r="N189" s="281"/>
       <c r="Q189" s="57" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
     </row>
     <row r="190" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9037,7 +9177,7 @@
       <c r="M190" s="281"/>
       <c r="N190" s="281"/>
       <c r="Q190" s="57" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
     </row>
     <row r="191" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9056,7 +9196,7 @@
       <c r="M191" s="281"/>
       <c r="N191" s="281"/>
       <c r="Q191" s="57" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
     </row>
     <row r="192" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9075,7 +9215,7 @@
       <c r="M192" s="281"/>
       <c r="N192" s="281"/>
       <c r="Q192" s="57" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="193" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9094,7 +9234,7 @@
       <c r="M193" s="281"/>
       <c r="N193" s="281"/>
       <c r="Q193" s="57" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
     </row>
     <row r="194" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9113,7 +9253,7 @@
       <c r="M194" s="281"/>
       <c r="N194" s="281"/>
       <c r="Q194" s="57" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
     </row>
     <row r="195" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9132,7 +9272,7 @@
       <c r="M195" s="281"/>
       <c r="N195" s="281"/>
       <c r="Q195" s="57" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
     </row>
     <row r="196" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9151,7 +9291,7 @@
       <c r="M196" s="281"/>
       <c r="N196" s="281"/>
       <c r="Q196" s="57" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
     </row>
     <row r="197" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9170,7 +9310,7 @@
       <c r="M197" s="281"/>
       <c r="N197" s="281"/>
       <c r="Q197" s="57" t="s">
-        <v>310</v>
+        <v>329</v>
       </c>
     </row>
     <row r="198" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9189,7 +9329,7 @@
       <c r="M198" s="281"/>
       <c r="N198" s="281"/>
       <c r="Q198" s="57" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="199" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9208,7 +9348,7 @@
       <c r="M199" s="281"/>
       <c r="N199" s="281"/>
       <c r="Q199" s="57" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
     </row>
     <row r="200" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9227,7 +9367,7 @@
       <c r="M200" s="281"/>
       <c r="N200" s="281"/>
       <c r="Q200" s="57" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
     </row>
     <row r="201" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9246,7 +9386,7 @@
       <c r="M201" s="281"/>
       <c r="N201" s="281"/>
       <c r="Q201" s="57" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
     </row>
     <row r="202" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9265,7 +9405,7 @@
       <c r="M202" s="281"/>
       <c r="N202" s="281"/>
       <c r="Q202" s="57" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
     </row>
     <row r="203" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9284,7 +9424,7 @@
       <c r="M203" s="281"/>
       <c r="N203" s="281"/>
       <c r="Q203" s="57" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
     </row>
     <row r="204" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9303,7 +9443,7 @@
       <c r="M204" s="281"/>
       <c r="N204" s="281"/>
       <c r="Q204" s="57" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
     </row>
     <row r="205" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9322,7 +9462,7 @@
       <c r="M205" s="281"/>
       <c r="N205" s="281"/>
       <c r="Q205" s="57" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
     </row>
     <row r="206" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9341,7 +9481,7 @@
       <c r="M206" s="281"/>
       <c r="N206" s="281"/>
       <c r="Q206" s="57" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
     </row>
     <row r="207" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9360,7 +9500,7 @@
       <c r="M207" s="281"/>
       <c r="N207" s="281"/>
       <c r="Q207" s="57" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
     </row>
     <row r="208" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9379,7 +9519,7 @@
       <c r="M208" s="281"/>
       <c r="N208" s="281"/>
       <c r="Q208" s="57" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
     </row>
     <row r="209" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9398,7 +9538,7 @@
       <c r="M209" s="281"/>
       <c r="N209" s="281"/>
       <c r="Q209" s="57" t="s">
-        <v>322</v>
+        <v>341</v>
       </c>
     </row>
     <row r="210" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9417,7 +9557,7 @@
       <c r="M210" s="281"/>
       <c r="N210" s="281"/>
       <c r="Q210" s="57" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
     </row>
     <row r="211" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9436,7 +9576,7 @@
       <c r="M211" s="281"/>
       <c r="N211" s="281"/>
       <c r="Q211" s="57" t="s">
-        <v>324</v>
+        <v>343</v>
       </c>
     </row>
     <row r="212" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9455,7 +9595,7 @@
       <c r="M212" s="281"/>
       <c r="N212" s="281"/>
       <c r="Q212" s="57" t="s">
-        <v>325</v>
+        <v>344</v>
       </c>
     </row>
     <row r="213" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9474,7 +9614,7 @@
       <c r="M213" s="281"/>
       <c r="N213" s="281"/>
       <c r="Q213" s="57" t="s">
-        <v>326</v>
+        <v>345</v>
       </c>
     </row>
     <row r="214" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9493,7 +9633,7 @@
       <c r="M214" s="281"/>
       <c r="N214" s="281"/>
       <c r="Q214" s="57" t="s">
-        <v>327</v>
+        <v>346</v>
       </c>
     </row>
     <row r="215" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9512,7 +9652,7 @@
       <c r="M215" s="281"/>
       <c r="N215" s="281"/>
       <c r="Q215" s="57" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
     </row>
     <row r="216" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9531,7 +9671,7 @@
       <c r="M216" s="281"/>
       <c r="N216" s="281"/>
       <c r="Q216" s="57" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.25">
@@ -10654,6 +10794,7 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.3" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="80" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <drawing r:id="rId205"/>
 </worksheet>
 </file>
 
@@ -10702,7 +10843,7 @@
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="286" t="s">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="B2" s="287"/>
       <c r="C2" s="287"/>
@@ -10719,28 +10860,28 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="289" t="s">
-        <v>331</v>
+        <v>350</v>
       </c>
       <c r="B3" s="290" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="C3" s="290"/>
       <c r="D3" s="290"/>
       <c r="E3" s="291"/>
       <c r="F3" s="292" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="G3" s="293" t="s">
-        <v>334</v>
+        <v>353</v>
       </c>
       <c r="H3" s="291"/>
       <c r="I3" s="293" t="s">
-        <v>335</v>
+        <v>354</v>
       </c>
       <c r="J3" s="290"/>
       <c r="K3" s="291"/>
       <c r="L3" s="294" t="s">
-        <v>336</v>
+        <v>355</v>
       </c>
       <c r="M3" s="295"/>
     </row>
@@ -10757,10 +10898,10 @@
       <c r="J4" s="297"/>
       <c r="K4" s="298"/>
       <c r="L4" s="301" t="s">
-        <v>337</v>
+        <v>356</v>
       </c>
       <c r="M4" s="302" t="s">
-        <v>338</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -10870,7 +11011,7 @@
     </row>
     <row r="12" ht="12" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="317" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B12" s="318"/>
       <c r="C12" s="318"/>
@@ -10887,7 +11028,7 @@
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="170" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="B13" s="171"/>
       <c r="C13" s="171"/>
@@ -10904,7 +11045,7 @@
     </row>
     <row r="14" ht="12" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="320" t="s">
-        <v>340</v>
+        <v>359</v>
       </c>
       <c r="B14" s="203"/>
       <c r="C14" s="203"/>
@@ -10921,33 +11062,33 @@
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="296" t="s">
-        <v>341</v>
+        <v>360</v>
       </c>
       <c r="B15" s="322" t="s">
-        <v>342</v>
+        <v>361</v>
       </c>
       <c r="C15" s="323"/>
       <c r="D15" s="324" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
       <c r="E15" s="322"/>
       <c r="F15" s="323"/>
       <c r="G15" s="324" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
       <c r="H15" s="322"/>
       <c r="I15" s="323"/>
       <c r="J15" s="325" t="s">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="K15" s="326" t="s">
-        <v>346</v>
+        <v>365</v>
       </c>
       <c r="L15" s="327" t="s">
-        <v>347</v>
+        <v>366</v>
       </c>
       <c r="M15" s="328" t="s">
-        <v>348</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -10967,11 +11108,11 @@
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="330" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B17" s="331"/>
       <c r="C17" s="332" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D17" s="300"/>
       <c r="E17" s="297"/>
@@ -11406,7 +11547,7 @@
     </row>
     <row r="46" ht="9.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="346" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B46" s="347"/>
       <c r="C46" s="347"/>
@@ -11423,7 +11564,7 @@
     </row>
     <row r="47" ht="27.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="268" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B47" s="269"/>
       <c r="C47" s="270"/>
@@ -11433,7 +11574,7 @@
       <c r="G47" s="351"/>
       <c r="H47" s="352"/>
       <c r="I47" s="353" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="J47" s="354"/>
       <c r="K47" s="355"/>
@@ -11443,7 +11584,7 @@
     </row>
     <row r="48" ht="9" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="358" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="B48" s="358"/>
       <c r="C48" s="358"/>
@@ -11637,7 +11778,7 @@
     </row>
     <row r="2" ht="22.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="363" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
       <c r="B2" s="364"/>
       <c r="C2" s="364"/>
@@ -11652,22 +11793,22 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="366" t="s">
-        <v>351</v>
+        <v>370</v>
       </c>
       <c r="B3" s="367" t="s">
-        <v>352</v>
+        <v>371</v>
       </c>
       <c r="C3" s="367"/>
       <c r="D3" s="368"/>
       <c r="E3" s="290" t="s">
-        <v>353</v>
+        <v>372</v>
       </c>
       <c r="F3" s="291"/>
       <c r="G3" s="369" t="s">
-        <v>354</v>
+        <v>373</v>
       </c>
       <c r="H3" s="293" t="s">
-        <v>355</v>
+        <v>374</v>
       </c>
       <c r="I3" s="370"/>
       <c r="J3" s="370"/>
@@ -11692,10 +11833,10 @@
       <c r="C5" s="378"/>
       <c r="D5" s="379"/>
       <c r="E5" s="331" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F5" s="332" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G5" s="334"/>
       <c r="H5" s="380"/>
@@ -11796,7 +11937,7 @@
     </row>
     <row r="13" ht="11.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="317" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B13" s="318"/>
       <c r="C13" s="318"/>
@@ -11811,7 +11952,7 @@
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:11" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="395" t="s">
-        <v>356</v>
+        <v>375</v>
       </c>
       <c r="B14" s="396"/>
       <c r="C14" s="396"/>
@@ -11826,25 +11967,25 @@
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="372" t="s">
-        <v>357</v>
+        <v>376</v>
       </c>
       <c r="B15" s="322" t="s">
-        <v>358</v>
+        <v>377</v>
       </c>
       <c r="C15" s="282"/>
       <c r="D15" s="398"/>
       <c r="E15" s="322" t="s">
-        <v>359</v>
+        <v>378</v>
       </c>
       <c r="F15" s="323"/>
       <c r="G15" s="326" t="s">
-        <v>354</v>
+        <v>373</v>
       </c>
       <c r="H15" s="325" t="s">
-        <v>360</v>
+        <v>379</v>
       </c>
       <c r="I15" s="324" t="s">
-        <v>361</v>
+        <v>380</v>
       </c>
       <c r="J15" s="282"/>
       <c r="K15" s="376"/>
@@ -11868,10 +12009,10 @@
       <c r="C17" s="125"/>
       <c r="D17" s="399"/>
       <c r="E17" s="331" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F17" s="332" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G17" s="334"/>
       <c r="H17" s="333"/>
@@ -12154,7 +12295,7 @@
     </row>
     <row r="39" ht="13.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="265" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B39" s="266"/>
       <c r="C39" s="266"/>
@@ -12169,7 +12310,7 @@
     </row>
     <row r="40" ht="22.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="420" t="s">
-        <v>362</v>
+        <v>381</v>
       </c>
       <c r="B40" s="421"/>
       <c r="C40" s="421"/>
@@ -12184,26 +12325,26 @@
     </row>
     <row r="41" ht="33.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="423" t="s">
-        <v>363</v>
+        <v>382</v>
       </c>
       <c r="B41" s="424" t="s">
-        <v>364</v>
+        <v>383</v>
       </c>
       <c r="C41" s="425" t="s">
-        <v>365</v>
+        <v>384</v>
       </c>
       <c r="D41" s="424" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
       <c r="E41" s="424"/>
       <c r="F41" s="424"/>
       <c r="G41" s="424"/>
       <c r="H41" s="426"/>
       <c r="I41" s="425" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
       <c r="J41" s="424" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="K41" s="427"/>
     </row>
@@ -12300,7 +12441,7 @@
     </row>
     <row r="49" ht="11.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="265" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B49" s="266"/>
       <c r="C49" s="266"/>
@@ -12315,7 +12456,7 @@
     </row>
     <row r="50" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="268" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B50" s="270"/>
       <c r="C50" s="350"/>
@@ -12323,7 +12464,7 @@
       <c r="E50" s="351"/>
       <c r="F50" s="352"/>
       <c r="G50" s="433" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="H50" s="434"/>
       <c r="I50" s="350"/>
@@ -12334,7 +12475,7 @@
     </row>
     <row r="51" ht="9.75" customHeight="1" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K51" s="436" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12475,11 +12616,11 @@
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="440" t="s">
-        <v>370</v>
+        <v>389</v>
       </c>
       <c r="B2" s="441"/>
       <c r="C2" s="442" t="s">
-        <v>371</v>
+        <v>390</v>
       </c>
       <c r="D2" s="442"/>
       <c r="E2" s="442"/>
@@ -12496,7 +12637,7 @@
       <c r="A3" s="448"/>
       <c r="B3" s="449"/>
       <c r="C3" s="450" t="s">
-        <v>372</v>
+        <v>391</v>
       </c>
       <c r="D3" s="450"/>
       <c r="E3" s="450"/>
@@ -12513,7 +12654,7 @@
       <c r="A4" s="448"/>
       <c r="B4" s="449"/>
       <c r="C4" s="450" t="s">
-        <v>373</v>
+        <v>392</v>
       </c>
       <c r="D4" s="450"/>
       <c r="E4" s="450"/>
@@ -12545,7 +12686,7 @@
       <c r="A6" s="448"/>
       <c r="B6" s="449"/>
       <c r="C6" s="450" t="s">
-        <v>374</v>
+        <v>393</v>
       </c>
       <c r="D6" s="450"/>
       <c r="E6" s="450"/>
@@ -12577,7 +12718,7 @@
       <c r="A8" s="448"/>
       <c r="B8" s="449"/>
       <c r="C8" s="450" t="s">
-        <v>375</v>
+        <v>394</v>
       </c>
       <c r="D8" s="450"/>
       <c r="E8" s="450"/>
@@ -12613,7 +12754,7 @@
       <c r="E10" s="450"/>
       <c r="F10" s="451"/>
       <c r="G10" s="456" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
       <c r="H10" s="456"/>
       <c r="I10" s="456"/>
@@ -12654,11 +12795,11 @@
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="469" t="s">
-        <v>377</v>
+        <v>396</v>
       </c>
       <c r="B13" s="470"/>
       <c r="C13" s="471" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
       <c r="D13" s="471"/>
       <c r="E13" s="282"/>
@@ -12679,7 +12820,7 @@
       <c r="E14" s="282"/>
       <c r="F14" s="398"/>
       <c r="G14" s="476" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
       <c r="H14" s="456"/>
       <c r="I14" s="456"/>
@@ -12737,7 +12878,7 @@
       <c r="A18" s="484"/>
       <c r="B18" s="485"/>
       <c r="C18" s="492" t="s">
-        <v>379</v>
+        <v>398</v>
       </c>
       <c r="D18" s="492"/>
       <c r="E18" s="493"/>
@@ -12758,7 +12899,7 @@
       <c r="E19" s="493"/>
       <c r="F19" s="494"/>
       <c r="G19" s="476" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
       <c r="H19" s="456"/>
       <c r="I19" s="456"/>
@@ -12776,7 +12917,7 @@
       <c r="F20" s="494"/>
       <c r="G20" s="495"/>
       <c r="H20" s="497" t="s">
-        <v>380</v>
+        <v>399</v>
       </c>
       <c r="I20" s="497"/>
       <c r="J20" s="498"/>
@@ -12792,7 +12933,7 @@
       <c r="E21" s="493"/>
       <c r="F21" s="494"/>
       <c r="G21" s="501" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="H21" s="502"/>
       <c r="I21" s="502"/>
@@ -12809,7 +12950,7 @@
       <c r="E22" s="506"/>
       <c r="F22" s="507"/>
       <c r="G22" s="480" t="s">
-        <v>382</v>
+        <v>401</v>
       </c>
       <c r="H22" s="481"/>
       <c r="I22" s="508"/>
@@ -12820,11 +12961,11 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="194" t="s">
-        <v>383</v>
+        <v>402</v>
       </c>
       <c r="B23" s="195"/>
       <c r="C23" s="510" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="D23" s="510"/>
       <c r="E23" s="510"/>
@@ -12845,7 +12986,7 @@
       <c r="E24" s="512"/>
       <c r="F24" s="513"/>
       <c r="G24" s="476" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
       <c r="H24" s="456"/>
       <c r="I24" s="456"/>
@@ -12886,11 +13027,11 @@
     </row>
     <row r="27" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="194" t="s">
-        <v>385</v>
+        <v>404</v>
       </c>
       <c r="B27" s="195"/>
       <c r="C27" s="510" t="s">
-        <v>386</v>
+        <v>405</v>
       </c>
       <c r="D27" s="510"/>
       <c r="E27" s="510"/>
@@ -12911,7 +13052,7 @@
       <c r="E28" s="512"/>
       <c r="F28" s="513"/>
       <c r="G28" s="476" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
       <c r="H28" s="456"/>
       <c r="I28" s="456"/>
@@ -12952,11 +13093,11 @@
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="194" t="s">
-        <v>387</v>
+        <v>406</v>
       </c>
       <c r="B31" s="195"/>
       <c r="C31" s="510" t="s">
-        <v>388</v>
+        <v>407</v>
       </c>
       <c r="D31" s="510"/>
       <c r="E31" s="510"/>
@@ -12977,7 +13118,7 @@
       <c r="E32" s="512"/>
       <c r="F32" s="513"/>
       <c r="G32" s="523" t="s">
-        <v>389</v>
+        <v>408</v>
       </c>
       <c r="H32" s="524"/>
       <c r="I32" s="524"/>
@@ -13005,7 +13146,7 @@
       <c r="A34" s="474"/>
       <c r="B34" s="475"/>
       <c r="C34" s="512" t="s">
-        <v>390</v>
+        <v>409</v>
       </c>
       <c r="D34" s="512"/>
       <c r="E34" s="512"/>
@@ -13026,7 +13167,7 @@
       <c r="E35" s="512"/>
       <c r="F35" s="513"/>
       <c r="G35" s="523" t="s">
-        <v>389</v>
+        <v>408</v>
       </c>
       <c r="H35" s="524"/>
       <c r="I35" s="524"/>
@@ -13052,11 +13193,11 @@
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="194" t="s">
-        <v>391</v>
+        <v>410</v>
       </c>
       <c r="B37" s="195"/>
       <c r="C37" s="533" t="s">
-        <v>392</v>
+        <v>411</v>
       </c>
       <c r="D37" s="533"/>
       <c r="E37" s="533"/>
@@ -13077,7 +13218,7 @@
       <c r="E38" s="471"/>
       <c r="F38" s="535"/>
       <c r="G38" s="476" t="s">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="H38" s="456"/>
       <c r="I38" s="456"/>
@@ -13118,11 +13259,11 @@
     </row>
     <row r="41" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="539" t="s">
-        <v>394</v>
+        <v>413</v>
       </c>
       <c r="B41" s="540"/>
       <c r="C41" s="512" t="s">
-        <v>395</v>
+        <v>414</v>
       </c>
       <c r="D41" s="512"/>
       <c r="E41" s="512"/>
@@ -13153,11 +13294,11 @@
     </row>
     <row r="43" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="544" t="s">
-        <v>396</v>
+        <v>415</v>
       </c>
       <c r="B43" s="545"/>
       <c r="C43" s="512" t="s">
-        <v>397</v>
+        <v>416</v>
       </c>
       <c r="D43" s="512"/>
       <c r="E43" s="512"/>
@@ -13179,7 +13320,7 @@
       <c r="E44" s="512"/>
       <c r="F44" s="513"/>
       <c r="G44" s="548" t="s">
-        <v>398</v>
+        <v>417</v>
       </c>
       <c r="H44" s="549"/>
       <c r="I44" s="528"/>
@@ -13191,11 +13332,11 @@
     </row>
     <row r="45" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="544" t="s">
-        <v>399</v>
+        <v>418</v>
       </c>
       <c r="B45" s="545"/>
       <c r="C45" s="513" t="s">
-        <v>400</v>
+        <v>419</v>
       </c>
       <c r="D45" s="513"/>
       <c r="E45" s="513"/>
@@ -13217,7 +13358,7 @@
       <c r="E46" s="513"/>
       <c r="F46" s="513"/>
       <c r="G46" s="551" t="s">
-        <v>401</v>
+        <v>420</v>
       </c>
       <c r="H46" s="552"/>
       <c r="I46" s="528"/>
@@ -13229,11 +13370,11 @@
     </row>
     <row r="47" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="544" t="s">
-        <v>402</v>
+        <v>421</v>
       </c>
       <c r="B47" s="545"/>
       <c r="C47" s="512" t="s">
-        <v>403</v>
+        <v>422</v>
       </c>
       <c r="D47" s="512"/>
       <c r="E47" s="553"/>
@@ -13255,7 +13396,7 @@
       <c r="E48" s="556"/>
       <c r="F48" s="557"/>
       <c r="G48" s="558" t="s">
-        <v>401</v>
+        <v>420</v>
       </c>
       <c r="H48" s="559"/>
       <c r="I48" s="560"/>
@@ -13283,11 +13424,11 @@
     </row>
     <row r="50" ht="23.25" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="568" t="s">
-        <v>404</v>
+        <v>423</v>
       </c>
       <c r="B50" s="569"/>
       <c r="C50" s="570" t="s">
-        <v>405</v>
+        <v>424</v>
       </c>
       <c r="D50" s="570"/>
       <c r="E50" s="570"/>
@@ -13303,17 +13444,17 @@
     </row>
     <row r="51" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="575" t="s">
-        <v>406</v>
+        <v>425</v>
       </c>
       <c r="B51" s="576"/>
       <c r="C51" s="576"/>
       <c r="D51" s="576"/>
       <c r="E51" s="577"/>
       <c r="F51" s="294" t="s">
-        <v>407</v>
+        <v>426</v>
       </c>
       <c r="G51" s="578" t="s">
-        <v>408</v>
+        <v>427</v>
       </c>
       <c r="H51" s="424"/>
       <c r="I51" s="427"/>
@@ -13369,11 +13510,11 @@
     </row>
     <row r="55" ht="39.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="440" t="s">
-        <v>409</v>
+        <v>428</v>
       </c>
       <c r="B55" s="441"/>
       <c r="C55" s="599" t="s">
-        <v>410</v>
+        <v>429</v>
       </c>
       <c r="D55" s="599"/>
       <c r="E55" s="599"/>
@@ -13398,7 +13539,7 @@
       <c r="I56" s="604"/>
       <c r="J56" s="605"/>
       <c r="K56" s="606" t="s">
-        <v>411</v>
+        <v>430</v>
       </c>
       <c r="L56" s="606"/>
       <c r="M56" s="607"/>
@@ -13451,7 +13592,7 @@
     <row r="60" ht="25.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="618"/>
       <c r="B60" s="619" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
       <c r="C60" s="620"/>
       <c r="D60" s="621"/>
@@ -13468,7 +13609,7 @@
     <row r="61" ht="20.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="618"/>
       <c r="B61" s="626" t="s">
-        <v>413</v>
+        <v>432</v>
       </c>
       <c r="C61" s="627"/>
       <c r="D61" s="628"/>
@@ -13485,7 +13626,7 @@
     <row r="62" ht="9" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="618"/>
       <c r="B62" s="632" t="s">
-        <v>414</v>
+        <v>433</v>
       </c>
       <c r="C62" s="633"/>
       <c r="D62" s="634"/>
@@ -13506,7 +13647,7 @@
       <c r="D63" s="640"/>
       <c r="E63" s="282"/>
       <c r="F63" s="641" t="s">
-        <v>415</v>
+        <v>434</v>
       </c>
       <c r="G63" s="642"/>
       <c r="H63" s="642"/>
@@ -13519,7 +13660,7 @@
     <row r="64" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="618"/>
       <c r="B64" s="632" t="s">
-        <v>416</v>
+        <v>435</v>
       </c>
       <c r="C64" s="633"/>
       <c r="D64" s="634"/>
@@ -13540,14 +13681,14 @@
       <c r="D65" s="650"/>
       <c r="E65" s="282"/>
       <c r="F65" s="651" t="s">
-        <v>417</v>
+        <v>436</v>
       </c>
       <c r="G65" s="652"/>
       <c r="H65" s="652"/>
       <c r="I65" s="653"/>
       <c r="J65" s="645"/>
       <c r="K65" s="654" t="s">
-        <v>418</v>
+        <v>437</v>
       </c>
       <c r="L65" s="655"/>
       <c r="M65" s="625"/>
@@ -13569,7 +13710,7 @@
     </row>
     <row r="67" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="660" t="s">
-        <v>419</v>
+        <v>438</v>
       </c>
       <c r="B67" s="661"/>
       <c r="C67" s="661"/>
@@ -13605,7 +13746,7 @@
       <c r="C69" s="580"/>
       <c r="D69" s="580"/>
       <c r="E69" s="668" t="s">
-        <v>420</v>
+        <v>439</v>
       </c>
       <c r="F69" s="669"/>
       <c r="G69" s="669"/>
@@ -13633,7 +13774,7 @@
     </row>
     <row r="71" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="677" t="s">
-        <v>421</v>
+        <v>440</v>
       </c>
       <c r="B71" s="677"/>
       <c r="C71" s="677"/>
@@ -13760,35 +13901,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="678" t="s">
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="B1" s="678" t="s">
-        <v>423</v>
+        <v>442</v>
       </c>
       <c r="C1" s="678" t="s">
-        <v>424</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>425</v>
+        <v>444</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>445</v>
       </c>
       <c r="C2" t="s">
-        <v>427</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>428</v>
+        <v>447</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>429</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -13798,7 +13939,7 @@
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>430</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish pds page 3
</commit_message>
<xml_diff>
--- a/backend/temp/updated_filled_pds.xlsx
+++ b/backend/temp/updated_filled_pds.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="459">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -2700,7 +2700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="669">
+  <cellXfs count="668">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4019,15 +4019,11 @@
     <xf numFmtId="49" fontId="17" fillId="3" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="27" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -12509,95 +12505,107 @@
       <c r="K41" s="417"/>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="418"/>
+      <c r="A42" s="418" t="s">
+        <v>358</v>
+      </c>
       <c r="B42" s="419"/>
-      <c r="C42" s="420"/>
-      <c r="D42" s="421"/>
-      <c r="E42" s="421"/>
-      <c r="F42" s="421"/>
-      <c r="G42" s="421"/>
+      <c r="C42" s="385" t="s">
+        <v>358</v>
+      </c>
+      <c r="D42" s="420"/>
+      <c r="E42" s="420"/>
+      <c r="F42" s="420"/>
+      <c r="G42" s="420"/>
       <c r="H42" s="419"/>
-      <c r="I42" s="420"/>
-      <c r="J42" s="421"/>
-      <c r="K42" s="422"/>
+      <c r="I42" s="385" t="s">
+        <v>358</v>
+      </c>
+      <c r="J42" s="420"/>
+      <c r="K42" s="421"/>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="418"/>
+      <c r="A43" s="418" t="s">
+        <v>358</v>
+      </c>
       <c r="B43" s="419"/>
-      <c r="C43" s="420"/>
-      <c r="D43" s="421"/>
-      <c r="E43" s="421"/>
-      <c r="F43" s="421"/>
-      <c r="G43" s="421"/>
+      <c r="C43" s="385" t="s">
+        <v>358</v>
+      </c>
+      <c r="D43" s="420"/>
+      <c r="E43" s="420"/>
+      <c r="F43" s="420"/>
+      <c r="G43" s="420"/>
       <c r="H43" s="419"/>
-      <c r="I43" s="420"/>
-      <c r="J43" s="421"/>
-      <c r="K43" s="422"/>
+      <c r="I43" s="385" t="s">
+        <v>358</v>
+      </c>
+      <c r="J43" s="420"/>
+      <c r="K43" s="421"/>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="418"/>
       <c r="B44" s="419"/>
-      <c r="C44" s="420"/>
-      <c r="D44" s="421"/>
-      <c r="E44" s="421"/>
-      <c r="F44" s="421"/>
-      <c r="G44" s="421"/>
+      <c r="C44" s="385"/>
+      <c r="D44" s="420"/>
+      <c r="E44" s="420"/>
+      <c r="F44" s="420"/>
+      <c r="G44" s="420"/>
       <c r="H44" s="419"/>
-      <c r="I44" s="420"/>
-      <c r="J44" s="421"/>
-      <c r="K44" s="422"/>
+      <c r="I44" s="385"/>
+      <c r="J44" s="420"/>
+      <c r="K44" s="421"/>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="418"/>
       <c r="B45" s="419"/>
-      <c r="C45" s="420"/>
-      <c r="D45" s="421"/>
-      <c r="E45" s="421"/>
-      <c r="F45" s="421"/>
-      <c r="G45" s="421"/>
+      <c r="C45" s="385"/>
+      <c r="D45" s="420"/>
+      <c r="E45" s="420"/>
+      <c r="F45" s="420"/>
+      <c r="G45" s="420"/>
       <c r="H45" s="419"/>
-      <c r="I45" s="420"/>
-      <c r="J45" s="421"/>
-      <c r="K45" s="422"/>
+      <c r="I45" s="385"/>
+      <c r="J45" s="420"/>
+      <c r="K45" s="421"/>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="418"/>
       <c r="B46" s="419"/>
-      <c r="C46" s="420"/>
-      <c r="D46" s="421"/>
-      <c r="E46" s="421"/>
-      <c r="F46" s="421"/>
-      <c r="G46" s="421"/>
+      <c r="C46" s="385"/>
+      <c r="D46" s="420"/>
+      <c r="E46" s="420"/>
+      <c r="F46" s="420"/>
+      <c r="G46" s="420"/>
       <c r="H46" s="419"/>
-      <c r="I46" s="420"/>
-      <c r="J46" s="421"/>
-      <c r="K46" s="422"/>
+      <c r="I46" s="385"/>
+      <c r="J46" s="420"/>
+      <c r="K46" s="421"/>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="418"/>
       <c r="B47" s="419"/>
-      <c r="C47" s="420"/>
-      <c r="D47" s="421"/>
-      <c r="E47" s="421"/>
-      <c r="F47" s="421"/>
-      <c r="G47" s="421"/>
+      <c r="C47" s="385"/>
+      <c r="D47" s="420"/>
+      <c r="E47" s="420"/>
+      <c r="F47" s="420"/>
+      <c r="G47" s="420"/>
       <c r="H47" s="419"/>
-      <c r="I47" s="420"/>
-      <c r="J47" s="421"/>
-      <c r="K47" s="422"/>
+      <c r="I47" s="385"/>
+      <c r="J47" s="420"/>
+      <c r="K47" s="421"/>
     </row>
     <row r="48" ht="25.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="418"/>
       <c r="B48" s="419"/>
-      <c r="C48" s="420"/>
-      <c r="D48" s="421"/>
-      <c r="E48" s="421"/>
-      <c r="F48" s="421"/>
-      <c r="G48" s="421"/>
+      <c r="C48" s="385"/>
+      <c r="D48" s="420"/>
+      <c r="E48" s="420"/>
+      <c r="F48" s="420"/>
+      <c r="G48" s="420"/>
       <c r="H48" s="419"/>
-      <c r="I48" s="420"/>
-      <c r="J48" s="421"/>
-      <c r="K48" s="422"/>
+      <c r="I48" s="385"/>
+      <c r="J48" s="420"/>
+      <c r="K48" s="421"/>
     </row>
     <row r="49" ht="11.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="265" t="s">
@@ -12623,20 +12631,20 @@
       <c r="D50" s="353"/>
       <c r="E50" s="353"/>
       <c r="F50" s="354"/>
-      <c r="G50" s="423" t="s">
+      <c r="G50" s="422" t="s">
         <v>190</v>
       </c>
-      <c r="H50" s="424"/>
+      <c r="H50" s="423"/>
       <c r="I50" s="352" t="s">
         <v>182</v>
       </c>
       <c r="J50" s="353"/>
       <c r="K50" s="354"/>
-      <c r="L50" s="425"/>
-      <c r="M50" s="425"/>
+      <c r="L50" s="424"/>
+      <c r="M50" s="424"/>
     </row>
     <row r="51" ht="9.75" customHeight="1" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K51" s="426" t="s">
+      <c r="K51" s="425" t="s">
         <v>397</v>
       </c>
     </row>
@@ -12763,65 +12771,65 @@
   </cols>
   <sheetData>
     <row r="1" ht="3" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="427"/>
-      <c r="B1" s="428"/>
-      <c r="C1" s="428"/>
-      <c r="D1" s="428"/>
-      <c r="E1" s="428"/>
-      <c r="F1" s="428"/>
-      <c r="G1" s="428"/>
-      <c r="H1" s="428"/>
-      <c r="I1" s="428"/>
-      <c r="J1" s="428"/>
-      <c r="K1" s="428"/>
-      <c r="L1" s="428"/>
-      <c r="M1" s="429"/>
+      <c r="A1" s="426"/>
+      <c r="B1" s="427"/>
+      <c r="C1" s="427"/>
+      <c r="D1" s="427"/>
+      <c r="E1" s="427"/>
+      <c r="F1" s="427"/>
+      <c r="G1" s="427"/>
+      <c r="H1" s="427"/>
+      <c r="I1" s="427"/>
+      <c r="J1" s="427"/>
+      <c r="K1" s="427"/>
+      <c r="L1" s="427"/>
+      <c r="M1" s="428"/>
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="430" t="s">
+      <c r="A2" s="429" t="s">
         <v>398</v>
       </c>
-      <c r="B2" s="431"/>
-      <c r="C2" s="432" t="s">
+      <c r="B2" s="430"/>
+      <c r="C2" s="431" t="s">
         <v>399</v>
       </c>
-      <c r="D2" s="432"/>
-      <c r="E2" s="432"/>
-      <c r="F2" s="433"/>
-      <c r="G2" s="434"/>
-      <c r="H2" s="434"/>
-      <c r="I2" s="435"/>
-      <c r="J2" s="435"/>
-      <c r="K2" s="436"/>
-      <c r="L2" s="436"/>
-      <c r="M2" s="437"/>
+      <c r="D2" s="431"/>
+      <c r="E2" s="431"/>
+      <c r="F2" s="432"/>
+      <c r="G2" s="433"/>
+      <c r="H2" s="433"/>
+      <c r="I2" s="434"/>
+      <c r="J2" s="434"/>
+      <c r="K2" s="435"/>
+      <c r="L2" s="435"/>
+      <c r="M2" s="436"/>
     </row>
     <row r="3" ht="12.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="438"/>
-      <c r="B3" s="439"/>
-      <c r="C3" s="440" t="s">
+      <c r="A3" s="437"/>
+      <c r="B3" s="438"/>
+      <c r="C3" s="439" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="440"/>
-      <c r="E3" s="440"/>
-      <c r="F3" s="441"/>
-      <c r="G3" s="442"/>
-      <c r="H3" s="442"/>
-      <c r="I3" s="443"/>
-      <c r="J3" s="443"/>
-      <c r="K3" s="444"/>
-      <c r="L3" s="444"/>
-      <c r="M3" s="445"/>
+      <c r="D3" s="439"/>
+      <c r="E3" s="439"/>
+      <c r="F3" s="440"/>
+      <c r="G3" s="441"/>
+      <c r="H3" s="441"/>
+      <c r="I3" s="442"/>
+      <c r="J3" s="442"/>
+      <c r="K3" s="443"/>
+      <c r="L3" s="443"/>
+      <c r="M3" s="444"/>
     </row>
     <row r="4" ht="12" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="438"/>
-      <c r="B4" s="439"/>
-      <c r="C4" s="440" t="s">
+      <c r="A4" s="437"/>
+      <c r="B4" s="438"/>
+      <c r="C4" s="439" t="s">
         <v>401</v>
       </c>
-      <c r="D4" s="440"/>
-      <c r="E4" s="440"/>
-      <c r="F4" s="441"/>
+      <c r="D4" s="439"/>
+      <c r="E4" s="439"/>
+      <c r="F4" s="440"/>
       <c r="G4" s="282"/>
       <c r="H4" s="282"/>
       <c r="I4" s="282"/>
@@ -12831,641 +12839,641 @@
       <c r="M4" s="378"/>
     </row>
     <row r="5" ht="3" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="438"/>
-      <c r="B5" s="439"/>
-      <c r="C5" s="440"/>
-      <c r="D5" s="440"/>
-      <c r="E5" s="440"/>
-      <c r="F5" s="441"/>
-      <c r="G5" s="446"/>
-      <c r="H5" s="446"/>
-      <c r="I5" s="446"/>
-      <c r="J5" s="446"/>
-      <c r="K5" s="446"/>
-      <c r="L5" s="446"/>
+      <c r="A5" s="437"/>
+      <c r="B5" s="438"/>
+      <c r="C5" s="439"/>
+      <c r="D5" s="439"/>
+      <c r="E5" s="439"/>
+      <c r="F5" s="440"/>
+      <c r="G5" s="445"/>
+      <c r="H5" s="445"/>
+      <c r="I5" s="445"/>
+      <c r="J5" s="445"/>
+      <c r="K5" s="445"/>
+      <c r="L5" s="445"/>
       <c r="M5" s="378"/>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="438"/>
-      <c r="B6" s="439"/>
-      <c r="C6" s="440" t="s">
+      <c r="A6" s="437"/>
+      <c r="B6" s="438"/>
+      <c r="C6" s="439" t="s">
         <v>402</v>
       </c>
-      <c r="D6" s="440"/>
-      <c r="E6" s="440"/>
-      <c r="F6" s="441"/>
+      <c r="D6" s="439"/>
+      <c r="E6" s="439"/>
+      <c r="F6" s="440"/>
       <c r="G6" s="282"/>
       <c r="H6" s="282"/>
-      <c r="I6" s="447"/>
-      <c r="J6" s="447"/>
-      <c r="K6" s="447"/>
-      <c r="L6" s="447"/>
+      <c r="I6" s="446"/>
+      <c r="J6" s="446"/>
+      <c r="K6" s="446"/>
+      <c r="L6" s="446"/>
       <c r="M6" s="378"/>
     </row>
     <row r="7" ht="3" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="438"/>
-      <c r="B7" s="439"/>
-      <c r="C7" s="440"/>
-      <c r="D7" s="440"/>
-      <c r="E7" s="440"/>
-      <c r="F7" s="441"/>
+      <c r="A7" s="437"/>
+      <c r="B7" s="438"/>
+      <c r="C7" s="439"/>
+      <c r="D7" s="439"/>
+      <c r="E7" s="439"/>
+      <c r="F7" s="440"/>
       <c r="G7" s="282"/>
       <c r="H7" s="282"/>
-      <c r="I7" s="447"/>
-      <c r="J7" s="447"/>
-      <c r="K7" s="447"/>
-      <c r="L7" s="447"/>
+      <c r="I7" s="446"/>
+      <c r="J7" s="446"/>
+      <c r="K7" s="446"/>
+      <c r="L7" s="446"/>
       <c r="M7" s="378"/>
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="438"/>
-      <c r="B8" s="439"/>
-      <c r="C8" s="440" t="s">
+      <c r="A8" s="437"/>
+      <c r="B8" s="438"/>
+      <c r="C8" s="439" t="s">
         <v>403</v>
       </c>
-      <c r="D8" s="440"/>
-      <c r="E8" s="440"/>
-      <c r="F8" s="441"/>
+      <c r="D8" s="439"/>
+      <c r="E8" s="439"/>
+      <c r="F8" s="440"/>
       <c r="G8" s="282"/>
       <c r="H8" s="282"/>
       <c r="I8" s="282"/>
       <c r="J8" s="282"/>
       <c r="K8" s="282"/>
       <c r="L8" s="282"/>
-      <c r="M8" s="448"/>
+      <c r="M8" s="447"/>
     </row>
     <row r="9" ht="3.75" customHeight="1" hidden="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="438"/>
-      <c r="B9" s="439"/>
-      <c r="C9" s="440"/>
-      <c r="D9" s="440"/>
-      <c r="E9" s="440"/>
-      <c r="F9" s="441"/>
+      <c r="A9" s="437"/>
+      <c r="B9" s="438"/>
+      <c r="C9" s="439"/>
+      <c r="D9" s="439"/>
+      <c r="E9" s="439"/>
+      <c r="F9" s="440"/>
       <c r="G9" s="282"/>
       <c r="H9" s="282"/>
       <c r="I9" s="282"/>
       <c r="J9" s="282"/>
       <c r="K9" s="282"/>
       <c r="L9" s="282"/>
-      <c r="M9" s="448"/>
+      <c r="M9" s="447"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="438"/>
-      <c r="B10" s="439"/>
-      <c r="C10" s="440"/>
-      <c r="D10" s="440"/>
-      <c r="E10" s="440"/>
-      <c r="F10" s="441"/>
-      <c r="G10" s="446" t="s">
+      <c r="A10" s="437"/>
+      <c r="B10" s="438"/>
+      <c r="C10" s="439"/>
+      <c r="D10" s="439"/>
+      <c r="E10" s="439"/>
+      <c r="F10" s="440"/>
+      <c r="G10" s="445" t="s">
         <v>404</v>
       </c>
-      <c r="H10" s="446"/>
-      <c r="I10" s="446"/>
-      <c r="J10" s="446"/>
-      <c r="K10" s="446"/>
-      <c r="L10" s="446"/>
-      <c r="M10" s="449"/>
+      <c r="H10" s="445"/>
+      <c r="I10" s="445"/>
+      <c r="J10" s="445"/>
+      <c r="K10" s="445"/>
+      <c r="L10" s="445"/>
+      <c r="M10" s="448"/>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="438"/>
-      <c r="B11" s="439"/>
-      <c r="C11" s="440"/>
-      <c r="D11" s="440"/>
-      <c r="E11" s="440"/>
-      <c r="F11" s="441"/>
-      <c r="G11" s="450"/>
-      <c r="H11" s="451"/>
-      <c r="I11" s="452"/>
-      <c r="J11" s="452"/>
-      <c r="K11" s="452"/>
-      <c r="L11" s="452"/>
-      <c r="M11" s="449"/>
+      <c r="A11" s="437"/>
+      <c r="B11" s="438"/>
+      <c r="C11" s="439"/>
+      <c r="D11" s="439"/>
+      <c r="E11" s="439"/>
+      <c r="F11" s="440"/>
+      <c r="G11" s="449"/>
+      <c r="H11" s="450"/>
+      <c r="I11" s="451"/>
+      <c r="J11" s="451"/>
+      <c r="K11" s="451"/>
+      <c r="L11" s="451"/>
+      <c r="M11" s="448"/>
     </row>
     <row r="12" ht="5.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="453"/>
-      <c r="B12" s="454"/>
-      <c r="C12" s="455"/>
-      <c r="D12" s="455"/>
-      <c r="E12" s="455"/>
-      <c r="F12" s="456"/>
-      <c r="G12" s="451"/>
-      <c r="H12" s="451"/>
-      <c r="I12" s="457"/>
-      <c r="J12" s="457"/>
-      <c r="K12" s="457"/>
-      <c r="L12" s="457"/>
-      <c r="M12" s="458"/>
+      <c r="A12" s="452"/>
+      <c r="B12" s="453"/>
+      <c r="C12" s="454"/>
+      <c r="D12" s="454"/>
+      <c r="E12" s="454"/>
+      <c r="F12" s="455"/>
+      <c r="G12" s="450"/>
+      <c r="H12" s="450"/>
+      <c r="I12" s="456"/>
+      <c r="J12" s="456"/>
+      <c r="K12" s="456"/>
+      <c r="L12" s="456"/>
+      <c r="M12" s="457"/>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="459" t="s">
+      <c r="A13" s="458" t="s">
         <v>405</v>
       </c>
-      <c r="B13" s="460"/>
-      <c r="C13" s="461" t="s">
+      <c r="B13" s="459"/>
+      <c r="C13" s="460" t="s">
         <v>406</v>
       </c>
-      <c r="D13" s="461"/>
+      <c r="D13" s="460"/>
       <c r="E13" s="282"/>
       <c r="F13" s="398"/>
-      <c r="G13" s="462"/>
-      <c r="H13" s="462"/>
-      <c r="I13" s="462"/>
-      <c r="J13" s="462"/>
-      <c r="K13" s="462"/>
-      <c r="L13" s="462"/>
-      <c r="M13" s="463"/>
+      <c r="G13" s="461"/>
+      <c r="H13" s="461"/>
+      <c r="I13" s="461"/>
+      <c r="J13" s="461"/>
+      <c r="K13" s="461"/>
+      <c r="L13" s="461"/>
+      <c r="M13" s="462"/>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="464"/>
-      <c r="B14" s="465"/>
-      <c r="C14" s="461"/>
-      <c r="D14" s="461"/>
+      <c r="A14" s="463"/>
+      <c r="B14" s="464"/>
+      <c r="C14" s="460"/>
+      <c r="D14" s="460"/>
       <c r="E14" s="282"/>
       <c r="F14" s="398"/>
-      <c r="G14" s="466" t="s">
+      <c r="G14" s="465" t="s">
         <v>404</v>
       </c>
-      <c r="H14" s="446"/>
-      <c r="I14" s="446"/>
-      <c r="J14" s="446"/>
-      <c r="K14" s="446"/>
-      <c r="L14" s="446"/>
-      <c r="M14" s="467"/>
+      <c r="H14" s="445"/>
+      <c r="I14" s="445"/>
+      <c r="J14" s="445"/>
+      <c r="K14" s="445"/>
+      <c r="L14" s="445"/>
+      <c r="M14" s="466"/>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="464"/>
-      <c r="B15" s="465"/>
-      <c r="C15" s="461"/>
-      <c r="D15" s="461"/>
+      <c r="A15" s="463"/>
+      <c r="B15" s="464"/>
+      <c r="C15" s="460"/>
+      <c r="D15" s="460"/>
       <c r="E15" s="282"/>
       <c r="F15" s="398"/>
-      <c r="G15" s="442"/>
-      <c r="H15" s="468"/>
-      <c r="I15" s="469"/>
-      <c r="J15" s="469"/>
-      <c r="K15" s="469"/>
-      <c r="L15" s="469"/>
-      <c r="M15" s="467"/>
+      <c r="G15" s="441"/>
+      <c r="H15" s="467"/>
+      <c r="I15" s="468"/>
+      <c r="J15" s="468"/>
+      <c r="K15" s="468"/>
+      <c r="L15" s="468"/>
+      <c r="M15" s="466"/>
     </row>
     <row r="16" ht="5.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="464"/>
-      <c r="B16" s="465"/>
+      <c r="A16" s="463"/>
+      <c r="B16" s="464"/>
       <c r="C16" s="282"/>
       <c r="D16" s="282"/>
       <c r="E16" s="282"/>
       <c r="F16" s="398"/>
-      <c r="G16" s="470"/>
-      <c r="H16" s="471"/>
-      <c r="I16" s="472"/>
-      <c r="J16" s="472"/>
-      <c r="K16" s="472"/>
-      <c r="L16" s="472"/>
-      <c r="M16" s="473"/>
+      <c r="G16" s="469"/>
+      <c r="H16" s="470"/>
+      <c r="I16" s="471"/>
+      <c r="J16" s="471"/>
+      <c r="K16" s="471"/>
+      <c r="L16" s="471"/>
+      <c r="M16" s="472"/>
     </row>
     <row r="17" ht="6.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="474"/>
-      <c r="B17" s="475"/>
-      <c r="C17" s="476"/>
-      <c r="D17" s="476"/>
-      <c r="E17" s="477"/>
-      <c r="F17" s="478"/>
-      <c r="G17" s="479"/>
-      <c r="H17" s="480"/>
-      <c r="I17" s="480"/>
-      <c r="J17" s="480"/>
-      <c r="K17" s="480"/>
-      <c r="L17" s="480"/>
-      <c r="M17" s="481"/>
+      <c r="A17" s="473"/>
+      <c r="B17" s="474"/>
+      <c r="C17" s="475"/>
+      <c r="D17" s="475"/>
+      <c r="E17" s="476"/>
+      <c r="F17" s="477"/>
+      <c r="G17" s="478"/>
+      <c r="H17" s="479"/>
+      <c r="I17" s="479"/>
+      <c r="J17" s="479"/>
+      <c r="K17" s="479"/>
+      <c r="L17" s="479"/>
+      <c r="M17" s="480"/>
     </row>
     <row r="18" ht="12.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="474"/>
-      <c r="B18" s="475"/>
-      <c r="C18" s="482" t="s">
+      <c r="A18" s="473"/>
+      <c r="B18" s="474"/>
+      <c r="C18" s="481" t="s">
         <v>407</v>
       </c>
-      <c r="D18" s="482"/>
-      <c r="E18" s="483"/>
-      <c r="F18" s="484"/>
-      <c r="G18" s="485"/>
-      <c r="H18" s="485"/>
-      <c r="I18" s="485"/>
-      <c r="J18" s="485"/>
-      <c r="K18" s="485"/>
-      <c r="L18" s="485"/>
-      <c r="M18" s="486"/>
+      <c r="D18" s="481"/>
+      <c r="E18" s="482"/>
+      <c r="F18" s="483"/>
+      <c r="G18" s="484"/>
+      <c r="H18" s="484"/>
+      <c r="I18" s="484"/>
+      <c r="J18" s="484"/>
+      <c r="K18" s="484"/>
+      <c r="L18" s="484"/>
+      <c r="M18" s="485"/>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="474"/>
-      <c r="B19" s="475"/>
-      <c r="C19" s="482"/>
-      <c r="D19" s="482"/>
-      <c r="E19" s="483"/>
-      <c r="F19" s="484"/>
-      <c r="G19" s="466" t="s">
+      <c r="A19" s="473"/>
+      <c r="B19" s="474"/>
+      <c r="C19" s="481"/>
+      <c r="D19" s="481"/>
+      <c r="E19" s="482"/>
+      <c r="F19" s="483"/>
+      <c r="G19" s="465" t="s">
         <v>404</v>
       </c>
-      <c r="H19" s="446"/>
-      <c r="I19" s="446"/>
-      <c r="J19" s="446"/>
-      <c r="K19" s="446"/>
-      <c r="L19" s="446"/>
-      <c r="M19" s="486"/>
+      <c r="H19" s="445"/>
+      <c r="I19" s="445"/>
+      <c r="J19" s="445"/>
+      <c r="K19" s="445"/>
+      <c r="L19" s="445"/>
+      <c r="M19" s="485"/>
     </row>
     <row r="20" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="474"/>
-      <c r="B20" s="475"/>
-      <c r="C20" s="482"/>
-      <c r="D20" s="482"/>
-      <c r="E20" s="483"/>
-      <c r="F20" s="484"/>
-      <c r="G20" s="485"/>
-      <c r="H20" s="487" t="s">
+      <c r="A20" s="473"/>
+      <c r="B20" s="474"/>
+      <c r="C20" s="481"/>
+      <c r="D20" s="481"/>
+      <c r="E20" s="482"/>
+      <c r="F20" s="483"/>
+      <c r="G20" s="484"/>
+      <c r="H20" s="486" t="s">
         <v>408</v>
       </c>
-      <c r="I20" s="487"/>
-      <c r="J20" s="488"/>
-      <c r="K20" s="489"/>
-      <c r="L20" s="490"/>
-      <c r="M20" s="486"/>
+      <c r="I20" s="486"/>
+      <c r="J20" s="487"/>
+      <c r="K20" s="488"/>
+      <c r="L20" s="489"/>
+      <c r="M20" s="485"/>
     </row>
     <row r="21" ht="14.25" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="474"/>
-      <c r="B21" s="475"/>
-      <c r="C21" s="482"/>
-      <c r="D21" s="482"/>
-      <c r="E21" s="483"/>
-      <c r="F21" s="484"/>
-      <c r="G21" s="491" t="s">
+      <c r="A21" s="473"/>
+      <c r="B21" s="474"/>
+      <c r="C21" s="481"/>
+      <c r="D21" s="481"/>
+      <c r="E21" s="482"/>
+      <c r="F21" s="483"/>
+      <c r="G21" s="490" t="s">
         <v>409</v>
       </c>
-      <c r="H21" s="492"/>
-      <c r="I21" s="492"/>
-      <c r="J21" s="488"/>
-      <c r="K21" s="493"/>
-      <c r="L21" s="490"/>
-      <c r="M21" s="486"/>
+      <c r="H21" s="491"/>
+      <c r="I21" s="491"/>
+      <c r="J21" s="487"/>
+      <c r="K21" s="492"/>
+      <c r="L21" s="489"/>
+      <c r="M21" s="485"/>
     </row>
     <row r="22" ht="5.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="494"/>
-      <c r="B22" s="495"/>
-      <c r="C22" s="496"/>
-      <c r="D22" s="496"/>
-      <c r="E22" s="496"/>
-      <c r="F22" s="497"/>
-      <c r="G22" s="470" t="s">
+      <c r="A22" s="493"/>
+      <c r="B22" s="494"/>
+      <c r="C22" s="495"/>
+      <c r="D22" s="495"/>
+      <c r="E22" s="495"/>
+      <c r="F22" s="496"/>
+      <c r="G22" s="469" t="s">
         <v>410</v>
       </c>
-      <c r="H22" s="471"/>
-      <c r="I22" s="498"/>
-      <c r="J22" s="498"/>
-      <c r="K22" s="498"/>
-      <c r="L22" s="499"/>
-      <c r="M22" s="473"/>
+      <c r="H22" s="470"/>
+      <c r="I22" s="497"/>
+      <c r="J22" s="497"/>
+      <c r="K22" s="497"/>
+      <c r="L22" s="498"/>
+      <c r="M22" s="472"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="194" t="s">
         <v>411</v>
       </c>
       <c r="B23" s="195"/>
-      <c r="C23" s="500" t="s">
+      <c r="C23" s="499" t="s">
         <v>412</v>
       </c>
-      <c r="D23" s="500"/>
-      <c r="E23" s="500"/>
-      <c r="F23" s="501"/>
-      <c r="G23" s="462"/>
-      <c r="H23" s="462"/>
-      <c r="I23" s="462"/>
-      <c r="J23" s="462"/>
-      <c r="K23" s="462"/>
-      <c r="L23" s="462"/>
-      <c r="M23" s="463"/>
+      <c r="D23" s="499"/>
+      <c r="E23" s="499"/>
+      <c r="F23" s="500"/>
+      <c r="G23" s="461"/>
+      <c r="H23" s="461"/>
+      <c r="I23" s="461"/>
+      <c r="J23" s="461"/>
+      <c r="K23" s="461"/>
+      <c r="L23" s="461"/>
+      <c r="M23" s="462"/>
     </row>
     <row r="24" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="464"/>
-      <c r="B24" s="465"/>
-      <c r="C24" s="502"/>
-      <c r="D24" s="502"/>
-      <c r="E24" s="502"/>
-      <c r="F24" s="503"/>
-      <c r="G24" s="466" t="s">
+      <c r="A24" s="463"/>
+      <c r="B24" s="464"/>
+      <c r="C24" s="501"/>
+      <c r="D24" s="501"/>
+      <c r="E24" s="501"/>
+      <c r="F24" s="502"/>
+      <c r="G24" s="465" t="s">
         <v>404</v>
       </c>
-      <c r="H24" s="446"/>
-      <c r="I24" s="446"/>
-      <c r="J24" s="446"/>
-      <c r="K24" s="446"/>
-      <c r="L24" s="446"/>
-      <c r="M24" s="504"/>
+      <c r="H24" s="445"/>
+      <c r="I24" s="445"/>
+      <c r="J24" s="445"/>
+      <c r="K24" s="445"/>
+      <c r="L24" s="445"/>
+      <c r="M24" s="503"/>
     </row>
     <row r="25" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="464"/>
-      <c r="B25" s="465"/>
-      <c r="C25" s="502"/>
-      <c r="D25" s="502"/>
-      <c r="E25" s="502"/>
-      <c r="F25" s="503"/>
-      <c r="G25" s="505"/>
-      <c r="H25" s="471"/>
-      <c r="I25" s="506"/>
-      <c r="J25" s="506"/>
-      <c r="K25" s="506"/>
-      <c r="L25" s="506"/>
-      <c r="M25" s="504"/>
+      <c r="A25" s="463"/>
+      <c r="B25" s="464"/>
+      <c r="C25" s="501"/>
+      <c r="D25" s="501"/>
+      <c r="E25" s="501"/>
+      <c r="F25" s="502"/>
+      <c r="G25" s="504"/>
+      <c r="H25" s="470"/>
+      <c r="I25" s="505"/>
+      <c r="J25" s="505"/>
+      <c r="K25" s="505"/>
+      <c r="L25" s="505"/>
+      <c r="M25" s="503"/>
     </row>
     <row r="26" ht="6" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="507"/>
-      <c r="B26" s="508"/>
-      <c r="C26" s="509"/>
-      <c r="D26" s="509"/>
-      <c r="E26" s="509"/>
-      <c r="F26" s="510"/>
-      <c r="G26" s="470"/>
-      <c r="H26" s="471"/>
-      <c r="I26" s="472"/>
-      <c r="J26" s="472"/>
-      <c r="K26" s="472"/>
-      <c r="L26" s="472"/>
-      <c r="M26" s="473"/>
+      <c r="A26" s="506"/>
+      <c r="B26" s="507"/>
+      <c r="C26" s="508"/>
+      <c r="D26" s="508"/>
+      <c r="E26" s="508"/>
+      <c r="F26" s="509"/>
+      <c r="G26" s="469"/>
+      <c r="H26" s="470"/>
+      <c r="I26" s="471"/>
+      <c r="J26" s="471"/>
+      <c r="K26" s="471"/>
+      <c r="L26" s="471"/>
+      <c r="M26" s="472"/>
     </row>
     <row r="27" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="194" t="s">
         <v>413</v>
       </c>
       <c r="B27" s="195"/>
-      <c r="C27" s="500" t="s">
+      <c r="C27" s="499" t="s">
         <v>414</v>
       </c>
-      <c r="D27" s="500"/>
-      <c r="E27" s="500"/>
-      <c r="F27" s="501"/>
-      <c r="G27" s="462"/>
-      <c r="H27" s="462"/>
-      <c r="I27" s="462"/>
-      <c r="J27" s="462"/>
-      <c r="K27" s="462"/>
-      <c r="L27" s="462"/>
-      <c r="M27" s="463"/>
+      <c r="D27" s="499"/>
+      <c r="E27" s="499"/>
+      <c r="F27" s="500"/>
+      <c r="G27" s="461"/>
+      <c r="H27" s="461"/>
+      <c r="I27" s="461"/>
+      <c r="J27" s="461"/>
+      <c r="K27" s="461"/>
+      <c r="L27" s="461"/>
+      <c r="M27" s="462"/>
     </row>
     <row r="28" ht="12" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="464"/>
-      <c r="B28" s="465"/>
-      <c r="C28" s="502"/>
-      <c r="D28" s="502"/>
-      <c r="E28" s="502"/>
-      <c r="F28" s="503"/>
-      <c r="G28" s="466" t="s">
+      <c r="A28" s="463"/>
+      <c r="B28" s="464"/>
+      <c r="C28" s="501"/>
+      <c r="D28" s="501"/>
+      <c r="E28" s="501"/>
+      <c r="F28" s="502"/>
+      <c r="G28" s="465" t="s">
         <v>404</v>
       </c>
-      <c r="H28" s="446"/>
-      <c r="I28" s="446"/>
-      <c r="J28" s="446"/>
-      <c r="K28" s="446"/>
-      <c r="L28" s="446"/>
+      <c r="H28" s="445"/>
+      <c r="I28" s="445"/>
+      <c r="J28" s="445"/>
+      <c r="K28" s="445"/>
+      <c r="L28" s="445"/>
       <c r="M28" s="378"/>
     </row>
     <row r="29" ht="11.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="464"/>
-      <c r="B29" s="465"/>
-      <c r="C29" s="502"/>
-      <c r="D29" s="502"/>
-      <c r="E29" s="502"/>
-      <c r="F29" s="503"/>
+      <c r="A29" s="463"/>
+      <c r="B29" s="464"/>
+      <c r="C29" s="501"/>
+      <c r="D29" s="501"/>
+      <c r="E29" s="501"/>
+      <c r="F29" s="502"/>
       <c r="G29" s="282"/>
       <c r="H29" s="125"/>
-      <c r="I29" s="506"/>
-      <c r="J29" s="506"/>
-      <c r="K29" s="506"/>
-      <c r="L29" s="506"/>
-      <c r="M29" s="504"/>
+      <c r="I29" s="505"/>
+      <c r="J29" s="505"/>
+      <c r="K29" s="505"/>
+      <c r="L29" s="505"/>
+      <c r="M29" s="503"/>
     </row>
     <row r="30" ht="6" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="507"/>
-      <c r="B30" s="508"/>
-      <c r="C30" s="509"/>
-      <c r="D30" s="509"/>
-      <c r="E30" s="509"/>
-      <c r="F30" s="510"/>
-      <c r="G30" s="511"/>
-      <c r="H30" s="512"/>
+      <c r="A30" s="506"/>
+      <c r="B30" s="507"/>
+      <c r="C30" s="508"/>
+      <c r="D30" s="508"/>
+      <c r="E30" s="508"/>
+      <c r="F30" s="509"/>
+      <c r="G30" s="510"/>
+      <c r="H30" s="511"/>
       <c r="I30" s="125"/>
       <c r="J30" s="125"/>
       <c r="K30" s="125"/>
       <c r="L30" s="125"/>
-      <c r="M30" s="473"/>
+      <c r="M30" s="472"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="194" t="s">
         <v>415</v>
       </c>
       <c r="B31" s="195"/>
-      <c r="C31" s="500" t="s">
+      <c r="C31" s="499" t="s">
         <v>416</v>
       </c>
-      <c r="D31" s="500"/>
-      <c r="E31" s="500"/>
-      <c r="F31" s="501"/>
-      <c r="G31" s="462"/>
-      <c r="H31" s="462"/>
-      <c r="I31" s="462"/>
-      <c r="J31" s="462"/>
-      <c r="K31" s="462"/>
-      <c r="L31" s="462"/>
-      <c r="M31" s="463"/>
+      <c r="D31" s="499"/>
+      <c r="E31" s="499"/>
+      <c r="F31" s="500"/>
+      <c r="G31" s="461"/>
+      <c r="H31" s="461"/>
+      <c r="I31" s="461"/>
+      <c r="J31" s="461"/>
+      <c r="K31" s="461"/>
+      <c r="L31" s="461"/>
+      <c r="M31" s="462"/>
     </row>
     <row r="32" ht="12" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="464"/>
-      <c r="B32" s="465"/>
-      <c r="C32" s="502"/>
-      <c r="D32" s="502"/>
-      <c r="E32" s="502"/>
-      <c r="F32" s="503"/>
-      <c r="G32" s="513" t="s">
+      <c r="A32" s="463"/>
+      <c r="B32" s="464"/>
+      <c r="C32" s="501"/>
+      <c r="D32" s="501"/>
+      <c r="E32" s="501"/>
+      <c r="F32" s="502"/>
+      <c r="G32" s="512" t="s">
         <v>417</v>
       </c>
-      <c r="H32" s="514"/>
-      <c r="I32" s="514"/>
-      <c r="J32" s="514"/>
-      <c r="K32" s="515"/>
-      <c r="L32" s="515"/>
-      <c r="M32" s="504"/>
+      <c r="H32" s="513"/>
+      <c r="I32" s="513"/>
+      <c r="J32" s="513"/>
+      <c r="K32" s="514"/>
+      <c r="L32" s="514"/>
+      <c r="M32" s="503"/>
     </row>
     <row r="33" ht="6.75" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="464"/>
-      <c r="B33" s="465"/>
-      <c r="C33" s="502"/>
-      <c r="D33" s="502"/>
-      <c r="E33" s="502"/>
-      <c r="F33" s="503"/>
-      <c r="G33" s="516"/>
-      <c r="H33" s="517"/>
-      <c r="I33" s="518"/>
-      <c r="J33" s="518"/>
-      <c r="K33" s="519"/>
-      <c r="L33" s="519"/>
-      <c r="M33" s="504"/>
+      <c r="A33" s="463"/>
+      <c r="B33" s="464"/>
+      <c r="C33" s="501"/>
+      <c r="D33" s="501"/>
+      <c r="E33" s="501"/>
+      <c r="F33" s="502"/>
+      <c r="G33" s="515"/>
+      <c r="H33" s="516"/>
+      <c r="I33" s="517"/>
+      <c r="J33" s="517"/>
+      <c r="K33" s="518"/>
+      <c r="L33" s="518"/>
+      <c r="M33" s="503"/>
     </row>
     <row r="34" ht="14.25" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="464"/>
-      <c r="B34" s="465"/>
-      <c r="C34" s="502" t="s">
+      <c r="A34" s="463"/>
+      <c r="B34" s="464"/>
+      <c r="C34" s="501" t="s">
         <v>418</v>
       </c>
-      <c r="D34" s="502"/>
-      <c r="E34" s="502"/>
-      <c r="F34" s="503"/>
-      <c r="G34" s="505"/>
-      <c r="H34" s="520"/>
-      <c r="I34" s="521"/>
-      <c r="J34" s="521"/>
-      <c r="K34" s="521"/>
-      <c r="L34" s="521"/>
-      <c r="M34" s="504"/>
+      <c r="D34" s="501"/>
+      <c r="E34" s="501"/>
+      <c r="F34" s="502"/>
+      <c r="G34" s="504"/>
+      <c r="H34" s="519"/>
+      <c r="I34" s="520"/>
+      <c r="J34" s="520"/>
+      <c r="K34" s="520"/>
+      <c r="L34" s="520"/>
+      <c r="M34" s="503"/>
     </row>
     <row r="35" ht="14.25" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="464"/>
-      <c r="B35" s="465"/>
-      <c r="C35" s="502"/>
-      <c r="D35" s="502"/>
-      <c r="E35" s="502"/>
-      <c r="F35" s="503"/>
-      <c r="G35" s="513" t="s">
+      <c r="A35" s="463"/>
+      <c r="B35" s="464"/>
+      <c r="C35" s="501"/>
+      <c r="D35" s="501"/>
+      <c r="E35" s="501"/>
+      <c r="F35" s="502"/>
+      <c r="G35" s="512" t="s">
         <v>417</v>
       </c>
-      <c r="H35" s="514"/>
-      <c r="I35" s="514"/>
-      <c r="J35" s="514"/>
-      <c r="K35" s="515"/>
-      <c r="L35" s="515"/>
-      <c r="M35" s="504"/>
+      <c r="H35" s="513"/>
+      <c r="I35" s="513"/>
+      <c r="J35" s="513"/>
+      <c r="K35" s="514"/>
+      <c r="L35" s="514"/>
+      <c r="M35" s="503"/>
     </row>
     <row r="36" ht="4.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="507"/>
-      <c r="B36" s="508"/>
-      <c r="C36" s="509"/>
-      <c r="D36" s="509"/>
-      <c r="E36" s="509"/>
-      <c r="F36" s="510"/>
-      <c r="G36" s="516"/>
-      <c r="H36" s="517"/>
-      <c r="I36" s="518"/>
-      <c r="J36" s="518"/>
+      <c r="A36" s="506"/>
+      <c r="B36" s="507"/>
+      <c r="C36" s="508"/>
+      <c r="D36" s="508"/>
+      <c r="E36" s="508"/>
+      <c r="F36" s="509"/>
+      <c r="G36" s="515"/>
+      <c r="H36" s="516"/>
+      <c r="I36" s="517"/>
+      <c r="J36" s="517"/>
       <c r="K36" s="282"/>
-      <c r="L36" s="522"/>
-      <c r="M36" s="473"/>
+      <c r="L36" s="521"/>
+      <c r="M36" s="472"/>
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="194" t="s">
         <v>419</v>
       </c>
       <c r="B37" s="195"/>
-      <c r="C37" s="523" t="s">
+      <c r="C37" s="522" t="s">
         <v>420</v>
       </c>
-      <c r="D37" s="523"/>
-      <c r="E37" s="523"/>
-      <c r="F37" s="524"/>
-      <c r="G37" s="462"/>
-      <c r="H37" s="462"/>
-      <c r="I37" s="462"/>
-      <c r="J37" s="462"/>
-      <c r="K37" s="462"/>
-      <c r="L37" s="462"/>
-      <c r="M37" s="463"/>
+      <c r="D37" s="522"/>
+      <c r="E37" s="522"/>
+      <c r="F37" s="523"/>
+      <c r="G37" s="461"/>
+      <c r="H37" s="461"/>
+      <c r="I37" s="461"/>
+      <c r="J37" s="461"/>
+      <c r="K37" s="461"/>
+      <c r="L37" s="461"/>
+      <c r="M37" s="462"/>
     </row>
     <row r="38" ht="12" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="464"/>
-      <c r="B38" s="465"/>
-      <c r="C38" s="461"/>
-      <c r="D38" s="461"/>
-      <c r="E38" s="461"/>
-      <c r="F38" s="525"/>
-      <c r="G38" s="466" t="s">
+      <c r="A38" s="463"/>
+      <c r="B38" s="464"/>
+      <c r="C38" s="460"/>
+      <c r="D38" s="460"/>
+      <c r="E38" s="460"/>
+      <c r="F38" s="524"/>
+      <c r="G38" s="465" t="s">
         <v>421</v>
       </c>
-      <c r="H38" s="446"/>
-      <c r="I38" s="446"/>
-      <c r="J38" s="446"/>
-      <c r="K38" s="446"/>
-      <c r="L38" s="446"/>
-      <c r="M38" s="526"/>
+      <c r="H38" s="445"/>
+      <c r="I38" s="445"/>
+      <c r="J38" s="445"/>
+      <c r="K38" s="445"/>
+      <c r="L38" s="445"/>
+      <c r="M38" s="525"/>
     </row>
     <row r="39" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="464"/>
-      <c r="B39" s="465"/>
-      <c r="C39" s="461"/>
-      <c r="D39" s="461"/>
-      <c r="E39" s="461"/>
-      <c r="F39" s="525"/>
-      <c r="G39" s="505"/>
-      <c r="H39" s="471"/>
-      <c r="I39" s="506"/>
-      <c r="J39" s="506"/>
-      <c r="K39" s="506"/>
-      <c r="L39" s="506"/>
-      <c r="M39" s="504"/>
+      <c r="A39" s="463"/>
+      <c r="B39" s="464"/>
+      <c r="C39" s="460"/>
+      <c r="D39" s="460"/>
+      <c r="E39" s="460"/>
+      <c r="F39" s="524"/>
+      <c r="G39" s="504"/>
+      <c r="H39" s="470"/>
+      <c r="I39" s="505"/>
+      <c r="J39" s="505"/>
+      <c r="K39" s="505"/>
+      <c r="L39" s="505"/>
+      <c r="M39" s="503"/>
     </row>
     <row r="40" ht="6" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="507"/>
-      <c r="B40" s="508"/>
-      <c r="C40" s="527"/>
-      <c r="D40" s="527"/>
-      <c r="E40" s="527"/>
-      <c r="F40" s="528"/>
-      <c r="G40" s="470"/>
-      <c r="H40" s="471"/>
-      <c r="I40" s="472"/>
-      <c r="J40" s="472"/>
-      <c r="K40" s="472"/>
-      <c r="L40" s="472"/>
-      <c r="M40" s="473"/>
+      <c r="A40" s="506"/>
+      <c r="B40" s="507"/>
+      <c r="C40" s="526"/>
+      <c r="D40" s="526"/>
+      <c r="E40" s="526"/>
+      <c r="F40" s="527"/>
+      <c r="G40" s="469"/>
+      <c r="H40" s="470"/>
+      <c r="I40" s="471"/>
+      <c r="J40" s="471"/>
+      <c r="K40" s="471"/>
+      <c r="L40" s="471"/>
+      <c r="M40" s="472"/>
     </row>
     <row r="41" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="529" t="s">
+      <c r="A41" s="528" t="s">
         <v>422</v>
       </c>
-      <c r="B41" s="530"/>
-      <c r="C41" s="502" t="s">
+      <c r="B41" s="529"/>
+      <c r="C41" s="501" t="s">
         <v>423</v>
       </c>
-      <c r="D41" s="502"/>
-      <c r="E41" s="502"/>
-      <c r="F41" s="503"/>
-      <c r="G41" s="462"/>
-      <c r="H41" s="462"/>
-      <c r="I41" s="531"/>
-      <c r="J41" s="531"/>
-      <c r="K41" s="532"/>
-      <c r="L41" s="532"/>
-      <c r="M41" s="533"/>
+      <c r="D41" s="501"/>
+      <c r="E41" s="501"/>
+      <c r="F41" s="502"/>
+      <c r="G41" s="461"/>
+      <c r="H41" s="461"/>
+      <c r="I41" s="530"/>
+      <c r="J41" s="530"/>
+      <c r="K41" s="531"/>
+      <c r="L41" s="531"/>
+      <c r="M41" s="532"/>
     </row>
     <row r="42" ht="0.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="534"/>
-      <c r="B42" s="535"/>
-      <c r="C42" s="502"/>
-      <c r="D42" s="502"/>
-      <c r="E42" s="502"/>
-      <c r="F42" s="503"/>
-      <c r="G42" s="536"/>
-      <c r="H42" s="536"/>
-      <c r="I42" s="536"/>
-      <c r="J42" s="536"/>
-      <c r="K42" s="536"/>
-      <c r="L42" s="536"/>
-      <c r="M42" s="537"/>
+      <c r="A42" s="533"/>
+      <c r="B42" s="534"/>
+      <c r="C42" s="501"/>
+      <c r="D42" s="501"/>
+      <c r="E42" s="501"/>
+      <c r="F42" s="502"/>
+      <c r="G42" s="535"/>
+      <c r="H42" s="535"/>
+      <c r="I42" s="535"/>
+      <c r="J42" s="535"/>
+      <c r="K42" s="535"/>
+      <c r="L42" s="535"/>
+      <c r="M42" s="536"/>
       <c r="N42" s="282"/>
     </row>
     <row r="43" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="534" t="s">
+      <c r="A43" s="533" t="s">
         <v>424</v>
       </c>
-      <c r="B43" s="535"/>
-      <c r="C43" s="502" t="s">
+      <c r="B43" s="534"/>
+      <c r="C43" s="501" t="s">
         <v>425</v>
       </c>
-      <c r="D43" s="502"/>
-      <c r="E43" s="502"/>
-      <c r="F43" s="503"/>
+      <c r="D43" s="501"/>
+      <c r="E43" s="501"/>
+      <c r="F43" s="502"/>
       <c r="G43" s="282"/>
       <c r="H43" s="282"/>
       <c r="I43" s="282"/>
@@ -13476,34 +13484,34 @@
       <c r="N43" s="282"/>
     </row>
     <row r="44" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="534"/>
-      <c r="B44" s="535"/>
-      <c r="C44" s="502"/>
-      <c r="D44" s="502"/>
-      <c r="E44" s="502"/>
-      <c r="F44" s="503"/>
-      <c r="G44" s="538" t="s">
+      <c r="A44" s="533"/>
+      <c r="B44" s="534"/>
+      <c r="C44" s="501"/>
+      <c r="D44" s="501"/>
+      <c r="E44" s="501"/>
+      <c r="F44" s="502"/>
+      <c r="G44" s="537" t="s">
         <v>426</v>
       </c>
-      <c r="H44" s="539"/>
-      <c r="I44" s="518"/>
-      <c r="J44" s="518"/>
+      <c r="H44" s="538"/>
+      <c r="I44" s="517"/>
+      <c r="J44" s="517"/>
       <c r="K44" s="282"/>
-      <c r="L44" s="522"/>
-      <c r="M44" s="540"/>
-      <c r="N44" s="517"/>
+      <c r="L44" s="521"/>
+      <c r="M44" s="539"/>
+      <c r="N44" s="516"/>
     </row>
     <row r="45" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="534" t="s">
+      <c r="A45" s="533" t="s">
         <v>427</v>
       </c>
-      <c r="B45" s="535"/>
-      <c r="C45" s="503" t="s">
+      <c r="B45" s="534"/>
+      <c r="C45" s="502" t="s">
         <v>428</v>
       </c>
-      <c r="D45" s="503"/>
-      <c r="E45" s="503"/>
-      <c r="F45" s="503"/>
+      <c r="D45" s="502"/>
+      <c r="E45" s="502"/>
+      <c r="F45" s="502"/>
       <c r="G45" s="282"/>
       <c r="H45" s="282"/>
       <c r="I45" s="282"/>
@@ -13514,34 +13522,34 @@
       <c r="N45" s="282"/>
     </row>
     <row r="46" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="534"/>
-      <c r="B46" s="535"/>
-      <c r="C46" s="503"/>
-      <c r="D46" s="503"/>
-      <c r="E46" s="503"/>
-      <c r="F46" s="503"/>
-      <c r="G46" s="541" t="s">
+      <c r="A46" s="533"/>
+      <c r="B46" s="534"/>
+      <c r="C46" s="502"/>
+      <c r="D46" s="502"/>
+      <c r="E46" s="502"/>
+      <c r="F46" s="502"/>
+      <c r="G46" s="540" t="s">
         <v>429</v>
       </c>
-      <c r="H46" s="542"/>
-      <c r="I46" s="518"/>
-      <c r="J46" s="518"/>
-      <c r="K46" s="518"/>
-      <c r="L46" s="522"/>
-      <c r="M46" s="540"/>
-      <c r="N46" s="517"/>
+      <c r="H46" s="541"/>
+      <c r="I46" s="517"/>
+      <c r="J46" s="517"/>
+      <c r="K46" s="517"/>
+      <c r="L46" s="521"/>
+      <c r="M46" s="539"/>
+      <c r="N46" s="516"/>
     </row>
     <row r="47" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="534" t="s">
+      <c r="A47" s="533" t="s">
         <v>430</v>
       </c>
-      <c r="B47" s="535"/>
-      <c r="C47" s="502" t="s">
+      <c r="B47" s="534"/>
+      <c r="C47" s="501" t="s">
         <v>431</v>
       </c>
-      <c r="D47" s="502"/>
-      <c r="E47" s="543"/>
-      <c r="F47" s="544"/>
+      <c r="D47" s="501"/>
+      <c r="E47" s="542"/>
+      <c r="F47" s="543"/>
       <c r="G47" s="282"/>
       <c r="H47" s="282"/>
       <c r="I47" s="282"/>
@@ -13552,405 +13560,405 @@
       <c r="N47" s="282"/>
     </row>
     <row r="48" ht="12" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="545"/>
-      <c r="B48" s="546"/>
-      <c r="C48" s="546"/>
-      <c r="D48" s="546"/>
-      <c r="E48" s="546"/>
-      <c r="F48" s="547"/>
-      <c r="G48" s="548" t="s">
+      <c r="A48" s="544"/>
+      <c r="B48" s="545"/>
+      <c r="C48" s="545"/>
+      <c r="D48" s="545"/>
+      <c r="E48" s="545"/>
+      <c r="F48" s="546"/>
+      <c r="G48" s="547" t="s">
         <v>429</v>
       </c>
-      <c r="H48" s="549"/>
-      <c r="I48" s="550"/>
-      <c r="J48" s="550"/>
-      <c r="K48" s="550"/>
-      <c r="L48" s="522"/>
-      <c r="M48" s="551"/>
-      <c r="N48" s="517"/>
+      <c r="H48" s="548"/>
+      <c r="I48" s="549"/>
+      <c r="J48" s="549"/>
+      <c r="K48" s="549"/>
+      <c r="L48" s="521"/>
+      <c r="M48" s="550"/>
+      <c r="N48" s="516"/>
     </row>
     <row r="49" ht="6.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="552"/>
-      <c r="B49" s="553"/>
-      <c r="C49" s="553"/>
-      <c r="D49" s="553"/>
-      <c r="E49" s="553"/>
-      <c r="F49" s="554"/>
-      <c r="G49" s="555"/>
-      <c r="H49" s="556"/>
-      <c r="I49" s="556"/>
-      <c r="J49" s="556"/>
-      <c r="K49" s="556"/>
-      <c r="L49" s="556"/>
-      <c r="M49" s="557"/>
-      <c r="N49" s="517"/>
+      <c r="A49" s="551"/>
+      <c r="B49" s="552"/>
+      <c r="C49" s="552"/>
+      <c r="D49" s="552"/>
+      <c r="E49" s="552"/>
+      <c r="F49" s="553"/>
+      <c r="G49" s="554"/>
+      <c r="H49" s="555"/>
+      <c r="I49" s="555"/>
+      <c r="J49" s="555"/>
+      <c r="K49" s="555"/>
+      <c r="L49" s="555"/>
+      <c r="M49" s="556"/>
+      <c r="N49" s="516"/>
     </row>
     <row r="50" ht="23.25" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="558" t="s">
+      <c r="A50" s="557" t="s">
         <v>432</v>
       </c>
-      <c r="B50" s="559"/>
-      <c r="C50" s="560" t="s">
+      <c r="B50" s="558"/>
+      <c r="C50" s="559" t="s">
         <v>433</v>
       </c>
-      <c r="D50" s="560"/>
-      <c r="E50" s="560"/>
-      <c r="F50" s="560"/>
-      <c r="G50" s="560"/>
-      <c r="H50" s="560"/>
-      <c r="I50" s="561"/>
-      <c r="J50" s="562"/>
-      <c r="K50" s="563"/>
-      <c r="L50" s="563"/>
-      <c r="M50" s="564"/>
+      <c r="D50" s="559"/>
+      <c r="E50" s="559"/>
+      <c r="F50" s="559"/>
+      <c r="G50" s="559"/>
+      <c r="H50" s="559"/>
+      <c r="I50" s="560"/>
+      <c r="J50" s="561"/>
+      <c r="K50" s="562"/>
+      <c r="L50" s="562"/>
+      <c r="M50" s="563"/>
       <c r="N50" s="282"/>
     </row>
     <row r="51" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="565" t="s">
+      <c r="A51" s="564" t="s">
         <v>434</v>
       </c>
-      <c r="B51" s="566"/>
-      <c r="C51" s="566"/>
-      <c r="D51" s="566"/>
-      <c r="E51" s="567"/>
+      <c r="B51" s="565"/>
+      <c r="C51" s="565"/>
+      <c r="D51" s="565"/>
+      <c r="E51" s="566"/>
       <c r="F51" s="294" t="s">
         <v>435</v>
       </c>
-      <c r="G51" s="568" t="s">
+      <c r="G51" s="567" t="s">
         <v>436</v>
       </c>
       <c r="H51" s="414"/>
       <c r="I51" s="417"/>
-      <c r="J51" s="569"/>
-      <c r="K51" s="570"/>
-      <c r="L51" s="570"/>
-      <c r="M51" s="571"/>
+      <c r="J51" s="568"/>
+      <c r="K51" s="569"/>
+      <c r="L51" s="569"/>
+      <c r="M51" s="570"/>
     </row>
     <row r="52" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="572"/>
-      <c r="B52" s="573"/>
-      <c r="C52" s="574"/>
-      <c r="D52" s="574"/>
-      <c r="E52" s="575"/>
-      <c r="F52" s="576"/>
-      <c r="G52" s="577"/>
-      <c r="H52" s="578"/>
-      <c r="I52" s="579"/>
-      <c r="J52" s="569"/>
-      <c r="K52" s="570"/>
-      <c r="L52" s="570"/>
-      <c r="M52" s="571"/>
+      <c r="A52" s="571"/>
+      <c r="B52" s="572"/>
+      <c r="C52" s="573"/>
+      <c r="D52" s="573"/>
+      <c r="E52" s="574"/>
+      <c r="F52" s="575"/>
+      <c r="G52" s="576"/>
+      <c r="H52" s="577"/>
+      <c r="I52" s="578"/>
+      <c r="J52" s="568"/>
+      <c r="K52" s="569"/>
+      <c r="L52" s="569"/>
+      <c r="M52" s="570"/>
     </row>
     <row r="53" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="572"/>
-      <c r="B53" s="573"/>
-      <c r="C53" s="573"/>
-      <c r="D53" s="573"/>
-      <c r="E53" s="580"/>
-      <c r="F53" s="576"/>
-      <c r="G53" s="577"/>
-      <c r="H53" s="578"/>
-      <c r="I53" s="579"/>
-      <c r="J53" s="569"/>
-      <c r="K53" s="570"/>
-      <c r="L53" s="570"/>
-      <c r="M53" s="571"/>
+      <c r="A53" s="571"/>
+      <c r="B53" s="572"/>
+      <c r="C53" s="572"/>
+      <c r="D53" s="572"/>
+      <c r="E53" s="579"/>
+      <c r="F53" s="575"/>
+      <c r="G53" s="576"/>
+      <c r="H53" s="577"/>
+      <c r="I53" s="578"/>
+      <c r="J53" s="568"/>
+      <c r="K53" s="569"/>
+      <c r="L53" s="569"/>
+      <c r="M53" s="570"/>
     </row>
     <row r="54" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="581"/>
-      <c r="B54" s="582"/>
-      <c r="C54" s="583"/>
-      <c r="D54" s="583"/>
-      <c r="E54" s="584"/>
-      <c r="F54" s="585"/>
-      <c r="G54" s="586"/>
-      <c r="H54" s="587"/>
-      <c r="I54" s="588"/>
-      <c r="J54" s="569"/>
-      <c r="K54" s="570"/>
-      <c r="L54" s="570"/>
-      <c r="M54" s="571"/>
+      <c r="A54" s="580"/>
+      <c r="B54" s="581"/>
+      <c r="C54" s="582"/>
+      <c r="D54" s="582"/>
+      <c r="E54" s="583"/>
+      <c r="F54" s="584"/>
+      <c r="G54" s="585"/>
+      <c r="H54" s="586"/>
+      <c r="I54" s="587"/>
+      <c r="J54" s="568"/>
+      <c r="K54" s="569"/>
+      <c r="L54" s="569"/>
+      <c r="M54" s="570"/>
     </row>
     <row r="55" ht="39.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="430" t="s">
+      <c r="A55" s="429" t="s">
         <v>437</v>
       </c>
-      <c r="B55" s="431"/>
-      <c r="C55" s="589" t="s">
+      <c r="B55" s="430"/>
+      <c r="C55" s="588" t="s">
         <v>438</v>
       </c>
-      <c r="D55" s="589"/>
-      <c r="E55" s="589"/>
-      <c r="F55" s="589"/>
-      <c r="G55" s="589"/>
-      <c r="H55" s="589"/>
-      <c r="I55" s="590"/>
-      <c r="J55" s="570"/>
-      <c r="K55" s="570"/>
-      <c r="L55" s="570"/>
-      <c r="M55" s="571"/>
+      <c r="D55" s="588"/>
+      <c r="E55" s="588"/>
+      <c r="F55" s="588"/>
+      <c r="G55" s="588"/>
+      <c r="H55" s="588"/>
+      <c r="I55" s="589"/>
+      <c r="J55" s="569"/>
+      <c r="K55" s="569"/>
+      <c r="L55" s="569"/>
+      <c r="M55" s="570"/>
     </row>
     <row r="56" ht="13.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="591"/>
-      <c r="B56" s="592"/>
-      <c r="C56" s="593"/>
-      <c r="D56" s="593"/>
-      <c r="E56" s="593"/>
-      <c r="F56" s="593"/>
-      <c r="G56" s="593"/>
-      <c r="H56" s="593"/>
-      <c r="I56" s="594"/>
-      <c r="J56" s="595"/>
-      <c r="K56" s="596" t="s">
+      <c r="A56" s="590"/>
+      <c r="B56" s="591"/>
+      <c r="C56" s="592"/>
+      <c r="D56" s="592"/>
+      <c r="E56" s="592"/>
+      <c r="F56" s="592"/>
+      <c r="G56" s="592"/>
+      <c r="H56" s="592"/>
+      <c r="I56" s="593"/>
+      <c r="J56" s="594"/>
+      <c r="K56" s="595" t="s">
         <v>439</v>
       </c>
-      <c r="L56" s="596"/>
-      <c r="M56" s="597"/>
+      <c r="L56" s="595"/>
+      <c r="M56" s="596"/>
     </row>
     <row r="57" ht="13.5" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="591"/>
-      <c r="B57" s="592"/>
-      <c r="C57" s="593"/>
-      <c r="D57" s="593"/>
-      <c r="E57" s="593"/>
-      <c r="F57" s="593"/>
-      <c r="G57" s="593"/>
-      <c r="H57" s="593"/>
-      <c r="I57" s="594"/>
-      <c r="J57" s="596"/>
-      <c r="K57" s="596"/>
-      <c r="L57" s="596"/>
-      <c r="M57" s="598"/>
+      <c r="A57" s="590"/>
+      <c r="B57" s="591"/>
+      <c r="C57" s="592"/>
+      <c r="D57" s="592"/>
+      <c r="E57" s="592"/>
+      <c r="F57" s="592"/>
+      <c r="G57" s="592"/>
+      <c r="H57" s="592"/>
+      <c r="I57" s="593"/>
+      <c r="J57" s="595"/>
+      <c r="K57" s="595"/>
+      <c r="L57" s="595"/>
+      <c r="M57" s="597"/>
     </row>
     <row r="58" ht="7.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="599"/>
-      <c r="B58" s="600"/>
-      <c r="C58" s="601"/>
-      <c r="D58" s="601"/>
-      <c r="E58" s="601"/>
-      <c r="F58" s="601"/>
-      <c r="G58" s="601"/>
-      <c r="H58" s="601"/>
-      <c r="I58" s="602"/>
+      <c r="A58" s="598"/>
+      <c r="B58" s="599"/>
+      <c r="C58" s="600"/>
+      <c r="D58" s="600"/>
+      <c r="E58" s="600"/>
+      <c r="F58" s="600"/>
+      <c r="G58" s="600"/>
+      <c r="H58" s="600"/>
+      <c r="I58" s="601"/>
       <c r="J58" s="282"/>
-      <c r="K58" s="603"/>
-      <c r="L58" s="604"/>
+      <c r="K58" s="602"/>
+      <c r="L58" s="603"/>
       <c r="M58" s="378"/>
     </row>
     <row r="59" ht="8.25" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="605"/>
+      <c r="A59" s="604"/>
       <c r="B59" s="282"/>
-      <c r="C59" s="444"/>
-      <c r="D59" s="444"/>
-      <c r="E59" s="444"/>
-      <c r="F59" s="444"/>
-      <c r="G59" s="444"/>
-      <c r="H59" s="444"/>
-      <c r="I59" s="444"/>
+      <c r="C59" s="443"/>
+      <c r="D59" s="443"/>
+      <c r="E59" s="443"/>
+      <c r="F59" s="443"/>
+      <c r="G59" s="443"/>
+      <c r="H59" s="443"/>
+      <c r="I59" s="443"/>
       <c r="J59" s="282"/>
-      <c r="K59" s="606"/>
-      <c r="L59" s="607"/>
+      <c r="K59" s="605"/>
+      <c r="L59" s="606"/>
       <c r="M59" s="378"/>
     </row>
     <row r="60" ht="25.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="608"/>
-      <c r="B60" s="609" t="s">
+      <c r="A60" s="607"/>
+      <c r="B60" s="608" t="s">
         <v>440</v>
       </c>
-      <c r="C60" s="610"/>
-      <c r="D60" s="611"/>
+      <c r="C60" s="609"/>
+      <c r="D60" s="610"/>
       <c r="E60" s="282"/>
-      <c r="F60" s="612"/>
-      <c r="G60" s="613"/>
-      <c r="H60" s="613"/>
-      <c r="I60" s="614"/>
+      <c r="F60" s="611"/>
+      <c r="G60" s="612"/>
+      <c r="H60" s="612"/>
+      <c r="I60" s="613"/>
       <c r="J60" s="282"/>
-      <c r="K60" s="606"/>
-      <c r="L60" s="607"/>
-      <c r="M60" s="615"/>
+      <c r="K60" s="605"/>
+      <c r="L60" s="606"/>
+      <c r="M60" s="614"/>
     </row>
     <row r="61" ht="20.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="608"/>
-      <c r="B61" s="616" t="s">
+      <c r="A61" s="607"/>
+      <c r="B61" s="615" t="s">
         <v>441</v>
       </c>
-      <c r="C61" s="617"/>
-      <c r="D61" s="618"/>
+      <c r="C61" s="616"/>
+      <c r="D61" s="617"/>
       <c r="E61" s="282"/>
-      <c r="F61" s="619"/>
-      <c r="G61" s="620"/>
-      <c r="H61" s="620"/>
-      <c r="I61" s="621"/>
+      <c r="F61" s="618"/>
+      <c r="G61" s="619"/>
+      <c r="H61" s="619"/>
+      <c r="I61" s="620"/>
       <c r="J61" s="282"/>
-      <c r="K61" s="606"/>
-      <c r="L61" s="607"/>
-      <c r="M61" s="615"/>
+      <c r="K61" s="605"/>
+      <c r="L61" s="606"/>
+      <c r="M61" s="614"/>
     </row>
     <row r="62" ht="9" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="608"/>
-      <c r="B62" s="622" t="s">
+      <c r="A62" s="607"/>
+      <c r="B62" s="621" t="s">
         <v>442</v>
       </c>
-      <c r="C62" s="623"/>
-      <c r="D62" s="624"/>
+      <c r="C62" s="622"/>
+      <c r="D62" s="623"/>
       <c r="E62" s="282"/>
-      <c r="F62" s="625"/>
-      <c r="G62" s="626"/>
-      <c r="H62" s="626"/>
-      <c r="I62" s="627"/>
+      <c r="F62" s="624"/>
+      <c r="G62" s="625"/>
+      <c r="H62" s="625"/>
+      <c r="I62" s="626"/>
       <c r="J62" s="282"/>
-      <c r="K62" s="606"/>
-      <c r="L62" s="607"/>
-      <c r="M62" s="615"/>
+      <c r="K62" s="605"/>
+      <c r="L62" s="606"/>
+      <c r="M62" s="614"/>
     </row>
     <row r="63" ht="12" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="608"/>
-      <c r="B63" s="628"/>
-      <c r="C63" s="629"/>
-      <c r="D63" s="630"/>
+      <c r="A63" s="607"/>
+      <c r="B63" s="627"/>
+      <c r="C63" s="628"/>
+      <c r="D63" s="629"/>
       <c r="E63" s="282"/>
-      <c r="F63" s="631" t="s">
+      <c r="F63" s="630" t="s">
         <v>443</v>
       </c>
-      <c r="G63" s="632"/>
-      <c r="H63" s="632"/>
-      <c r="I63" s="633"/>
+      <c r="G63" s="631"/>
+      <c r="H63" s="631"/>
+      <c r="I63" s="632"/>
       <c r="J63" s="282"/>
-      <c r="K63" s="606"/>
-      <c r="L63" s="607"/>
-      <c r="M63" s="615"/>
+      <c r="K63" s="605"/>
+      <c r="L63" s="606"/>
+      <c r="M63" s="614"/>
     </row>
     <row r="64" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="608"/>
-      <c r="B64" s="622" t="s">
+      <c r="A64" s="607"/>
+      <c r="B64" s="621" t="s">
         <v>444</v>
       </c>
-      <c r="C64" s="623"/>
-      <c r="D64" s="624"/>
+      <c r="C64" s="622"/>
+      <c r="D64" s="623"/>
       <c r="E64" s="282"/>
-      <c r="F64" s="634"/>
+      <c r="F64" s="633"/>
       <c r="G64" s="125"/>
       <c r="H64" s="125"/>
       <c r="I64" s="126"/>
-      <c r="J64" s="635"/>
-      <c r="K64" s="636"/>
-      <c r="L64" s="637"/>
-      <c r="M64" s="615"/>
+      <c r="J64" s="634"/>
+      <c r="K64" s="635"/>
+      <c r="L64" s="636"/>
+      <c r="M64" s="614"/>
     </row>
     <row r="65" ht="12.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="608"/>
-      <c r="B65" s="638"/>
-      <c r="C65" s="639"/>
-      <c r="D65" s="640"/>
+      <c r="A65" s="607"/>
+      <c r="B65" s="637"/>
+      <c r="C65" s="638"/>
+      <c r="D65" s="639"/>
       <c r="E65" s="282"/>
-      <c r="F65" s="641" t="s">
+      <c r="F65" s="640" t="s">
         <v>445</v>
       </c>
-      <c r="G65" s="642"/>
-      <c r="H65" s="642"/>
-      <c r="I65" s="643"/>
-      <c r="J65" s="635"/>
-      <c r="K65" s="644" t="s">
+      <c r="G65" s="641"/>
+      <c r="H65" s="641"/>
+      <c r="I65" s="642"/>
+      <c r="J65" s="634"/>
+      <c r="K65" s="643" t="s">
         <v>446</v>
       </c>
-      <c r="L65" s="645"/>
-      <c r="M65" s="615"/>
+      <c r="L65" s="644"/>
+      <c r="M65" s="614"/>
     </row>
     <row r="66" ht="8.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="638"/>
-      <c r="B66" s="639"/>
-      <c r="C66" s="646"/>
-      <c r="D66" s="646"/>
-      <c r="E66" s="647"/>
-      <c r="F66" s="646"/>
-      <c r="G66" s="646"/>
-      <c r="H66" s="646"/>
-      <c r="I66" s="646"/>
-      <c r="J66" s="639"/>
-      <c r="K66" s="648"/>
-      <c r="L66" s="648"/>
-      <c r="M66" s="649"/>
+      <c r="A66" s="637"/>
+      <c r="B66" s="638"/>
+      <c r="C66" s="645"/>
+      <c r="D66" s="645"/>
+      <c r="E66" s="646"/>
+      <c r="F66" s="645"/>
+      <c r="G66" s="645"/>
+      <c r="H66" s="645"/>
+      <c r="I66" s="645"/>
+      <c r="J66" s="638"/>
+      <c r="K66" s="647"/>
+      <c r="L66" s="647"/>
+      <c r="M66" s="648"/>
     </row>
     <row r="67" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="650" t="s">
+      <c r="A67" s="649" t="s">
         <v>447</v>
       </c>
-      <c r="B67" s="651"/>
-      <c r="C67" s="651"/>
-      <c r="D67" s="651"/>
-      <c r="E67" s="651"/>
-      <c r="F67" s="651"/>
-      <c r="G67" s="651"/>
-      <c r="H67" s="651"/>
-      <c r="I67" s="651"/>
-      <c r="J67" s="651"/>
-      <c r="K67" s="651"/>
-      <c r="L67" s="651"/>
-      <c r="M67" s="652"/>
+      <c r="B67" s="650"/>
+      <c r="C67" s="650"/>
+      <c r="D67" s="650"/>
+      <c r="E67" s="650"/>
+      <c r="F67" s="650"/>
+      <c r="G67" s="650"/>
+      <c r="H67" s="650"/>
+      <c r="I67" s="650"/>
+      <c r="J67" s="650"/>
+      <c r="K67" s="650"/>
+      <c r="L67" s="650"/>
+      <c r="M67" s="651"/>
     </row>
     <row r="68" ht="53.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="608"/>
-      <c r="B68" s="635"/>
-      <c r="C68" s="653"/>
-      <c r="D68" s="653"/>
-      <c r="E68" s="654"/>
-      <c r="F68" s="655"/>
-      <c r="G68" s="655"/>
-      <c r="H68" s="655"/>
-      <c r="I68" s="656"/>
-      <c r="J68" s="657"/>
-      <c r="K68" s="657"/>
+      <c r="A68" s="607"/>
+      <c r="B68" s="634"/>
+      <c r="C68" s="652"/>
+      <c r="D68" s="652"/>
+      <c r="E68" s="653"/>
+      <c r="F68" s="654"/>
+      <c r="G68" s="654"/>
+      <c r="H68" s="654"/>
+      <c r="I68" s="655"/>
+      <c r="J68" s="656"/>
+      <c r="K68" s="656"/>
       <c r="L68" s="282"/>
-      <c r="M68" s="615"/>
+      <c r="M68" s="614"/>
     </row>
     <row r="69" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="608"/>
-      <c r="B69" s="635"/>
-      <c r="C69" s="570"/>
-      <c r="D69" s="570"/>
-      <c r="E69" s="658" t="s">
+      <c r="A69" s="607"/>
+      <c r="B69" s="634"/>
+      <c r="C69" s="569"/>
+      <c r="D69" s="569"/>
+      <c r="E69" s="657" t="s">
         <v>448</v>
       </c>
-      <c r="F69" s="659"/>
-      <c r="G69" s="659"/>
-      <c r="H69" s="659"/>
-      <c r="I69" s="660"/>
-      <c r="J69" s="661"/>
-      <c r="K69" s="662"/>
+      <c r="F69" s="658"/>
+      <c r="G69" s="658"/>
+      <c r="H69" s="658"/>
+      <c r="I69" s="659"/>
+      <c r="J69" s="660"/>
+      <c r="K69" s="661"/>
       <c r="L69" s="1"/>
-      <c r="M69" s="615"/>
-    </row>
-    <row r="70" ht="11.25" customHeight="1" spans="1:13" s="663" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="664"/>
-      <c r="B70" s="665"/>
-      <c r="C70" s="665"/>
-      <c r="D70" s="665"/>
-      <c r="E70" s="665"/>
-      <c r="F70" s="665"/>
-      <c r="G70" s="665"/>
-      <c r="H70" s="665"/>
-      <c r="I70" s="665"/>
-      <c r="J70" s="665"/>
-      <c r="K70" s="665"/>
-      <c r="L70" s="665"/>
-      <c r="M70" s="666"/>
+      <c r="M69" s="614"/>
+    </row>
+    <row r="70" ht="11.25" customHeight="1" spans="1:13" s="662" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="663"/>
+      <c r="B70" s="664"/>
+      <c r="C70" s="664"/>
+      <c r="D70" s="664"/>
+      <c r="E70" s="664"/>
+      <c r="F70" s="664"/>
+      <c r="G70" s="664"/>
+      <c r="H70" s="664"/>
+      <c r="I70" s="664"/>
+      <c r="J70" s="664"/>
+      <c r="K70" s="664"/>
+      <c r="L70" s="664"/>
+      <c r="M70" s="665"/>
     </row>
     <row r="71" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="667" t="s">
+      <c r="A71" s="666" t="s">
         <v>449</v>
       </c>
-      <c r="B71" s="667"/>
-      <c r="C71" s="667"/>
-      <c r="D71" s="667"/>
-      <c r="E71" s="667"/>
-      <c r="F71" s="667"/>
-      <c r="G71" s="667"/>
-      <c r="H71" s="667"/>
-      <c r="I71" s="667"/>
-      <c r="J71" s="667"/>
-      <c r="K71" s="667"/>
-      <c r="L71" s="667"/>
-      <c r="M71" s="667"/>
+      <c r="B71" s="666"/>
+      <c r="C71" s="666"/>
+      <c r="D71" s="666"/>
+      <c r="E71" s="666"/>
+      <c r="F71" s="666"/>
+      <c r="G71" s="666"/>
+      <c r="H71" s="666"/>
+      <c r="I71" s="666"/>
+      <c r="J71" s="666"/>
+      <c r="K71" s="666"/>
+      <c r="L71" s="666"/>
+      <c r="M71" s="666"/>
     </row>
   </sheetData>
   <mergeCells count="85">
@@ -14063,13 +14071,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="668" t="s">
+      <c r="A1" s="667" t="s">
         <v>450</v>
       </c>
-      <c r="B1" s="668" t="s">
+      <c r="B1" s="667" t="s">
         <v>451</v>
       </c>
-      <c r="C1" s="668" t="s">
+      <c r="C1" s="667" t="s">
         <v>452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add signature to page 4
</commit_message>
<xml_diff>
--- a/backend/temp/updated_filled_pds.xlsx
+++ b/backend/temp/updated_filled_pds.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="461">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -1381,6 +1381,12 @@
   </si>
   <si>
     <t>TEL. NO.</t>
+  </si>
+  <si>
+    <t>079678575467</t>
+  </si>
+  <si>
+    <t>879567463</t>
   </si>
   <si>
     <t>42.</t>
@@ -4485,7 +4491,7 @@
     <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="27" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4497,10 +4503,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4512,7 +4518,7 @@
     <xf numFmtId="49" fontId="27" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="27" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4524,10 +4530,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4771,19 +4777,14 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="476250"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1">
@@ -4814,105 +4815,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6760,7 +6663,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="60" ht="90" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" ht="27.75" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="268" t="s">
         <v>189</v>
       </c>
@@ -10875,7 +10778,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.3" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="80" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-  <drawing r:id="rId205"/>
 </worksheet>
 </file>
 
@@ -11683,7 +11585,7 @@
       <c r="L46" s="350"/>
       <c r="M46" s="351"/>
     </row>
-    <row r="47" ht="60" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" ht="27.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="268" t="s">
         <v>189</v>
       </c>
@@ -11855,7 +11757,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.15748031496062992" right="0" top="0.15748031496062992" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="92" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11874,7 +11775,7 @@
   <cols>
     <col min="1" max="1" width="3.7109375" style="282" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" style="282" customWidth="1"/>
-    <col min="3" max="3" width="10" style="282" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="282" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="282" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="282" customWidth="1"/>
     <col min="6" max="7" width="10.140625" style="282" customWidth="1"/>
@@ -12622,7 +12523,7 @@
       <c r="J49" s="266"/>
       <c r="K49" s="321"/>
     </row>
-    <row r="50" ht="70" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="268" t="s">
         <v>189</v>
       </c>
@@ -12738,7 +12639,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.15748031496062992" right="0" top="0.35433070866141736" bottom="0" header="0.31496062992125984" footer="0"/>
   <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="81" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13635,13 +13535,19 @@
       <c r="M51" s="570"/>
     </row>
     <row r="52" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="571"/>
+      <c r="A52" s="571" t="s">
+        <v>358</v>
+      </c>
       <c r="B52" s="572"/>
       <c r="C52" s="573"/>
       <c r="D52" s="573"/>
       <c r="E52" s="574"/>
-      <c r="F52" s="575"/>
-      <c r="G52" s="576"/>
+      <c r="F52" s="575" t="s">
+        <v>358</v>
+      </c>
+      <c r="G52" s="576" t="s">
+        <v>437</v>
+      </c>
       <c r="H52" s="577"/>
       <c r="I52" s="578"/>
       <c r="J52" s="568"/>
@@ -13650,13 +13556,19 @@
       <c r="M52" s="570"/>
     </row>
     <row r="53" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="571"/>
+      <c r="A53" s="571" t="s">
+        <v>358</v>
+      </c>
       <c r="B53" s="572"/>
       <c r="C53" s="572"/>
       <c r="D53" s="572"/>
       <c r="E53" s="579"/>
-      <c r="F53" s="575"/>
-      <c r="G53" s="576"/>
+      <c r="F53" s="575" t="s">
+        <v>358</v>
+      </c>
+      <c r="G53" s="576" t="s">
+        <v>438</v>
+      </c>
       <c r="H53" s="577"/>
       <c r="I53" s="578"/>
       <c r="J53" s="568"/>
@@ -13681,11 +13593,11 @@
     </row>
     <row r="55" ht="39.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="429" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B55" s="430"/>
       <c r="C55" s="588" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D55" s="588"/>
       <c r="E55" s="588"/>
@@ -13710,7 +13622,7 @@
       <c r="I56" s="593"/>
       <c r="J56" s="594"/>
       <c r="K56" s="595" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="L56" s="595"/>
       <c r="M56" s="596"/>
@@ -13763,7 +13675,7 @@
     <row r="60" ht="25.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="607"/>
       <c r="B60" s="608" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C60" s="609"/>
       <c r="D60" s="610"/>
@@ -13777,10 +13689,10 @@
       <c r="L60" s="606"/>
       <c r="M60" s="614"/>
     </row>
-    <row r="61" ht="20.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" ht="50" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="607"/>
       <c r="B61" s="615" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C61" s="616"/>
       <c r="D61" s="617"/>
@@ -13797,7 +13709,7 @@
     <row r="62" ht="9" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="607"/>
       <c r="B62" s="621" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C62" s="622"/>
       <c r="D62" s="623"/>
@@ -13818,7 +13730,7 @@
       <c r="D63" s="629"/>
       <c r="E63" s="282"/>
       <c r="F63" s="630" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="G63" s="631"/>
       <c r="H63" s="631"/>
@@ -13831,12 +13743,14 @@
     <row r="64" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="607"/>
       <c r="B64" s="621" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C64" s="622"/>
       <c r="D64" s="623"/>
       <c r="E64" s="282"/>
-      <c r="F64" s="633"/>
+      <c r="F64" s="633" t="s">
+        <v>182</v>
+      </c>
       <c r="G64" s="125"/>
       <c r="H64" s="125"/>
       <c r="I64" s="126"/>
@@ -13852,14 +13766,14 @@
       <c r="D65" s="639"/>
       <c r="E65" s="282"/>
       <c r="F65" s="640" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="G65" s="641"/>
       <c r="H65" s="641"/>
       <c r="I65" s="642"/>
       <c r="J65" s="634"/>
       <c r="K65" s="643" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="L65" s="644"/>
       <c r="M65" s="614"/>
@@ -13881,7 +13795,7 @@
     </row>
     <row r="67" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="649" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B67" s="650"/>
       <c r="C67" s="650"/>
@@ -13917,7 +13831,7 @@
       <c r="C69" s="569"/>
       <c r="D69" s="569"/>
       <c r="E69" s="657" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="F69" s="658"/>
       <c r="G69" s="658"/>
@@ -13945,7 +13859,7 @@
     </row>
     <row r="71" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="666" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B71" s="666"/>
       <c r="C71" s="666"/>
@@ -14051,6 +13965,7 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.12" right="0" top="0.34" bottom="0" header="0.17" footer="0"/>
   <pageSetup paperSize="5" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="97" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14072,35 +13987,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="667" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B1" s="667" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C1" s="667" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -14110,7 +14025,7 @@
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add initial pds fix
</commit_message>
<xml_diff>
--- a/backend/temp/updated_filled_pds.xlsx
+++ b/backend/temp/updated_filled_pds.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="460">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -88,7 +88,7 @@
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> Adnan</t>
+    <t xml:space="preserve"> Adnanss</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -383,6 +383,9 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
+    <t xml:space="preserve"> s</t>
+  </si>
+  <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
   </si>
   <si>
@@ -618,7 +621,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>2024-10-03</t>
+    <t>2024-10-09</t>
   </si>
   <si>
     <t>Cyprus</t>
@@ -1121,7 +1124,7 @@
 Validity</t>
   </si>
   <si>
-    <t>s</t>
+    <t>test122</t>
   </si>
   <si>
     <t xml:space="preserve">V.  WORK EXPERIENCE </t>
@@ -1154,46 +1157,37 @@
     <t>GOV'T SERVICE                                                                                                                                       (Y/ N)</t>
   </si>
   <si>
+    <t xml:space="preserve">                               CS FORM 212 (Revised 2017), Page 2 of 4</t>
+  </si>
+  <si>
+    <t>VI. VOLUNTARY WORK OR INVOLVEMENT IN CIVIC / NON-GOVERNMENT / PEOPLE / VOLUNTARY ORGANIZATION/S</t>
+  </si>
+  <si>
+    <t>29.</t>
+  </si>
+  <si>
+    <t>NAME &amp; ADDRESS OF ORGANIZATION                                                                                                     (Write in full)</t>
+  </si>
+  <si>
+    <t>INCLUSIVE DATES                                                                                                                             (mm/dd/yyyy)</t>
+  </si>
+  <si>
+    <t>NUMBER OF HOURS</t>
+  </si>
+  <si>
+    <t>POSITION / NATURE OF WORK</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>asdasdas</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>20000.00</t>
-  </si>
-  <si>
-    <t>Permanent</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                               CS FORM 212 (Revised 2017), Page 2 of 4</t>
-  </si>
-  <si>
-    <t>VI. VOLUNTARY WORK OR INVOLVEMENT IN CIVIC / NON-GOVERNMENT / PEOPLE / VOLUNTARY ORGANIZATION/S</t>
-  </si>
-  <si>
-    <t>29.</t>
-  </si>
-  <si>
-    <t>NAME &amp; ADDRESS OF ORGANIZATION                                                                                                     (Write in full)</t>
-  </si>
-  <si>
-    <t>INCLUSIVE DATES                                                                                                                             (mm/dd/yyyy)</t>
-  </si>
-  <si>
-    <t>NUMBER OF HOURS</t>
-  </si>
-  <si>
-    <t>POSITION / NATURE OF WORK</t>
-  </si>
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>asdasdas</t>
-  </si>
-  <si>
-    <t>123123</t>
   </si>
   <si>
     <t>VII.  LEARNING AND DEVELOPMENT (L&amp;D) INTERVENTIONS/TRAINING PROGRAMS ATTENDED</t>
@@ -6068,30 +6062,30 @@
       </c>
       <c r="C36" s="174"/>
       <c r="D36" s="175" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="E36" s="175"/>
       <c r="F36" s="175"/>
       <c r="G36" s="175"/>
       <c r="H36" s="175"/>
       <c r="I36" s="176" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J36" s="176"/>
       <c r="K36" s="176"/>
       <c r="L36" s="177"/>
       <c r="M36" s="178" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N36" s="179"/>
       <c r="Q36" s="57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="69"/>
       <c r="B37" s="103" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C37" s="155"/>
       <c r="D37" s="180" t="s">
@@ -6100,27 +6094,27 @@
       <c r="E37" s="181"/>
       <c r="F37" s="182"/>
       <c r="G37" s="183" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H37" s="183"/>
       <c r="I37" s="184" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J37" s="184"/>
       <c r="K37" s="184"/>
       <c r="L37" s="185"/>
       <c r="M37" s="186" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N37" s="187"/>
       <c r="Q37" s="57" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="188"/>
       <c r="B38" s="189" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C38" s="190"/>
       <c r="D38" s="180" t="s">
@@ -6131,23 +6125,23 @@
       <c r="G38" s="181"/>
       <c r="H38" s="182"/>
       <c r="I38" s="184" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J38" s="184"/>
       <c r="K38" s="184"/>
       <c r="L38" s="185"/>
       <c r="M38" s="186" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N38" s="187"/>
       <c r="Q38" s="57" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="191"/>
       <c r="B39" s="73" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C39" s="83"/>
       <c r="D39" s="192" t="s">
@@ -6164,13 +6158,13 @@
       <c r="M39" s="186"/>
       <c r="N39" s="187"/>
       <c r="Q39" s="57" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="191"/>
       <c r="B40" s="73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C40" s="83"/>
       <c r="D40" s="192" t="s">
@@ -6187,13 +6181,13 @@
       <c r="M40" s="186"/>
       <c r="N40" s="187"/>
       <c r="Q40" s="57" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="191"/>
       <c r="B41" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C41" s="83"/>
       <c r="D41" s="192" t="s">
@@ -6210,13 +6204,13 @@
       <c r="M41" s="186"/>
       <c r="N41" s="187"/>
       <c r="Q41" s="57" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="93"/>
       <c r="B42" s="94" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C42" s="193"/>
       <c r="D42" s="192" t="s">
@@ -6233,19 +6227,19 @@
       <c r="M42" s="186"/>
       <c r="N42" s="187"/>
       <c r="Q42" s="57" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="194" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B43" s="195" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C43" s="94"/>
       <c r="D43" s="192" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E43" s="192"/>
       <c r="F43" s="192"/>
@@ -6258,7 +6252,7 @@
       <c r="M43" s="186"/>
       <c r="N43" s="187"/>
       <c r="Q43" s="57" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6268,12 +6262,12 @@
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="180" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E44" s="181"/>
       <c r="F44" s="182"/>
       <c r="G44" s="183" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H44" s="183"/>
       <c r="I44" s="184"/>
@@ -6283,7 +6277,7 @@
       <c r="M44" s="186"/>
       <c r="N44" s="187"/>
       <c r="Q44" s="57" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6306,15 +6300,15 @@
       <c r="M45" s="186"/>
       <c r="N45" s="187"/>
       <c r="Q45" s="57" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="69" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B46" s="127" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C46" s="127"/>
       <c r="D46" s="127"/>
@@ -6329,7 +6323,7 @@
       <c r="M46" s="186"/>
       <c r="N46" s="187"/>
       <c r="Q46" s="57" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6352,7 +6346,7 @@
       <c r="M47" s="186"/>
       <c r="N47" s="187"/>
       <c r="Q47" s="57" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6362,7 +6356,7 @@
       </c>
       <c r="C48" s="41"/>
       <c r="D48" s="196" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E48" s="196"/>
       <c r="F48" s="196"/>
@@ -6375,7 +6369,7 @@
       <c r="M48" s="186"/>
       <c r="N48" s="187"/>
       <c r="Q48" s="57" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" ht="21" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6392,7 +6386,7 @@
       <c r="G49" s="198"/>
       <c r="H49" s="198"/>
       <c r="I49" s="199" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J49" s="199"/>
       <c r="K49" s="199"/>
@@ -6400,12 +6394,12 @@
       <c r="M49" s="199"/>
       <c r="N49" s="200"/>
       <c r="Q49" s="57" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="201" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B50" s="201"/>
       <c r="C50" s="202"/>
@@ -6415,7 +6409,7 @@
       <c r="G50" s="203"/>
       <c r="H50" s="203"/>
       <c r="I50" s="204" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J50" s="204"/>
       <c r="K50" s="204"/>
@@ -6423,42 +6417,42 @@
       <c r="M50" s="204"/>
       <c r="N50" s="205"/>
       <c r="Q50" s="57" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="206" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B51" s="207" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C51" s="207"/>
       <c r="D51" s="208" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E51" s="209"/>
       <c r="F51" s="210"/>
       <c r="G51" s="208" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H51" s="209"/>
       <c r="I51" s="211"/>
       <c r="J51" s="212" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K51" s="213"/>
       <c r="L51" s="214" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M51" s="215" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N51" s="216" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Q51" s="57" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" ht="19.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6477,7 +6471,7 @@
       <c r="M52" s="215"/>
       <c r="N52" s="216"/>
       <c r="Q52" s="57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6491,10 +6485,10 @@
       <c r="H53" s="226"/>
       <c r="I53" s="227"/>
       <c r="J53" s="228" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K53" s="229" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L53" s="230"/>
       <c r="M53" s="231"/>
@@ -6502,17 +6496,17 @@
       <c r="O53" s="233"/>
       <c r="P53" s="233"/>
       <c r="Q53" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="234"/>
       <c r="B54" s="235" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C54" s="235"/>
       <c r="D54" s="236" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E54" s="237"/>
       <c r="F54" s="238"/>
@@ -6522,10 +6516,10 @@
       <c r="H54" s="240"/>
       <c r="I54" s="241"/>
       <c r="J54" s="242" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K54" s="243" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L54" s="244" t="s">
         <v>14</v>
@@ -6537,17 +6531,17 @@
         <v>14</v>
       </c>
       <c r="Q54" s="57" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="234"/>
       <c r="B55" s="235" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C55" s="235"/>
       <c r="D55" s="236" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E55" s="237"/>
       <c r="F55" s="238"/>
@@ -6557,28 +6551,28 @@
       <c r="H55" s="240"/>
       <c r="I55" s="241"/>
       <c r="J55" s="242" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K55" s="247" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L55" s="248" t="s">
         <v>14</v>
       </c>
       <c r="M55" s="249" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N55" s="246" t="s">
         <v>14</v>
       </c>
       <c r="Q55" s="57" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="234"/>
       <c r="B56" s="235" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C56" s="235"/>
       <c r="D56" s="236"/>
@@ -6593,48 +6587,48 @@
       <c r="M56" s="245"/>
       <c r="N56" s="246"/>
       <c r="Q56" s="57" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="234"/>
       <c r="B57" s="235" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C57" s="235"/>
       <c r="D57" s="236" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E57" s="237"/>
       <c r="F57" s="238"/>
       <c r="G57" s="250" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H57" s="251"/>
       <c r="I57" s="252"/>
       <c r="J57" s="242" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K57" s="247" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L57" s="244" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M57" s="249" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N57" s="246" t="s">
         <v>14</v>
       </c>
       <c r="Q57" s="57" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="253"/>
       <c r="B58" s="254" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C58" s="254"/>
       <c r="D58" s="255"/>
@@ -6649,12 +6643,12 @@
       <c r="M58" s="264"/>
       <c r="N58" s="246"/>
       <c r="Q58" s="57" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" ht="12" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="265" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B59" s="266"/>
       <c r="C59" s="266"/>
@@ -6670,12 +6664,12 @@
       <c r="M59" s="266"/>
       <c r="N59" s="267"/>
       <c r="Q59" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" ht="27.75" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="268" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B60" s="269"/>
       <c r="C60" s="270"/>
@@ -6686,23 +6680,23 @@
       <c r="H60" s="272"/>
       <c r="I60" s="273"/>
       <c r="J60" s="274" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K60" s="275"/>
       <c r="L60" s="276" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M60" s="277"/>
       <c r="N60" s="278"/>
       <c r="Q60" s="57" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
     </row>
     <row r="61" ht="12" customHeight="1" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="279" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B61" s="279"/>
       <c r="C61" s="279"/>
@@ -6718,7 +6712,7 @@
       <c r="M61" s="279"/>
       <c r="N61" s="279"/>
       <c r="Q61" s="280" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="R61" s="49"/>
       <c r="S61" s="49"/>
@@ -6739,7 +6733,7 @@
       <c r="M62" s="281"/>
       <c r="N62" s="281"/>
       <c r="Q62" s="57" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6758,7 +6752,7 @@
       <c r="M63" s="281"/>
       <c r="N63" s="281"/>
       <c r="Q63" s="57" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6777,7 +6771,7 @@
       <c r="M64" s="281"/>
       <c r="N64" s="281"/>
       <c r="Q64" s="57" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6796,7 +6790,7 @@
       <c r="M65" s="281"/>
       <c r="N65" s="281"/>
       <c r="Q65" s="57" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6815,7 +6809,7 @@
       <c r="M66" s="281"/>
       <c r="N66" s="281"/>
       <c r="Q66" s="57" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6834,7 +6828,7 @@
       <c r="M67" s="281"/>
       <c r="N67" s="281"/>
       <c r="Q67" s="57" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6853,7 +6847,7 @@
       <c r="M68" s="281"/>
       <c r="N68" s="281"/>
       <c r="Q68" s="57" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6872,7 +6866,7 @@
       <c r="M69" s="281"/>
       <c r="N69" s="281"/>
       <c r="Q69" s="57" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6891,7 +6885,7 @@
       <c r="M70" s="281"/>
       <c r="N70" s="281"/>
       <c r="Q70" s="57" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6910,7 +6904,7 @@
       <c r="M71" s="281"/>
       <c r="N71" s="281"/>
       <c r="Q71" s="57" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6929,7 +6923,7 @@
       <c r="M72" s="281"/>
       <c r="N72" s="281"/>
       <c r="Q72" s="57" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6948,7 +6942,7 @@
       <c r="M73" s="281"/>
       <c r="N73" s="281"/>
       <c r="Q73" s="57" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6967,7 +6961,7 @@
       <c r="M74" s="281"/>
       <c r="N74" s="281"/>
       <c r="Q74" s="57" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6986,7 +6980,7 @@
       <c r="M75" s="281"/>
       <c r="N75" s="281"/>
       <c r="Q75" s="57" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7005,7 +6999,7 @@
       <c r="M76" s="281"/>
       <c r="N76" s="281"/>
       <c r="Q76" s="57" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7024,7 +7018,7 @@
       <c r="M77" s="281"/>
       <c r="N77" s="281"/>
       <c r="Q77" s="57" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7043,7 +7037,7 @@
       <c r="M78" s="281"/>
       <c r="N78" s="281"/>
       <c r="Q78" s="57" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7062,7 +7056,7 @@
       <c r="M79" s="281"/>
       <c r="N79" s="281"/>
       <c r="Q79" s="57" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7081,7 +7075,7 @@
       <c r="M80" s="281"/>
       <c r="N80" s="281"/>
       <c r="Q80" s="57" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7100,7 +7094,7 @@
       <c r="M81" s="281"/>
       <c r="N81" s="281"/>
       <c r="Q81" s="57" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7119,7 +7113,7 @@
       <c r="M82" s="281"/>
       <c r="N82" s="281"/>
       <c r="Q82" s="57" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7138,7 +7132,7 @@
       <c r="M83" s="281"/>
       <c r="N83" s="281"/>
       <c r="Q83" s="57" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7157,7 +7151,7 @@
       <c r="M84" s="281"/>
       <c r="N84" s="281"/>
       <c r="Q84" s="57" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7176,7 +7170,7 @@
       <c r="M85" s="281"/>
       <c r="N85" s="281"/>
       <c r="Q85" s="57" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7195,7 +7189,7 @@
       <c r="M86" s="281"/>
       <c r="N86" s="281"/>
       <c r="Q86" s="57" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7214,7 +7208,7 @@
       <c r="M87" s="281"/>
       <c r="N87" s="281"/>
       <c r="Q87" s="57" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7233,7 +7227,7 @@
       <c r="M88" s="281"/>
       <c r="N88" s="281"/>
       <c r="Q88" s="57" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7252,7 +7246,7 @@
       <c r="M89" s="281"/>
       <c r="N89" s="281"/>
       <c r="Q89" s="57" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7271,7 +7265,7 @@
       <c r="M90" s="281"/>
       <c r="N90" s="281"/>
       <c r="Q90" s="57" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7290,7 +7284,7 @@
       <c r="M91" s="281"/>
       <c r="N91" s="281"/>
       <c r="Q91" s="57" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7309,7 +7303,7 @@
       <c r="M92" s="281"/>
       <c r="N92" s="281"/>
       <c r="Q92" s="57" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7328,7 +7322,7 @@
       <c r="M93" s="281"/>
       <c r="N93" s="281"/>
       <c r="Q93" s="57" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7347,7 +7341,7 @@
       <c r="M94" s="281"/>
       <c r="N94" s="281"/>
       <c r="Q94" s="57" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7366,7 +7360,7 @@
       <c r="M95" s="281"/>
       <c r="N95" s="281"/>
       <c r="Q95" s="57" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7385,7 +7379,7 @@
       <c r="M96" s="281"/>
       <c r="N96" s="281"/>
       <c r="Q96" s="57" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7404,7 +7398,7 @@
       <c r="M97" s="281"/>
       <c r="N97" s="281"/>
       <c r="Q97" s="57" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7423,7 +7417,7 @@
       <c r="M98" s="281"/>
       <c r="N98" s="281"/>
       <c r="Q98" s="57" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7442,7 +7436,7 @@
       <c r="M99" s="281"/>
       <c r="N99" s="281"/>
       <c r="Q99" s="57" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7461,7 +7455,7 @@
       <c r="M100" s="281"/>
       <c r="N100" s="281"/>
       <c r="Q100" s="57" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7499,7 +7493,7 @@
       <c r="M102" s="281"/>
       <c r="N102" s="281"/>
       <c r="Q102" s="57" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="103" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7518,7 +7512,7 @@
       <c r="M103" s="281"/>
       <c r="N103" s="281"/>
       <c r="Q103" s="57" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7537,7 +7531,7 @@
       <c r="M104" s="281"/>
       <c r="N104" s="281"/>
       <c r="Q104" s="57" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7556,7 +7550,7 @@
       <c r="M105" s="281"/>
       <c r="N105" s="281"/>
       <c r="Q105" s="57" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7575,7 +7569,7 @@
       <c r="M106" s="281"/>
       <c r="N106" s="281"/>
       <c r="Q106" s="57" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7594,7 +7588,7 @@
       <c r="M107" s="281"/>
       <c r="N107" s="281"/>
       <c r="Q107" s="57" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="108" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7613,7 +7607,7 @@
       <c r="M108" s="281"/>
       <c r="N108" s="281"/>
       <c r="Q108" s="57" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7632,7 +7626,7 @@
       <c r="M109" s="281"/>
       <c r="N109" s="281"/>
       <c r="Q109" s="57" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7651,7 +7645,7 @@
       <c r="M110" s="281"/>
       <c r="N110" s="281"/>
       <c r="Q110" s="57" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7670,7 +7664,7 @@
       <c r="M111" s="281"/>
       <c r="N111" s="281"/>
       <c r="Q111" s="57" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7689,7 +7683,7 @@
       <c r="M112" s="281"/>
       <c r="N112" s="281"/>
       <c r="Q112" s="57" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7708,7 +7702,7 @@
       <c r="M113" s="281"/>
       <c r="N113" s="281"/>
       <c r="Q113" s="57" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7727,7 +7721,7 @@
       <c r="M114" s="281"/>
       <c r="N114" s="281"/>
       <c r="Q114" s="57" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7746,7 +7740,7 @@
       <c r="M115" s="281"/>
       <c r="N115" s="281"/>
       <c r="Q115" s="57" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7765,7 +7759,7 @@
       <c r="M116" s="281"/>
       <c r="N116" s="281"/>
       <c r="Q116" s="57" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7784,7 +7778,7 @@
       <c r="M117" s="281"/>
       <c r="N117" s="281"/>
       <c r="Q117" s="57" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7803,7 +7797,7 @@
       <c r="M118" s="281"/>
       <c r="N118" s="281"/>
       <c r="Q118" s="57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7822,7 +7816,7 @@
       <c r="M119" s="281"/>
       <c r="N119" s="281"/>
       <c r="Q119" s="57" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7841,7 +7835,7 @@
       <c r="M120" s="281"/>
       <c r="N120" s="281"/>
       <c r="Q120" s="57" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7860,7 +7854,7 @@
       <c r="M121" s="281"/>
       <c r="N121" s="281"/>
       <c r="Q121" s="57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7879,7 +7873,7 @@
       <c r="M122" s="281"/>
       <c r="N122" s="281"/>
       <c r="Q122" s="57" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="123" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7898,7 +7892,7 @@
       <c r="M123" s="281"/>
       <c r="N123" s="281"/>
       <c r="Q123" s="57" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7917,7 +7911,7 @@
       <c r="M124" s="281"/>
       <c r="N124" s="281"/>
       <c r="Q124" s="57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7936,7 +7930,7 @@
       <c r="M125" s="281"/>
       <c r="N125" s="281"/>
       <c r="Q125" s="57" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7955,7 +7949,7 @@
       <c r="M126" s="281"/>
       <c r="N126" s="281"/>
       <c r="Q126" s="57" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="127" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7974,7 +7968,7 @@
       <c r="M127" s="281"/>
       <c r="N127" s="281"/>
       <c r="Q127" s="57" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -7993,7 +7987,7 @@
       <c r="M128" s="281"/>
       <c r="N128" s="281"/>
       <c r="Q128" s="57" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="129" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8012,7 +8006,7 @@
       <c r="M129" s="281"/>
       <c r="N129" s="281"/>
       <c r="Q129" s="57" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8031,7 +8025,7 @@
       <c r="M130" s="281"/>
       <c r="N130" s="281"/>
       <c r="Q130" s="57" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8050,7 +8044,7 @@
       <c r="M131" s="281"/>
       <c r="N131" s="281"/>
       <c r="Q131" s="57" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8069,7 +8063,7 @@
       <c r="M132" s="281"/>
       <c r="N132" s="281"/>
       <c r="Q132" s="57" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8088,7 +8082,7 @@
       <c r="M133" s="281"/>
       <c r="N133" s="281"/>
       <c r="Q133" s="57" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8107,7 +8101,7 @@
       <c r="M134" s="281"/>
       <c r="N134" s="281"/>
       <c r="Q134" s="57" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8126,7 +8120,7 @@
       <c r="M135" s="281"/>
       <c r="N135" s="281"/>
       <c r="Q135" s="57" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8145,7 +8139,7 @@
       <c r="M136" s="281"/>
       <c r="N136" s="281"/>
       <c r="Q136" s="57" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8164,7 +8158,7 @@
       <c r="M137" s="281"/>
       <c r="N137" s="281"/>
       <c r="Q137" s="57" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8183,7 +8177,7 @@
       <c r="M138" s="281"/>
       <c r="N138" s="281"/>
       <c r="Q138" s="57" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8202,7 +8196,7 @@
       <c r="M139" s="281"/>
       <c r="N139" s="281"/>
       <c r="Q139" s="57" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8221,7 +8215,7 @@
       <c r="M140" s="281"/>
       <c r="N140" s="281"/>
       <c r="Q140" s="57" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8240,7 +8234,7 @@
       <c r="M141" s="281"/>
       <c r="N141" s="281"/>
       <c r="Q141" s="57" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8259,7 +8253,7 @@
       <c r="M142" s="281"/>
       <c r="N142" s="281"/>
       <c r="Q142" s="57" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8278,7 +8272,7 @@
       <c r="M143" s="281"/>
       <c r="N143" s="281"/>
       <c r="Q143" s="57" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8297,7 +8291,7 @@
       <c r="M144" s="281"/>
       <c r="N144" s="281"/>
       <c r="Q144" s="57" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8316,7 +8310,7 @@
       <c r="M145" s="281"/>
       <c r="N145" s="281"/>
       <c r="Q145" s="57" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="146" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8335,7 +8329,7 @@
       <c r="M146" s="281"/>
       <c r="N146" s="281"/>
       <c r="Q146" s="57" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="147" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8354,7 +8348,7 @@
       <c r="M147" s="281"/>
       <c r="N147" s="281"/>
       <c r="Q147" s="57" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="148" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8373,7 +8367,7 @@
       <c r="M148" s="281"/>
       <c r="N148" s="281"/>
       <c r="Q148" s="57" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8392,7 +8386,7 @@
       <c r="M149" s="281"/>
       <c r="N149" s="281"/>
       <c r="Q149" s="57" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="150" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8411,7 +8405,7 @@
       <c r="M150" s="281"/>
       <c r="N150" s="281"/>
       <c r="Q150" s="57" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="151" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8430,7 +8424,7 @@
       <c r="M151" s="281"/>
       <c r="N151" s="281"/>
       <c r="Q151" s="57" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8449,7 +8443,7 @@
       <c r="M152" s="281"/>
       <c r="N152" s="281"/>
       <c r="Q152" s="57" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="153" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8468,7 +8462,7 @@
       <c r="M153" s="281"/>
       <c r="N153" s="281"/>
       <c r="Q153" s="57" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8487,7 +8481,7 @@
       <c r="M154" s="281"/>
       <c r="N154" s="281"/>
       <c r="Q154" s="57" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8506,7 +8500,7 @@
       <c r="M155" s="281"/>
       <c r="N155" s="281"/>
       <c r="Q155" s="57" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8525,7 +8519,7 @@
       <c r="M156" s="281"/>
       <c r="N156" s="281"/>
       <c r="Q156" s="57" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8544,7 +8538,7 @@
       <c r="M157" s="281"/>
       <c r="N157" s="281"/>
       <c r="Q157" s="57" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8563,7 +8557,7 @@
       <c r="M158" s="281"/>
       <c r="N158" s="281"/>
       <c r="Q158" s="57" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="159" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8582,7 +8576,7 @@
       <c r="M159" s="281"/>
       <c r="N159" s="281"/>
       <c r="Q159" s="57" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="160" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8601,7 +8595,7 @@
       <c r="M160" s="281"/>
       <c r="N160" s="281"/>
       <c r="Q160" s="57" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8620,7 +8614,7 @@
       <c r="M161" s="281"/>
       <c r="N161" s="281"/>
       <c r="Q161" s="57" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="162" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8639,7 +8633,7 @@
       <c r="M162" s="281"/>
       <c r="N162" s="281"/>
       <c r="Q162" s="57" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8658,7 +8652,7 @@
       <c r="M163" s="281"/>
       <c r="N163" s="281"/>
       <c r="Q163" s="57" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8677,7 +8671,7 @@
       <c r="M164" s="281"/>
       <c r="N164" s="281"/>
       <c r="Q164" s="57" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="165" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8696,7 +8690,7 @@
       <c r="M165" s="281"/>
       <c r="N165" s="281"/>
       <c r="Q165" s="57" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8715,7 +8709,7 @@
       <c r="M166" s="281"/>
       <c r="N166" s="281"/>
       <c r="Q166" s="57" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="167" ht="42.75" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8734,7 +8728,7 @@
       <c r="M167" s="281"/>
       <c r="N167" s="281"/>
       <c r="Q167" s="57" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="168" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8753,7 +8747,7 @@
       <c r="M168" s="281"/>
       <c r="N168" s="281"/>
       <c r="Q168" s="57" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="169" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8772,7 +8766,7 @@
       <c r="M169" s="281"/>
       <c r="N169" s="281"/>
       <c r="Q169" s="57" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8791,7 +8785,7 @@
       <c r="M170" s="281"/>
       <c r="N170" s="281"/>
       <c r="Q170" s="57" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="171" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8810,7 +8804,7 @@
       <c r="M171" s="281"/>
       <c r="N171" s="281"/>
       <c r="Q171" s="57" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="172" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8829,7 +8823,7 @@
       <c r="M172" s="281"/>
       <c r="N172" s="281"/>
       <c r="Q172" s="57" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="173" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8848,7 +8842,7 @@
       <c r="M173" s="281"/>
       <c r="N173" s="281"/>
       <c r="Q173" s="57" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="174" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8867,7 +8861,7 @@
       <c r="M174" s="281"/>
       <c r="N174" s="281"/>
       <c r="Q174" s="57" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="175" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8886,7 +8880,7 @@
       <c r="M175" s="281"/>
       <c r="N175" s="281"/>
       <c r="Q175" s="57" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8905,7 +8899,7 @@
       <c r="M176" s="281"/>
       <c r="N176" s="281"/>
       <c r="Q176" s="57" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="177" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8924,7 +8918,7 @@
       <c r="M177" s="281"/>
       <c r="N177" s="281"/>
       <c r="Q177" s="57" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8943,7 +8937,7 @@
       <c r="M178" s="281"/>
       <c r="N178" s="281"/>
       <c r="Q178" s="57" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="179" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8962,7 +8956,7 @@
       <c r="M179" s="281"/>
       <c r="N179" s="281"/>
       <c r="Q179" s="57" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="180" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -8981,7 +8975,7 @@
       <c r="M180" s="281"/>
       <c r="N180" s="281"/>
       <c r="Q180" s="57" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="181" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9000,7 +8994,7 @@
       <c r="M181" s="281"/>
       <c r="N181" s="281"/>
       <c r="Q181" s="57" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="182" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9019,7 +9013,7 @@
       <c r="M182" s="281"/>
       <c r="N182" s="281"/>
       <c r="Q182" s="57" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="183" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9038,7 +9032,7 @@
       <c r="M183" s="281"/>
       <c r="N183" s="281"/>
       <c r="Q183" s="57" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="184" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9057,7 +9051,7 @@
       <c r="M184" s="281"/>
       <c r="N184" s="281"/>
       <c r="Q184" s="57" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="185" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9076,7 +9070,7 @@
       <c r="M185" s="281"/>
       <c r="N185" s="281"/>
       <c r="Q185" s="57" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="186" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9095,7 +9089,7 @@
       <c r="M186" s="281"/>
       <c r="N186" s="281"/>
       <c r="Q186" s="57" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="187" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9114,7 +9108,7 @@
       <c r="M187" s="281"/>
       <c r="N187" s="281"/>
       <c r="Q187" s="57" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9133,7 +9127,7 @@
       <c r="M188" s="281"/>
       <c r="N188" s="281"/>
       <c r="Q188" s="57" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="189" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9152,7 +9146,7 @@
       <c r="M189" s="281"/>
       <c r="N189" s="281"/>
       <c r="Q189" s="57" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="190" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9171,7 +9165,7 @@
       <c r="M190" s="281"/>
       <c r="N190" s="281"/>
       <c r="Q190" s="57" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="191" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9190,7 +9184,7 @@
       <c r="M191" s="281"/>
       <c r="N191" s="281"/>
       <c r="Q191" s="57" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="192" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9209,7 +9203,7 @@
       <c r="M192" s="281"/>
       <c r="N192" s="281"/>
       <c r="Q192" s="57" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="193" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9228,7 +9222,7 @@
       <c r="M193" s="281"/>
       <c r="N193" s="281"/>
       <c r="Q193" s="57" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="194" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9247,7 +9241,7 @@
       <c r="M194" s="281"/>
       <c r="N194" s="281"/>
       <c r="Q194" s="57" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="195" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9266,7 +9260,7 @@
       <c r="M195" s="281"/>
       <c r="N195" s="281"/>
       <c r="Q195" s="57" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="196" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9285,7 +9279,7 @@
       <c r="M196" s="281"/>
       <c r="N196" s="281"/>
       <c r="Q196" s="57" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="197" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9304,7 +9298,7 @@
       <c r="M197" s="281"/>
       <c r="N197" s="281"/>
       <c r="Q197" s="57" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="198" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9323,7 +9317,7 @@
       <c r="M198" s="281"/>
       <c r="N198" s="281"/>
       <c r="Q198" s="57" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="199" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9342,7 +9336,7 @@
       <c r="M199" s="281"/>
       <c r="N199" s="281"/>
       <c r="Q199" s="57" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="200" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9361,7 +9355,7 @@
       <c r="M200" s="281"/>
       <c r="N200" s="281"/>
       <c r="Q200" s="57" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="201" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9380,7 +9374,7 @@
       <c r="M201" s="281"/>
       <c r="N201" s="281"/>
       <c r="Q201" s="57" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="202" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9399,7 +9393,7 @@
       <c r="M202" s="281"/>
       <c r="N202" s="281"/>
       <c r="Q202" s="57" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="203" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9418,7 +9412,7 @@
       <c r="M203" s="281"/>
       <c r="N203" s="281"/>
       <c r="Q203" s="57" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="204" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9437,7 +9431,7 @@
       <c r="M204" s="281"/>
       <c r="N204" s="281"/>
       <c r="Q204" s="57" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="205" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9456,7 +9450,7 @@
       <c r="M205" s="281"/>
       <c r="N205" s="281"/>
       <c r="Q205" s="57" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9475,7 +9469,7 @@
       <c r="M206" s="281"/>
       <c r="N206" s="281"/>
       <c r="Q206" s="57" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="207" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9494,7 +9488,7 @@
       <c r="M207" s="281"/>
       <c r="N207" s="281"/>
       <c r="Q207" s="57" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="208" ht="28.5" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9513,7 +9507,7 @@
       <c r="M208" s="281"/>
       <c r="N208" s="281"/>
       <c r="Q208" s="57" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="209" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9532,7 +9526,7 @@
       <c r="M209" s="281"/>
       <c r="N209" s="281"/>
       <c r="Q209" s="57" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="210" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9551,7 +9545,7 @@
       <c r="M210" s="281"/>
       <c r="N210" s="281"/>
       <c r="Q210" s="57" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9570,7 +9564,7 @@
       <c r="M211" s="281"/>
       <c r="N211" s="281"/>
       <c r="Q211" s="57" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="212" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9589,7 +9583,7 @@
       <c r="M212" s="281"/>
       <c r="N212" s="281"/>
       <c r="Q212" s="57" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="213" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9608,7 +9602,7 @@
       <c r="M213" s="281"/>
       <c r="N213" s="281"/>
       <c r="Q213" s="57" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="214" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9627,7 +9621,7 @@
       <c r="M214" s="281"/>
       <c r="N214" s="281"/>
       <c r="Q214" s="57" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="215" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9646,7 +9640,7 @@
       <c r="M215" s="281"/>
       <c r="N215" s="281"/>
       <c r="Q215" s="57" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="216" ht="14.25" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9665,7 +9659,7 @@
       <c r="M216" s="281"/>
       <c r="N216" s="281"/>
       <c r="Q216" s="57" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.25">
@@ -10836,7 +10830,7 @@
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="286" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B2" s="287"/>
       <c r="C2" s="287"/>
@@ -10853,28 +10847,28 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="289" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B3" s="290" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C3" s="290"/>
       <c r="D3" s="290"/>
       <c r="E3" s="291"/>
       <c r="F3" s="292" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G3" s="293" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H3" s="291"/>
       <c r="I3" s="293" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="J3" s="290"/>
       <c r="K3" s="291"/>
       <c r="L3" s="294" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M3" s="295"/>
     </row>
@@ -10891,15 +10885,15 @@
       <c r="J4" s="297"/>
       <c r="K4" s="298"/>
       <c r="L4" s="301" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M4" s="302" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="303" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B5" s="304"/>
       <c r="C5" s="304"/>
@@ -11016,7 +11010,7 @@
     </row>
     <row r="12" ht="12" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="319" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B12" s="320"/>
       <c r="C12" s="320"/>
@@ -11033,7 +11027,7 @@
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="170" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B13" s="171"/>
       <c r="C13" s="171"/>
@@ -11050,7 +11044,7 @@
     </row>
     <row r="14" ht="12" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="322" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B14" s="203"/>
       <c r="C14" s="203"/>
@@ -11067,33 +11061,33 @@
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="296" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B15" s="324" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C15" s="325"/>
       <c r="D15" s="326" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E15" s="324"/>
       <c r="F15" s="325"/>
       <c r="G15" s="326" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H15" s="324"/>
       <c r="I15" s="325"/>
       <c r="J15" s="327" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K15" s="328" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L15" s="329" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M15" s="330" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -11113,11 +11107,11 @@
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="332" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B17" s="333"/>
       <c r="C17" s="334" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D17" s="300"/>
       <c r="E17" s="297"/>
@@ -11131,35 +11125,19 @@
       <c r="M17" s="338"/>
     </row>
     <row r="18" ht="24" customHeight="1" spans="1:13" s="339" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="340">
-        <v>45548</v>
-      </c>
+      <c r="A18" s="340"/>
       <c r="B18" s="341"/>
-      <c r="C18" s="341">
-        <v>45547</v>
-      </c>
-      <c r="D18" s="304" t="s">
-        <v>369</v>
-      </c>
+      <c r="C18" s="341"/>
+      <c r="D18" s="304"/>
       <c r="E18" s="304"/>
       <c r="F18" s="304"/>
-      <c r="G18" s="304" t="s">
-        <v>369</v>
-      </c>
+      <c r="G18" s="304"/>
       <c r="H18" s="304"/>
       <c r="I18" s="304"/>
-      <c r="J18" s="342" t="s">
-        <v>370</v>
-      </c>
-      <c r="K18" s="308" t="s">
-        <v>369</v>
-      </c>
-      <c r="L18" s="308" t="s">
-        <v>371</v>
-      </c>
-      <c r="M18" s="343" t="s">
-        <v>372</v>
-      </c>
+      <c r="J18" s="342"/>
+      <c r="K18" s="308"/>
+      <c r="L18" s="308"/>
+      <c r="M18" s="343"/>
     </row>
     <row r="19" ht="24" customHeight="1" spans="1:13" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="340"/>
@@ -11568,7 +11546,7 @@
     </row>
     <row r="46" ht="9.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="348" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B46" s="349"/>
       <c r="C46" s="349"/>
@@ -11585,7 +11563,7 @@
     </row>
     <row r="47" ht="27.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="268" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B47" s="269"/>
       <c r="C47" s="270"/>
@@ -11595,11 +11573,11 @@
       <c r="G47" s="353"/>
       <c r="H47" s="354"/>
       <c r="I47" s="355" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J47" s="356"/>
       <c r="K47" s="357" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L47" s="357"/>
       <c r="M47" s="358"/>
@@ -11607,7 +11585,7 @@
     </row>
     <row r="48" ht="9" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="360" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B48" s="360"/>
       <c r="C48" s="360"/>
@@ -11801,7 +11779,7 @@
     </row>
     <row r="2" ht="22.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="365" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B2" s="366"/>
       <c r="C2" s="366"/>
@@ -11816,22 +11794,22 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="368" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B3" s="369" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C3" s="369"/>
       <c r="D3" s="370"/>
       <c r="E3" s="290" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F3" s="291"/>
       <c r="G3" s="371" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="H3" s="293" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I3" s="372"/>
       <c r="J3" s="372"/>
@@ -11856,10 +11834,10 @@
       <c r="C5" s="380"/>
       <c r="D5" s="381"/>
       <c r="E5" s="333" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F5" s="334" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G5" s="336"/>
       <c r="H5" s="382"/>
@@ -11869,7 +11847,7 @@
     </row>
     <row r="6" ht="27.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="383" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B6" s="384"/>
       <c r="C6" s="384"/>
@@ -11884,7 +11862,7 @@
         <v>123</v>
       </c>
       <c r="H6" s="385" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I6" s="386"/>
       <c r="J6" s="386"/>
@@ -11892,7 +11870,7 @@
     </row>
     <row r="7" ht="27.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="383" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B7" s="384"/>
       <c r="C7" s="384"/>
@@ -11907,7 +11885,7 @@
         <v>23</v>
       </c>
       <c r="H7" s="385" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="I7" s="386"/>
       <c r="J7" s="386"/>
@@ -11980,7 +11958,7 @@
     </row>
     <row r="13" ht="11.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="319" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B13" s="320"/>
       <c r="C13" s="320"/>
@@ -11995,7 +11973,7 @@
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:11" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="395" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B14" s="396"/>
       <c r="C14" s="396"/>
@@ -12010,25 +11988,25 @@
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="374" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B15" s="324" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C15" s="282"/>
       <c r="D15" s="398"/>
       <c r="E15" s="324" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F15" s="325"/>
       <c r="G15" s="328" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="H15" s="327" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I15" s="326" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J15" s="282"/>
       <c r="K15" s="378"/>
@@ -12052,10 +12030,10 @@
       <c r="C17" s="125"/>
       <c r="D17" s="399"/>
       <c r="E17" s="333" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F17" s="334" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G17" s="336"/>
       <c r="H17" s="335"/>
@@ -12065,7 +12043,7 @@
     </row>
     <row r="18" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="383" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="B18" s="400"/>
       <c r="C18" s="400"/>
@@ -12080,10 +12058,10 @@
         <v>32</v>
       </c>
       <c r="H18" s="308" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="I18" s="385" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="J18" s="402"/>
       <c r="K18" s="403"/>
@@ -12350,7 +12328,7 @@
     </row>
     <row r="39" ht="13.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="265" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B39" s="266"/>
       <c r="C39" s="266"/>
@@ -12365,7 +12343,7 @@
     </row>
     <row r="40" ht="22.5" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="410" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B40" s="411"/>
       <c r="C40" s="411"/>
@@ -12380,36 +12358,36 @@
     </row>
     <row r="41" ht="33.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="413" t="s">
+        <v>388</v>
+      </c>
+      <c r="B41" s="414" t="s">
+        <v>389</v>
+      </c>
+      <c r="C41" s="415" t="s">
         <v>390</v>
       </c>
-      <c r="B41" s="414" t="s">
+      <c r="D41" s="414" t="s">
         <v>391</v>
-      </c>
-      <c r="C41" s="415" t="s">
-        <v>392</v>
-      </c>
-      <c r="D41" s="414" t="s">
-        <v>393</v>
       </c>
       <c r="E41" s="414"/>
       <c r="F41" s="414"/>
       <c r="G41" s="414"/>
       <c r="H41" s="416"/>
       <c r="I41" s="415" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J41" s="414" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K41" s="417"/>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="418" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="B42" s="419"/>
       <c r="C42" s="385" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="D42" s="420"/>
       <c r="E42" s="420"/>
@@ -12417,27 +12395,21 @@
       <c r="G42" s="420"/>
       <c r="H42" s="419"/>
       <c r="I42" s="385" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="J42" s="420"/>
       <c r="K42" s="421"/>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="418" t="s">
-        <v>369</v>
-      </c>
+      <c r="A43" s="418"/>
       <c r="B43" s="419"/>
-      <c r="C43" s="385" t="s">
-        <v>369</v>
-      </c>
+      <c r="C43" s="385"/>
       <c r="D43" s="420"/>
       <c r="E43" s="420"/>
       <c r="F43" s="420"/>
       <c r="G43" s="420"/>
       <c r="H43" s="419"/>
-      <c r="I43" s="385" t="s">
-        <v>369</v>
-      </c>
+      <c r="I43" s="385"/>
       <c r="J43" s="420"/>
       <c r="K43" s="421"/>
     </row>
@@ -12508,7 +12480,7 @@
     </row>
     <row r="49" ht="11.25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="265" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B49" s="266"/>
       <c r="C49" s="266"/>
@@ -12523,7 +12495,7 @@
     </row>
     <row r="50" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="268" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B50" s="270"/>
       <c r="C50" s="352"/>
@@ -12531,11 +12503,11 @@
       <c r="E50" s="353"/>
       <c r="F50" s="354"/>
       <c r="G50" s="422" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H50" s="423"/>
       <c r="I50" s="352" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J50" s="353"/>
       <c r="K50" s="354"/>
@@ -12544,7 +12516,7 @@
     </row>
     <row r="51" ht="9.75" customHeight="1" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K51" s="425" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="52" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12685,11 +12657,11 @@
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="429" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B2" s="430"/>
       <c r="C2" s="431" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D2" s="431"/>
       <c r="E2" s="431"/>
@@ -12706,7 +12678,7 @@
       <c r="A3" s="437"/>
       <c r="B3" s="438"/>
       <c r="C3" s="439" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D3" s="439"/>
       <c r="E3" s="439"/>
@@ -12723,7 +12695,7 @@
       <c r="A4" s="437"/>
       <c r="B4" s="438"/>
       <c r="C4" s="439" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D4" s="439"/>
       <c r="E4" s="439"/>
@@ -12755,7 +12727,7 @@
       <c r="A6" s="437"/>
       <c r="B6" s="438"/>
       <c r="C6" s="439" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D6" s="439"/>
       <c r="E6" s="439"/>
@@ -12763,7 +12735,7 @@
       <c r="G6" s="282"/>
       <c r="H6" s="282"/>
       <c r="I6" s="447" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J6" s="447"/>
       <c r="K6" s="447"/>
@@ -12789,14 +12761,14 @@
       <c r="A8" s="437"/>
       <c r="B8" s="438"/>
       <c r="C8" s="439" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D8" s="439"/>
       <c r="E8" s="439"/>
       <c r="F8" s="440"/>
       <c r="G8" s="445"/>
       <c r="H8" s="282" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I8" s="445"/>
       <c r="J8" s="445"/>
@@ -12827,7 +12799,7 @@
       <c r="E10" s="439"/>
       <c r="F10" s="440"/>
       <c r="G10" s="446" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H10" s="446"/>
       <c r="I10" s="446"/>
@@ -12870,18 +12842,18 @@
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="460" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B13" s="461"/>
       <c r="C13" s="462" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D13" s="462"/>
       <c r="E13" s="282"/>
       <c r="F13" s="398"/>
       <c r="G13" s="463"/>
       <c r="H13" s="463" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I13" s="463"/>
       <c r="J13" s="463"/>
@@ -12897,7 +12869,7 @@
       <c r="E14" s="282"/>
       <c r="F14" s="398"/>
       <c r="G14" s="467" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H14" s="446"/>
       <c r="I14" s="446"/>
@@ -12955,14 +12927,14 @@
       <c r="A18" s="475"/>
       <c r="B18" s="476"/>
       <c r="C18" s="483" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D18" s="483"/>
       <c r="E18" s="484"/>
       <c r="F18" s="485"/>
       <c r="G18" s="486"/>
       <c r="H18" s="486" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I18" s="486"/>
       <c r="J18" s="486"/>
@@ -12978,7 +12950,7 @@
       <c r="E19" s="484"/>
       <c r="F19" s="485"/>
       <c r="G19" s="467" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H19" s="446"/>
       <c r="I19" s="446"/>
@@ -12996,7 +12968,7 @@
       <c r="F20" s="485"/>
       <c r="G20" s="486"/>
       <c r="H20" s="488" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I20" s="488"/>
       <c r="J20" s="489"/>
@@ -13012,7 +12984,7 @@
       <c r="E21" s="484"/>
       <c r="F21" s="485"/>
       <c r="G21" s="492" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H21" s="493"/>
       <c r="I21" s="493"/>
@@ -13029,7 +13001,7 @@
       <c r="E22" s="497"/>
       <c r="F22" s="498"/>
       <c r="G22" s="471" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H22" s="472"/>
       <c r="I22" s="499"/>
@@ -13040,18 +13012,18 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="194" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B23" s="195"/>
       <c r="C23" s="501" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D23" s="501"/>
       <c r="E23" s="501"/>
       <c r="F23" s="502"/>
       <c r="G23" s="463"/>
       <c r="H23" s="463" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I23" s="463"/>
       <c r="J23" s="463"/>
@@ -13067,7 +13039,7 @@
       <c r="E24" s="503"/>
       <c r="F24" s="504"/>
       <c r="G24" s="467" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H24" s="446"/>
       <c r="I24" s="446"/>
@@ -13108,11 +13080,11 @@
     </row>
     <row r="27" ht="14.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="194" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B27" s="195"/>
       <c r="C27" s="501" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D27" s="501"/>
       <c r="E27" s="501"/>
@@ -13133,7 +13105,7 @@
       <c r="E28" s="503"/>
       <c r="F28" s="504"/>
       <c r="G28" s="467" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H28" s="446"/>
       <c r="I28" s="446"/>
@@ -13174,18 +13146,18 @@
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:13" s="282" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="194" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B31" s="195"/>
       <c r="C31" s="501" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D31" s="501"/>
       <c r="E31" s="501"/>
       <c r="F31" s="502"/>
       <c r="G31" s="463"/>
       <c r="H31" s="463" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I31" s="463"/>
       <c r="J31" s="463"/>
@@ -13201,7 +13173,7 @@
       <c r="E32" s="503"/>
       <c r="F32" s="504"/>
       <c r="G32" s="514" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H32" s="515"/>
       <c r="I32" s="515"/>
@@ -13229,7 +13201,7 @@
       <c r="A34" s="465"/>
       <c r="B34" s="466"/>
       <c r="C34" s="503" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D34" s="503"/>
       <c r="E34" s="503"/>
@@ -13250,7 +13222,7 @@
       <c r="E35" s="503"/>
       <c r="F35" s="504"/>
       <c r="G35" s="514" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H35" s="515"/>
       <c r="I35" s="515"/>
@@ -13276,11 +13248,11 @@
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="194" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B37" s="195"/>
       <c r="C37" s="524" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D37" s="524"/>
       <c r="E37" s="524"/>
@@ -13301,7 +13273,7 @@
       <c r="E38" s="462"/>
       <c r="F38" s="526"/>
       <c r="G38" s="467" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H38" s="446"/>
       <c r="I38" s="446"/>
@@ -13342,11 +13314,11 @@
     </row>
     <row r="41" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="530" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B41" s="531"/>
       <c r="C41" s="503" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D41" s="503"/>
       <c r="E41" s="503"/>
@@ -13377,18 +13349,18 @@
     </row>
     <row r="43" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="535" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B43" s="536"/>
       <c r="C43" s="503" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D43" s="503"/>
       <c r="E43" s="503"/>
       <c r="F43" s="504"/>
       <c r="G43" s="445"/>
       <c r="H43" s="282" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I43" s="445"/>
       <c r="J43" s="445"/>
@@ -13405,7 +13377,7 @@
       <c r="E44" s="503"/>
       <c r="F44" s="504"/>
       <c r="G44" s="539" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H44" s="540"/>
       <c r="I44" s="519"/>
@@ -13417,18 +13389,18 @@
     </row>
     <row r="45" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="535" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B45" s="536"/>
       <c r="C45" s="504" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D45" s="504"/>
       <c r="E45" s="504"/>
       <c r="F45" s="504"/>
       <c r="G45" s="445"/>
       <c r="H45" s="282" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I45" s="445"/>
       <c r="J45" s="445"/>
@@ -13445,7 +13417,7 @@
       <c r="E46" s="504"/>
       <c r="F46" s="504"/>
       <c r="G46" s="542" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H46" s="543"/>
       <c r="I46" s="519"/>
@@ -13457,18 +13429,18 @@
     </row>
     <row r="47" ht="13.5" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="535" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B47" s="536"/>
       <c r="C47" s="503" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D47" s="503"/>
       <c r="E47" s="544"/>
       <c r="F47" s="545"/>
       <c r="G47" s="445"/>
       <c r="H47" s="282" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I47" s="445"/>
       <c r="J47" s="445"/>
@@ -13485,7 +13457,7 @@
       <c r="E48" s="547"/>
       <c r="F48" s="548"/>
       <c r="G48" s="549" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H48" s="550"/>
       <c r="I48" s="551"/>
@@ -13513,11 +13485,11 @@
     </row>
     <row r="50" ht="23.25" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="559" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B50" s="560"/>
       <c r="C50" s="561" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D50" s="561"/>
       <c r="E50" s="561"/>
@@ -13533,17 +13505,17 @@
     </row>
     <row r="51" ht="18" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="566" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B51" s="567"/>
       <c r="C51" s="567"/>
       <c r="D51" s="567"/>
       <c r="E51" s="568"/>
       <c r="F51" s="294" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G51" s="569" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H51" s="414"/>
       <c r="I51" s="417"/>
@@ -13554,17 +13526,17 @@
     </row>
     <row r="52" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="573" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="B52" s="574"/>
       <c r="C52" s="575"/>
       <c r="D52" s="575"/>
       <c r="E52" s="576"/>
       <c r="F52" s="577" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="G52" s="578" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H52" s="579"/>
       <c r="I52" s="580"/>
@@ -13575,17 +13547,17 @@
     </row>
     <row r="53" ht="24" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="573" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="B53" s="574"/>
       <c r="C53" s="574"/>
       <c r="D53" s="574"/>
       <c r="E53" s="581"/>
       <c r="F53" s="577" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="G53" s="578" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H53" s="579"/>
       <c r="I53" s="580"/>
@@ -13611,11 +13583,11 @@
     </row>
     <row r="55" ht="39.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="429" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B55" s="430"/>
       <c r="C55" s="590" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D55" s="590"/>
       <c r="E55" s="590"/>
@@ -13640,7 +13612,7 @@
       <c r="I56" s="595"/>
       <c r="J56" s="596"/>
       <c r="K56" s="597" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="L56" s="597"/>
       <c r="M56" s="598"/>
@@ -13693,7 +13665,7 @@
     <row r="60" ht="50" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="609"/>
       <c r="B60" s="610" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C60" s="611"/>
       <c r="D60" s="612"/>
@@ -13710,7 +13682,7 @@
     <row r="61" ht="20.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="609"/>
       <c r="B61" s="617" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C61" s="618"/>
       <c r="D61" s="619"/>
@@ -13727,7 +13699,7 @@
     <row r="62" ht="9" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="609"/>
       <c r="B62" s="623" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C62" s="624"/>
       <c r="D62" s="625"/>
@@ -13748,7 +13720,7 @@
       <c r="D63" s="631"/>
       <c r="E63" s="282"/>
       <c r="F63" s="632" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G63" s="633"/>
       <c r="H63" s="633"/>
@@ -13761,13 +13733,13 @@
     <row r="64" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="609"/>
       <c r="B64" s="623" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C64" s="624"/>
       <c r="D64" s="625"/>
       <c r="E64" s="282"/>
       <c r="F64" s="635" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G64" s="125"/>
       <c r="H64" s="125"/>
@@ -13784,14 +13756,14 @@
       <c r="D65" s="641"/>
       <c r="E65" s="282"/>
       <c r="F65" s="642" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G65" s="643"/>
       <c r="H65" s="643"/>
       <c r="I65" s="644"/>
       <c r="J65" s="636"/>
       <c r="K65" s="645" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L65" s="646"/>
       <c r="M65" s="616"/>
@@ -13813,7 +13785,7 @@
     </row>
     <row r="67" ht="28.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="651" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B67" s="652"/>
       <c r="C67" s="652"/>
@@ -13849,7 +13821,7 @@
       <c r="C69" s="571"/>
       <c r="D69" s="571"/>
       <c r="E69" s="659" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F69" s="660"/>
       <c r="G69" s="660"/>
@@ -13877,7 +13849,7 @@
     </row>
     <row r="71" ht="10.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="668" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B71" s="668"/>
       <c r="C71" s="668"/>
@@ -14005,35 +13977,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="669" t="s">
+        <v>451</v>
+      </c>
+      <c r="B1" s="669" t="s">
+        <v>452</v>
+      </c>
+      <c r="C1" s="669" t="s">
         <v>453</v>
-      </c>
-      <c r="B1" s="669" t="s">
-        <v>454</v>
-      </c>
-      <c r="C1" s="669" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" t="s">
         <v>456</v>
-      </c>
-      <c r="B2" t="s">
-        <v>457</v>
-      </c>
-      <c r="C2" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -14043,7 +14015,7 @@
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>